<commit_message>
Mostly finished adding Co1
</commit_message>
<xml_diff>
--- a/results/tables/All_F1_tables.xlsx
+++ b/results/tables/All_F1_tables.xlsx
@@ -13,6 +13,9 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -356,7 +359,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -370,40 +373,35 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Pair</t>
+          <t>Query</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Query</t>
+          <t>Subject</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Subject</t>
+          <t>Precision</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Precision</t>
+          <t>Recall</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Recall</t>
+          <t>F1</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>F1</t>
+          <t>F0.5</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>F0.5</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Accuracy</t>
         </is>
@@ -417,33 +415,28 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>100 Australian speces</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D2">
+        <v>0.9795918367346939</v>
       </c>
       <c r="E2">
-        <v>0.9076923076923077</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F2">
-        <v>0.6344086021505376</v>
+        <v>0.793388429752066</v>
       </c>
       <c r="G2">
-        <v>0.7468354430379748</v>
+        <v>0.8955223880597016</v>
       </c>
       <c r="H2">
-        <v>0.8356940509915014</v>
-      </c>
-      <c r="I2">
-        <v>0.5959595959595959</v>
+        <v>0.7474747474747475</v>
       </c>
     </row>
     <row r="3">
@@ -454,33 +447,28 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>100 Australian speces</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>0.9583333333333334</v>
       </c>
       <c r="E3">
-        <v>0.8571428571428571</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F3">
-        <v>0.5274725274725275</v>
+        <v>0.7863247863247863</v>
       </c>
       <c r="G3">
-        <v>0.6530612244897959</v>
+        <v>0.8812260536398469</v>
       </c>
       <c r="H3">
-        <v>0.761904761904762</v>
-      </c>
-      <c r="I3">
-        <v>0.4848484848484849</v>
+        <v>0.7474747474747475</v>
       </c>
     </row>
     <row r="4">
@@ -491,33 +479,28 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>100 Australian speces</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>0.96</v>
       </c>
       <c r="E4">
-        <v>0.7941176470588235</v>
+        <v>0.6956521739130435</v>
       </c>
       <c r="F4">
-        <v>0.6352941176470588</v>
+        <v>0.8067226890756302</v>
       </c>
       <c r="G4">
-        <v>0.7058823529411765</v>
+        <v>0.8921933085501859</v>
       </c>
       <c r="H4">
-        <v>0.7563025210084033</v>
-      </c>
-      <c r="I4">
-        <v>0.5454545454545454</v>
+        <v>0.7676767676767676</v>
       </c>
     </row>
     <row r="5">
@@ -528,33 +511,28 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>100 Australian speces</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>0.9743589743589743</v>
       </c>
       <c r="E5">
-        <v>0.8793103448275862</v>
+        <v>0.5428571428571428</v>
       </c>
       <c r="F5">
-        <v>0.5543478260869565</v>
+        <v>0.6972477064220183</v>
       </c>
       <c r="G5">
-        <v>0.6799999999999999</v>
+        <v>0.8407079646017698</v>
       </c>
       <c r="H5">
-        <v>0.787037037037037</v>
-      </c>
-      <c r="I5">
-        <v>0.5151515151515151</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="6">
@@ -565,144 +543,124 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>100 Australian speces</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>0.9642857142857143</v>
       </c>
       <c r="E6">
-        <v>0.9038461538461539</v>
+        <v>0.3857142857142857</v>
       </c>
       <c r="F6">
-        <v>0.5</v>
+        <v>0.5510204081632653</v>
       </c>
       <c r="G6">
-        <v>0.6438356164383562</v>
+        <v>0.7417582417582418</v>
       </c>
       <c r="H6">
-        <v>0.7781456953642384</v>
-      </c>
-      <c r="I6">
-        <v>0.4747474747474748</v>
+        <v>0.5555555555555556</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MMSeqs2</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>100 Australian speces</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0.8194444444444444</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>0.686046511627907</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>0.7468354430379746</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>0.7887700534759359</v>
-      </c>
-      <c r="I7">
-        <v>0.5959595959595959</v>
+        <v>0.2828282828282828</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>100 Australian speces</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>0.6721311475409836</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>0.5189873417721519</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>0.5857142857142856</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>0.6346749226006192</v>
-      </c>
-      <c r="I8">
-        <v>0.4141414141414141</v>
+        <v>0.2828282828282828</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>NBC</t>
+          <t>Mothur</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>100 Australian speces</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>0.8666666666666667</v>
       </c>
       <c r="E9">
-        <v>0.6885245901639344</v>
+        <v>0.8253968253968254</v>
       </c>
       <c r="F9">
-        <v>0.525</v>
+        <v>0.8455284552845528</v>
       </c>
       <c r="G9">
-        <v>0.5957446808510638</v>
+        <v>0.8580858085808584</v>
       </c>
       <c r="H9">
-        <v>0.6481481481481481</v>
-      </c>
-      <c r="I9">
-        <v>0.4242424242424243</v>
+        <v>0.8080808080808081</v>
       </c>
     </row>
     <row r="10">
@@ -713,107 +671,60 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>100 Australian speces</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>0.8909090909090909</v>
       </c>
       <c r="E10">
-        <v>0.5686274509803921</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="F10">
-        <v>0.3766233766233766</v>
+        <v>0.7050359712230215</v>
       </c>
       <c r="G10">
-        <v>0.453125</v>
+        <v>0.8059210526315789</v>
       </c>
       <c r="H10">
-        <v>0.5160142348754448</v>
-      </c>
-      <c r="I10">
-        <v>0.2929292929292929</v>
+        <v>0.5858585858585859</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>TNT</t>
+          <t>VSEARCH</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>100 Australian speces</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0.6111111111111112</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>0.2588235294117647</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>0.3636363636363637</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>0.480349344978166</v>
-      </c>
-      <c r="I11">
-        <v>0.2222222222222222</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>VSEARCH</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_12S_Lulu_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
-      </c>
-      <c r="E12">
-        <v>0.7272727272727273</v>
-      </c>
-      <c r="F12">
-        <v>0.4761904761904762</v>
-      </c>
-      <c r="G12">
-        <v>0.5755395683453238</v>
-      </c>
-      <c r="H12">
-        <v>0.6578947368421053</v>
-      </c>
-      <c r="I12">
-        <v>0.404040404040404</v>
+        <v>0.2828282828282828</v>
       </c>
     </row>
   </sheetData>
@@ -823,7 +734,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -837,40 +748,35 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Pair</t>
+          <t>Query</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Query</t>
+          <t>Subject</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Subject</t>
+          <t>Precision</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Precision</t>
+          <t>Recall</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Recall</t>
+          <t>F1</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>F1</t>
+          <t>F0.5</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>F0.5</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Accuracy</t>
         </is>
@@ -884,33 +790,28 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D2">
+        <v>0.9076923076923077</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0.6344086021505376</v>
       </c>
       <c r="F2">
-        <v>0.5151515151515151</v>
+        <v>0.7468354430379748</v>
       </c>
       <c r="G2">
-        <v>0.6799999999999999</v>
+        <v>0.8356940509915014</v>
       </c>
       <c r="H2">
-        <v>0.8415841584158416</v>
-      </c>
-      <c r="I2">
-        <v>0.5151515151515151</v>
+        <v>0.5959595959595959</v>
       </c>
     </row>
     <row r="3">
@@ -921,32 +822,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>0.8571428571428571</v>
       </c>
       <c r="E3">
-        <v>0.9056603773584906</v>
+        <v>0.5274725274725275</v>
       </c>
       <c r="F3">
-        <v>0.5106382978723404</v>
+        <v>0.6530612244897959</v>
       </c>
       <c r="G3">
-        <v>0.6530612244897959</v>
+        <v>0.761904761904762</v>
       </c>
       <c r="H3">
-        <v>0.784313725490196</v>
-      </c>
-      <c r="I3">
         <v>0.4848484848484849</v>
       </c>
     </row>
@@ -958,33 +854,28 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>0.7941176470588235</v>
       </c>
       <c r="E4">
-        <v>0.7761194029850746</v>
+        <v>0.6352941176470588</v>
       </c>
       <c r="F4">
-        <v>0.6190476190476191</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="G4">
-        <v>0.6887417218543046</v>
+        <v>0.7563025210084033</v>
       </c>
       <c r="H4">
-        <v>0.7386363636363638</v>
-      </c>
-      <c r="I4">
-        <v>0.5252525252525253</v>
+        <v>0.5454545454545454</v>
       </c>
     </row>
     <row r="5">
@@ -995,33 +886,28 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>0.8793103448275862</v>
       </c>
       <c r="E5">
-        <v>0.7868852459016393</v>
+        <v>0.5543478260869565</v>
       </c>
       <c r="F5">
-        <v>0.5581395348837209</v>
+        <v>0.6799999999999999</v>
       </c>
       <c r="G5">
-        <v>0.6530612244897959</v>
+        <v>0.787037037037037</v>
       </c>
       <c r="H5">
-        <v>0.7272727272727272</v>
-      </c>
-      <c r="I5">
-        <v>0.4848484848484849</v>
+        <v>0.5151515151515151</v>
       </c>
     </row>
     <row r="6">
@@ -1032,218 +918,220 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>0.9038461538461539</v>
       </c>
       <c r="E6">
-        <v>0.8181818181818182</v>
+        <v>0.5</v>
       </c>
       <c r="F6">
-        <v>0.5056179775280899</v>
+        <v>0.6438356164383562</v>
       </c>
       <c r="G6">
-        <v>0.6250000000000001</v>
+        <v>0.7781456953642384</v>
       </c>
       <c r="H6">
-        <v>0.7281553398058251</v>
-      </c>
-      <c r="I6">
-        <v>0.4545454545454545</v>
+        <v>0.4747474747474748</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MMSeqs2</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>0.9076923076923077</v>
       </c>
       <c r="E7">
-        <v>0.9230769230769231</v>
+        <v>0.6344086021505376</v>
       </c>
       <c r="F7">
-        <v>0.6382978723404256</v>
+        <v>0.7468354430379748</v>
       </c>
       <c r="G7">
-        <v>0.7547169811320755</v>
+        <v>0.8356940509915014</v>
       </c>
       <c r="H7">
-        <v>0.8474576271186441</v>
-      </c>
-      <c r="I7">
-        <v>0.6060606060606061</v>
+        <v>0.5959595959595959</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>0.8194444444444444</v>
       </c>
       <c r="E8">
-        <v>0.78125</v>
+        <v>0.686046511627907</v>
       </c>
       <c r="F8">
-        <v>0.5882352941176471</v>
+        <v>0.7468354430379746</v>
       </c>
       <c r="G8">
-        <v>0.6711409395973155</v>
+        <v>0.7887700534759359</v>
       </c>
       <c r="H8">
-        <v>0.7331378299120235</v>
-      </c>
-      <c r="I8">
-        <v>0.5050505050505051</v>
+        <v>0.5959595959595959</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>NBC</t>
+          <t>Mothur</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>0.6721311475409836</v>
       </c>
       <c r="E9">
-        <v>0.8181818181818182</v>
+        <v>0.5189873417721519</v>
       </c>
       <c r="F9">
-        <v>0.6206896551724138</v>
+        <v>0.5857142857142856</v>
       </c>
       <c r="G9">
-        <v>0.7058823529411765</v>
+        <v>0.6346749226006192</v>
       </c>
       <c r="H9">
-        <v>0.7692307692307693</v>
-      </c>
-      <c r="I9">
-        <v>0.5454545454545454</v>
+        <v>0.4141414141414141</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Qiime2</t>
+          <t>NBC</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>0.6885245901639344</v>
       </c>
       <c r="E10">
-        <v>0.7368421052631579</v>
+        <v>0.525</v>
       </c>
       <c r="F10">
-        <v>0.5</v>
+        <v>0.5957446808510638</v>
       </c>
       <c r="G10">
-        <v>0.5957446808510638</v>
+        <v>0.6481481481481481</v>
       </c>
       <c r="H10">
-        <v>0.673076923076923</v>
-      </c>
-      <c r="I10">
         <v>0.4242424242424243</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>Qiime2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>100 Australian species</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>0.5686274509803921</v>
+      </c>
+      <c r="E11">
+        <v>0.3766233766233766</v>
+      </c>
+      <c r="F11">
+        <v>0.453125</v>
+      </c>
+      <c r="G11">
+        <v>0.5160142348754448</v>
+      </c>
+      <c r="H11">
+        <v>0.2929292929292929</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>VSEARCH</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>make_12s_16s_simulated_reads_5-BetterDatabaseARTSimulation_runEDNAFLOW_16S_Lulu_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
-      </c>
-      <c r="E11">
-        <v>0.7818181818181819</v>
-      </c>
-      <c r="F11">
-        <v>0.4942528735632184</v>
-      </c>
-      <c r="G11">
-        <v>0.6056338028169014</v>
-      </c>
-      <c r="H11">
-        <v>0.7003257328990228</v>
-      </c>
-      <c r="I11">
-        <v>0.4343434343434344</v>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>100 Australian species</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D12">
+        <v>0.7272727272727273</v>
+      </c>
+      <c r="E12">
+        <v>0.4761904761904762</v>
+      </c>
+      <c r="F12">
+        <v>0.5755395683453238</v>
+      </c>
+      <c r="G12">
+        <v>0.6578947368421053</v>
+      </c>
+      <c r="H12">
+        <v>0.404040404040404</v>
       </c>
     </row>
   </sheetData>
@@ -1253,7 +1141,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1267,40 +1155,35 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Pair</t>
+          <t>Query</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Query</t>
+          <t>Subject</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Subject</t>
+          <t>Precision</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Precision</t>
+          <t>Recall</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Recall</t>
+          <t>F1</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>F1</t>
+          <t>F0.5</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>F0.5</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Accuracy</t>
         </is>
@@ -1314,33 +1197,28 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D2">
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0.9333333333333333</v>
+        <v>0.5151515151515151</v>
       </c>
       <c r="F2">
-        <v>0.6666666666666666</v>
+        <v>0.6799999999999999</v>
       </c>
       <c r="G2">
-        <v>0.7777777777777778</v>
+        <v>0.8415841584158416</v>
       </c>
       <c r="H2">
-        <v>0.8641975308641976</v>
-      </c>
-      <c r="I2">
-        <v>0.6666666666666666</v>
+        <v>0.5151515151515151</v>
       </c>
     </row>
     <row r="3">
@@ -1351,33 +1229,28 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>0.9056603773584906</v>
       </c>
       <c r="E3">
-        <v>0.8823529411764706</v>
+        <v>0.5106382978723404</v>
       </c>
       <c r="F3">
-        <v>0.75</v>
+        <v>0.6530612244897959</v>
       </c>
       <c r="G3">
-        <v>0.8108108108108107</v>
+        <v>0.784313725490196</v>
       </c>
       <c r="H3">
-        <v>0.8522727272727273</v>
-      </c>
-      <c r="I3">
-        <v>0.7083333333333334</v>
+        <v>0.4848484848484849</v>
       </c>
     </row>
     <row r="4">
@@ -1388,33 +1261,28 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>0.7761194029850746</v>
       </c>
       <c r="E4">
-        <v>0.8888888888888888</v>
+        <v>0.6190476190476191</v>
       </c>
       <c r="F4">
-        <v>0.8</v>
+        <v>0.6887417218543046</v>
       </c>
       <c r="G4">
-        <v>0.8421052631578948</v>
+        <v>0.7386363636363638</v>
       </c>
       <c r="H4">
-        <v>0.8695652173913044</v>
-      </c>
-      <c r="I4">
-        <v>0.75</v>
+        <v>0.5252525252525253</v>
       </c>
     </row>
     <row r="5">
@@ -1425,33 +1293,28 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>0.7868852459016393</v>
       </c>
       <c r="E5">
-        <v>0.9285714285714286</v>
+        <v>0.5581395348837209</v>
       </c>
       <c r="F5">
-        <v>0.6190476190476191</v>
+        <v>0.6530612244897959</v>
       </c>
       <c r="G5">
-        <v>0.742857142857143</v>
+        <v>0.7272727272727272</v>
       </c>
       <c r="H5">
-        <v>0.8441558441558441</v>
-      </c>
-      <c r="I5">
-        <v>0.625</v>
+        <v>0.4848484848484849</v>
       </c>
     </row>
     <row r="6">
@@ -1462,218 +1325,188 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>0.8181818181818182</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>0.5056179775280899</v>
       </c>
       <c r="F6">
-        <v>0.4090909090909091</v>
+        <v>0.6250000000000001</v>
       </c>
       <c r="G6">
-        <v>0.5806451612903226</v>
+        <v>0.7281553398058251</v>
       </c>
       <c r="H6">
-        <v>0.7758620689655171</v>
-      </c>
-      <c r="I6">
-        <v>0.4583333333333333</v>
+        <v>0.4545454545454545</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MMSeqs2</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>0.9411764705882353</v>
+        <v>0.5151515151515151</v>
       </c>
       <c r="F7">
-        <v>0.7619047619047619</v>
+        <v>0.6799999999999999</v>
       </c>
       <c r="G7">
-        <v>0.8421052631578947</v>
+        <v>0.8415841584158416</v>
       </c>
       <c r="H7">
-        <v>0.898876404494382</v>
-      </c>
-      <c r="I7">
-        <v>0.75</v>
+        <v>0.5151515151515151</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>0.9230769230769231</v>
       </c>
       <c r="E8">
-        <v>0.6923076923076923</v>
+        <v>0.6382978723404256</v>
       </c>
       <c r="F8">
-        <v>0.5</v>
+        <v>0.7547169811320755</v>
       </c>
       <c r="G8">
-        <v>0.5806451612903226</v>
+        <v>0.8474576271186441</v>
       </c>
       <c r="H8">
-        <v>0.6428571428571428</v>
-      </c>
-      <c r="I8">
-        <v>0.4583333333333333</v>
+        <v>0.6060606060606061</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>NBC</t>
+          <t>Mothur</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>0.78125</v>
       </c>
       <c r="E9">
-        <v>0.75</v>
+        <v>0.5882352941176471</v>
       </c>
       <c r="F9">
-        <v>0.6666666666666666</v>
+        <v>0.6711409395973155</v>
       </c>
       <c r="G9">
-        <v>0.7058823529411765</v>
+        <v>0.7331378299120235</v>
       </c>
       <c r="H9">
-        <v>0.7317073170731707</v>
-      </c>
-      <c r="I9">
-        <v>0.5833333333333334</v>
+        <v>0.5050505050505051</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Qiime2</t>
+          <t>NBC</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>0.8387096774193549</v>
       </c>
       <c r="E10">
-        <v>0.8888888888888888</v>
+        <v>0.5842696629213483</v>
       </c>
       <c r="F10">
-        <v>0.3478260869565217</v>
+        <v>0.6887417218543046</v>
       </c>
       <c r="G10">
-        <v>0.5</v>
+        <v>0.7715133531157269</v>
       </c>
       <c r="H10">
-        <v>0.6779661016949152</v>
-      </c>
-      <c r="I10">
-        <v>0.3333333333333333</v>
+        <v>0.5252525252525253</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>TNT</t>
+          <t>Qiime2</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>0.7368421052631579</v>
       </c>
       <c r="E11">
-        <v>0.875</v>
+        <v>0.5</v>
       </c>
       <c r="F11">
-        <v>0.7</v>
+        <v>0.5957446808510638</v>
       </c>
       <c r="G11">
-        <v>0.7777777777777777</v>
+        <v>0.673076923076923</v>
       </c>
       <c r="H11">
-        <v>0.8333333333333334</v>
-      </c>
-      <c r="I11">
-        <v>0.6666666666666666</v>
+        <v>0.4242424242424243</v>
       </c>
     </row>
     <row r="12">
@@ -1684,33 +1517,28 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_12S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D12">
+        <v>0.7818181818181819</v>
       </c>
       <c r="E12">
-        <v>0.6666666666666666</v>
+        <v>0.4942528735632184</v>
       </c>
       <c r="F12">
-        <v>0.4210526315789473</v>
+        <v>0.6056338028169014</v>
       </c>
       <c r="G12">
-        <v>0.5161290322580646</v>
+        <v>0.7003257328990228</v>
       </c>
       <c r="H12">
-        <v>0.5970149253731343</v>
-      </c>
-      <c r="I12">
-        <v>0.375</v>
+        <v>0.4343434343434344</v>
       </c>
     </row>
   </sheetData>
@@ -1720,7 +1548,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1734,40 +1562,35 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Pair</t>
+          <t>Query</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Query</t>
+          <t>Subject</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Subject</t>
+          <t>Precision</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Precision</t>
+          <t>Recall</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Recall</t>
+          <t>F1</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>F1</t>
+          <t>F0.5</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>F0.5</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Accuracy</t>
         </is>
@@ -1781,33 +1604,28 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D2">
+        <v>0.9333333333333333</v>
       </c>
       <c r="E2">
-        <v>0.9</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F2">
-        <v>0.36</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="G2">
-        <v>0.5142857142857143</v>
+        <v>0.8641975308641976</v>
       </c>
       <c r="H2">
-        <v>0.6923076923076923</v>
-      </c>
-      <c r="I2">
-        <v>0.3703703703703703</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="3">
@@ -1818,33 +1636,28 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>0.8823529411764706</v>
       </c>
       <c r="E3">
         <v>0.75</v>
       </c>
       <c r="F3">
-        <v>0.391304347826087</v>
+        <v>0.8108108108108107</v>
       </c>
       <c r="G3">
-        <v>0.5142857142857143</v>
+        <v>0.8522727272727273</v>
       </c>
       <c r="H3">
-        <v>0.6338028169014085</v>
-      </c>
-      <c r="I3">
-        <v>0.3703703703703703</v>
+        <v>0.7083333333333334</v>
       </c>
     </row>
     <row r="4">
@@ -1855,33 +1668,28 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>0.8888888888888888</v>
       </c>
       <c r="E4">
-        <v>0.4545454545454545</v>
+        <v>0.8</v>
       </c>
       <c r="F4">
-        <v>0.7142857142857143</v>
+        <v>0.8421052631578948</v>
       </c>
       <c r="G4">
-        <v>0.5555555555555556</v>
+        <v>0.8695652173913044</v>
       </c>
       <c r="H4">
-        <v>0.4901960784313725</v>
-      </c>
-      <c r="I4">
-        <v>0.4074074074074074</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="5">
@@ -1892,33 +1700,28 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>0.9285714285714286</v>
       </c>
       <c r="E5">
-        <v>0.5625</v>
+        <v>0.6190476190476191</v>
       </c>
       <c r="F5">
-        <v>0.4736842105263158</v>
+        <v>0.742857142857143</v>
       </c>
       <c r="G5">
-        <v>0.5142857142857142</v>
+        <v>0.8441558441558441</v>
       </c>
       <c r="H5">
-        <v>0.5421686746987953</v>
-      </c>
-      <c r="I5">
-        <v>0.3703703703703703</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="6">
@@ -1929,218 +1732,220 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>0.6666666666666666</v>
+        <v>0.4090909090909091</v>
       </c>
       <c r="F6">
-        <v>0.3636363636363636</v>
+        <v>0.5806451612903226</v>
       </c>
       <c r="G6">
-        <v>0.4705882352941177</v>
+        <v>0.7758620689655171</v>
       </c>
       <c r="H6">
-        <v>0.5714285714285715</v>
-      </c>
-      <c r="I6">
-        <v>0.3333333333333333</v>
+        <v>0.4583333333333333</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MMSeqs2</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>0.9333333333333333</v>
       </c>
       <c r="E7">
-        <v>0.7142857142857143</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F7">
-        <v>0.4545454545454545</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="G7">
-        <v>0.5555555555555556</v>
+        <v>0.8641975308641976</v>
       </c>
       <c r="H7">
-        <v>0.6410256410256411</v>
-      </c>
-      <c r="I7">
-        <v>0.4074074074074074</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>0.9411764705882353</v>
       </c>
       <c r="E8">
-        <v>0.5</v>
+        <v>0.7619047619047619</v>
       </c>
       <c r="F8">
-        <v>0.3684210526315789</v>
+        <v>0.8421052631578947</v>
       </c>
       <c r="G8">
-        <v>0.4242424242424242</v>
+        <v>0.898876404494382</v>
       </c>
       <c r="H8">
-        <v>0.4666666666666667</v>
-      </c>
-      <c r="I8">
-        <v>0.2962962962962963</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>NBC</t>
+          <t>Mothur</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>0.6923076923076923</v>
       </c>
       <c r="E9">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="F9">
-        <v>0.36</v>
+        <v>0.5806451612903226</v>
       </c>
       <c r="G9">
-        <v>0.5142857142857143</v>
+        <v>0.6428571428571428</v>
       </c>
       <c r="H9">
-        <v>0.6923076923076923</v>
-      </c>
-      <c r="I9">
-        <v>0.3703703703703703</v>
+        <v>0.4583333333333333</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Qiime2</t>
+          <t>NBC</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>0.8</v>
       </c>
       <c r="E10">
-        <v>0.5</v>
+        <v>0.631578947368421</v>
       </c>
       <c r="F10">
-        <v>0.3</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="G10">
-        <v>0.3749999999999999</v>
+        <v>0.759493670886076</v>
       </c>
       <c r="H10">
-        <v>0.4411764705882353</v>
-      </c>
-      <c r="I10">
-        <v>0.2592592592592592</v>
+        <v>0.5833333333333334</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>Qiime2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Lutjanidae</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="E11">
+        <v>0.3478260869565217</v>
+      </c>
+      <c r="F11">
+        <v>0.5</v>
+      </c>
+      <c r="G11">
+        <v>0.6779661016949152</v>
+      </c>
+      <c r="H11">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>VSEARCH</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>make_12s_16s_simulated_reads_7-Lutjanids_Mock_runEDNAFlow_16S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
-      </c>
-      <c r="E11">
-        <v>0.4615384615384616</v>
-      </c>
-      <c r="F11">
-        <v>0.3157894736842105</v>
-      </c>
-      <c r="G11">
-        <v>0.3749999999999999</v>
-      </c>
-      <c r="H11">
-        <v>0.4225352112676056</v>
-      </c>
-      <c r="I11">
-        <v>0.2592592592592592</v>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Lutjanidae</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D12">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="E12">
+        <v>0.4444444444444444</v>
+      </c>
+      <c r="F12">
+        <v>0.5333333333333333</v>
+      </c>
+      <c r="G12">
+        <v>0.606060606060606</v>
+      </c>
+      <c r="H12">
+        <v>0.4166666666666667</v>
       </c>
     </row>
   </sheetData>
@@ -2150,7 +1955,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2164,40 +1969,35 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Pair</t>
+          <t>Query</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Query</t>
+          <t>Subject</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Subject</t>
+          <t>Precision</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Precision</t>
+          <t>Recall</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Recall</t>
+          <t>F1</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>F1</t>
+          <t>F0.5</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>F0.5</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Accuracy</t>
         </is>
@@ -2211,33 +2011,28 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D2">
+        <v>0.9</v>
       </c>
       <c r="E2">
-        <v>0.9661016949152542</v>
+        <v>0.36</v>
       </c>
       <c r="F2">
-        <v>0.5757575757575758</v>
+        <v>0.5142857142857143</v>
       </c>
       <c r="G2">
-        <v>0.7215189873417721</v>
+        <v>0.6923076923076923</v>
       </c>
       <c r="H2">
-        <v>0.8507462686567164</v>
-      </c>
-      <c r="I2">
-        <v>0.5686274509803921</v>
+        <v>0.3703703703703703</v>
       </c>
     </row>
     <row r="3">
@@ -2248,33 +2043,28 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>0.75</v>
       </c>
       <c r="E3">
-        <v>0.8805970149253731</v>
+        <v>0.391304347826087</v>
       </c>
       <c r="F3">
-        <v>0.6344086021505376</v>
+        <v>0.5142857142857143</v>
       </c>
       <c r="G3">
-        <v>0.7375</v>
+        <v>0.6338028169014085</v>
       </c>
       <c r="H3">
-        <v>0.817174515235457</v>
-      </c>
-      <c r="I3">
-        <v>0.5882352941176471</v>
+        <v>0.3703703703703703</v>
       </c>
     </row>
     <row r="4">
@@ -2285,33 +2075,28 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>0.4545454545454545</v>
       </c>
       <c r="E4">
-        <v>0.8333333333333334</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="F4">
-        <v>0.6741573033707865</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="G4">
-        <v>0.7453416149068324</v>
+        <v>0.4901960784313725</v>
       </c>
       <c r="H4">
-        <v>0.7957559681697614</v>
-      </c>
-      <c r="I4">
-        <v>0.5980392156862745</v>
+        <v>0.4074074074074074</v>
       </c>
     </row>
     <row r="5">
@@ -2322,33 +2107,28 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>0.5625</v>
       </c>
       <c r="E5">
-        <v>0.8636363636363636</v>
+        <v>0.4736842105263158</v>
       </c>
       <c r="F5">
-        <v>0.6195652173913043</v>
+        <v>0.5142857142857142</v>
       </c>
       <c r="G5">
-        <v>0.7215189873417721</v>
+        <v>0.5421686746987953</v>
       </c>
       <c r="H5">
-        <v>0.800561797752809</v>
-      </c>
-      <c r="I5">
-        <v>0.5686274509803921</v>
+        <v>0.3703703703703703</v>
       </c>
     </row>
     <row r="6">
@@ -2359,218 +2139,188 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>0.6666666666666666</v>
       </c>
       <c r="E6">
-        <v>0.9137931034482759</v>
+        <v>0.3636363636363636</v>
       </c>
       <c r="F6">
-        <v>0.5520833333333334</v>
+        <v>0.4705882352941177</v>
       </c>
       <c r="G6">
-        <v>0.6883116883116883</v>
+        <v>0.5714285714285715</v>
       </c>
       <c r="H6">
-        <v>0.8079268292682928</v>
-      </c>
-      <c r="I6">
-        <v>0.5294117647058824</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MMSeqs2</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>0.9</v>
       </c>
       <c r="E7">
-        <v>0.9014084507042254</v>
+        <v>0.36</v>
       </c>
       <c r="F7">
-        <v>0.6808510638297872</v>
+        <v>0.5142857142857143</v>
       </c>
       <c r="G7">
-        <v>0.7757575757575758</v>
+        <v>0.6923076923076923</v>
       </c>
       <c r="H7">
-        <v>0.8465608465608466</v>
-      </c>
-      <c r="I7">
-        <v>0.6372549019607843</v>
+        <v>0.3703703703703703</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>0.7142857142857143</v>
       </c>
       <c r="E8">
-        <v>0.6666666666666666</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="F8">
-        <v>0.525</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="G8">
-        <v>0.5874125874125874</v>
+        <v>0.6410256410256411</v>
       </c>
       <c r="H8">
-        <v>0.6325301204819277</v>
-      </c>
-      <c r="I8">
-        <v>0.4215686274509804</v>
+        <v>0.4074074074074074</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>NBC</t>
+          <t>Mothur</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>0.5</v>
       </c>
       <c r="E9">
-        <v>0.7638888888888888</v>
+        <v>0.3684210526315789</v>
       </c>
       <c r="F9">
-        <v>0.6547619047619048</v>
+        <v>0.4242424242424242</v>
       </c>
       <c r="G9">
-        <v>0.7051282051282051</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="H9">
-        <v>0.739247311827957</v>
-      </c>
-      <c r="I9">
-        <v>0.5490196078431373</v>
+        <v>0.2962962962962963</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Qiime2</t>
+          <t>NBC</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>0.9</v>
       </c>
       <c r="E10">
-        <v>0.6458333333333334</v>
+        <v>0.36</v>
       </c>
       <c r="F10">
-        <v>0.3690476190476191</v>
+        <v>0.5142857142857143</v>
       </c>
       <c r="G10">
-        <v>0.4696969696969697</v>
+        <v>0.6923076923076923</v>
       </c>
       <c r="H10">
-        <v>0.5615942028985508</v>
-      </c>
-      <c r="I10">
-        <v>0.3137254901960784</v>
+        <v>0.3703703703703703</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>TNT</t>
+          <t>Qiime2</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>0.5</v>
       </c>
       <c r="E11">
-        <v>0.8541666666666666</v>
+        <v>0.3</v>
       </c>
       <c r="F11">
-        <v>0.4361702127659575</v>
+        <v>0.3749999999999999</v>
       </c>
       <c r="G11">
-        <v>0.5774647887323944</v>
+        <v>0.4411764705882353</v>
       </c>
       <c r="H11">
-        <v>0.7167832167832168</v>
-      </c>
-      <c r="I11">
-        <v>0.4117647058823529</v>
+        <v>0.2592592592592592</v>
       </c>
     </row>
     <row r="12">
@@ -2581,33 +2331,28 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa_12s_v010_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_12S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>12s_v010_final.fasta</t>
-        </is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D12">
+        <v>0.4615384615384616</v>
       </c>
       <c r="E12">
-        <v>0.7647058823529411</v>
+        <v>0.3157894736842105</v>
       </c>
       <c r="F12">
-        <v>0.611764705882353</v>
+        <v>0.3749999999999999</v>
       </c>
       <c r="G12">
-        <v>0.6797385620915033</v>
+        <v>0.4225352112676056</v>
       </c>
       <c r="H12">
-        <v>0.7282913165266106</v>
-      </c>
-      <c r="I12">
-        <v>0.5196078431372549</v>
+        <v>0.2592592592592592</v>
       </c>
     </row>
   </sheetData>
@@ -2617,7 +2362,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2631,40 +2376,35 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Pair</t>
+          <t>Query</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Query</t>
+          <t>Subject</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Subject</t>
+          <t>Precision</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Precision</t>
+          <t>Recall</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Recall</t>
+          <t>F1</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>F1</t>
+          <t>F0.5</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>F0.5</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Accuracy</t>
         </is>
@@ -2678,33 +2418,28 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D2">
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0.9464285714285714</v>
+        <v>0.52</v>
       </c>
       <c r="F2">
-        <v>0.4953271028037383</v>
+        <v>0.6842105263157895</v>
       </c>
       <c r="G2">
-        <v>0.6503067484662577</v>
+        <v>0.8441558441558442</v>
       </c>
       <c r="H2">
-        <v>0.8006042296072508</v>
-      </c>
-      <c r="I2">
-        <v>0.4910714285714285</v>
+        <v>0.5555555555555556</v>
       </c>
     </row>
     <row r="3">
@@ -2715,33 +2450,28 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>0.9117647058823529</v>
+        <v>0.68</v>
       </c>
       <c r="F3">
-        <v>0.6078431372549019</v>
+        <v>0.8095238095238095</v>
       </c>
       <c r="G3">
-        <v>0.7294117647058823</v>
+        <v>0.913978494623656</v>
       </c>
       <c r="H3">
-        <v>0.8288770053475936</v>
-      </c>
-      <c r="I3">
-        <v>0.5892857142857143</v>
+        <v>0.7037037037037037</v>
       </c>
     </row>
     <row r="4">
@@ -2752,33 +2482,28 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>1</v>
       </c>
       <c r="E4">
-        <v>0.813953488372093</v>
+        <v>0.76</v>
       </c>
       <c r="F4">
-        <v>0.7608695652173914</v>
+        <v>0.8636363636363636</v>
       </c>
       <c r="G4">
-        <v>0.7865168539325844</v>
+        <v>0.9405940594059405</v>
       </c>
       <c r="H4">
-        <v>0.8027522935779817</v>
-      </c>
-      <c r="I4">
-        <v>0.6607142857142857</v>
+        <v>0.7777777777777778</v>
       </c>
     </row>
     <row r="5">
@@ -2789,33 +2514,28 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>0.8625</v>
+        <v>0.44</v>
       </c>
       <c r="F5">
-        <v>0.711340206185567</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="G5">
-        <v>0.7796610169491526</v>
+        <v>0.7971014492753624</v>
       </c>
       <c r="H5">
-        <v>0.8273381294964028</v>
-      </c>
-      <c r="I5">
-        <v>0.6517857142857143</v>
+        <v>0.4814814814814815</v>
       </c>
     </row>
     <row r="6">
@@ -2826,144 +2546,124 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>0.8918918918918919</v>
+        <v>0.24</v>
       </c>
       <c r="F6">
-        <v>0.66</v>
+        <v>0.3870967741935484</v>
       </c>
       <c r="G6">
-        <v>0.7586206896551725</v>
+        <v>0.6122448979591837</v>
       </c>
       <c r="H6">
-        <v>0.8333333333333335</v>
-      </c>
-      <c r="I6">
-        <v>0.625</v>
+        <v>0.2962962962962963</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MMSeqs2</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0.8961038961038961</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>0.6899999999999999</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>0.7796610169491525</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>0.8455882352941176</v>
-      </c>
-      <c r="I7">
-        <v>0.6517857142857143</v>
+        <v>0.07407407407407407</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>0.7093023255813954</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>0.7349397590361446</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>0.7218934911242604</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="I8">
-        <v>0.5803571428571429</v>
+        <v>0.07407407407407407</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>NBC</t>
+          <t>Mothur</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>0.92</v>
       </c>
       <c r="E9">
-        <v>0.7466666666666667</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>0.6292134831460674</v>
+        <v>0.9583333333333334</v>
       </c>
       <c r="G9">
-        <v>0.6829268292682926</v>
+        <v>0.934959349593496</v>
       </c>
       <c r="H9">
-        <v>0.7197943444730078</v>
-      </c>
-      <c r="I9">
-        <v>0.5357142857142857</v>
+        <v>0.9259259259259259</v>
       </c>
     </row>
     <row r="10">
@@ -2974,33 +2674,28 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>0.92</v>
       </c>
       <c r="E10">
-        <v>0.7466666666666667</v>
+        <v>0.9583333333333334</v>
       </c>
       <c r="F10">
-        <v>0.6153846153846154</v>
+        <v>0.9387755102040817</v>
       </c>
       <c r="G10">
-        <v>0.674698795180723</v>
+        <v>0.9274193548387097</v>
       </c>
       <c r="H10">
-        <v>0.7161125319693096</v>
-      </c>
-      <c r="I10">
-        <v>0.5178571428571429</v>
+        <v>0.8888888888888888</v>
       </c>
     </row>
     <row r="11">
@@ -3011,33 +2706,1217 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa_16S_v04_final.fasta</t>
+          <t>Lutjanidae</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>make_12s_16s_simulated_reads_8-Rottnest_runEDNAFLOW_16S_RESULTS_dada2_asv.fa</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>16S_v04_final.fasta</t>
-        </is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>0</v>
       </c>
       <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0.07407407407407407</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Query</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Subject</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Precision</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Recall</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>F1</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>F0.5</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>BLAST100</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D2">
+        <v>0.9661016949152542</v>
+      </c>
+      <c r="E2">
+        <v>0.5757575757575758</v>
+      </c>
+      <c r="F2">
+        <v>0.7215189873417721</v>
+      </c>
+      <c r="G2">
+        <v>0.8507462686567164</v>
+      </c>
+      <c r="H2">
+        <v>0.5686274509803921</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>BLAST97</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>0.8805970149253731</v>
+      </c>
+      <c r="E3">
+        <v>0.6344086021505376</v>
+      </c>
+      <c r="F3">
+        <v>0.7375</v>
+      </c>
+      <c r="G3">
+        <v>0.817174515235457</v>
+      </c>
+      <c r="H3">
+        <v>0.5882352941176471</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Kraken2_0.0</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="E4">
+        <v>0.6741573033707865</v>
+      </c>
+      <c r="F4">
+        <v>0.7453416149068324</v>
+      </c>
+      <c r="G4">
+        <v>0.7957559681697614</v>
+      </c>
+      <c r="H4">
+        <v>0.5980392156862745</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Kraken2_0.05</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>0.8636363636363636</v>
+      </c>
+      <c r="E5">
+        <v>0.6195652173913043</v>
+      </c>
+      <c r="F5">
+        <v>0.7215189873417721</v>
+      </c>
+      <c r="G5">
+        <v>0.800561797752809</v>
+      </c>
+      <c r="H5">
+        <v>0.5686274509803921</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Kraken2_0.1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>0.9137931034482759</v>
+      </c>
+      <c r="E6">
+        <v>0.5520833333333334</v>
+      </c>
+      <c r="F6">
+        <v>0.6883116883116883</v>
+      </c>
+      <c r="G6">
+        <v>0.8079268292682928</v>
+      </c>
+      <c r="H6">
+        <v>0.5294117647058824</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MMSeqs2_100</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>0.9666666666666667</v>
+      </c>
+      <c r="E7">
+        <v>0.5858585858585859</v>
+      </c>
+      <c r="F7">
+        <v>0.729559748427673</v>
+      </c>
+      <c r="G7">
+        <v>0.8554572271386429</v>
+      </c>
+      <c r="H7">
+        <v>0.5784313725490197</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>MMSeqs2_97</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>0.9014084507042254</v>
+      </c>
+      <c r="E8">
+        <v>0.6808510638297872</v>
+      </c>
+      <c r="F8">
+        <v>0.7757575757575758</v>
+      </c>
+      <c r="G8">
+        <v>0.8465608465608466</v>
+      </c>
+      <c r="H8">
+        <v>0.6372549019607843</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Mothur</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="E9">
+        <v>0.525</v>
+      </c>
+      <c r="F9">
+        <v>0.5874125874125874</v>
+      </c>
+      <c r="G9">
+        <v>0.6325301204819277</v>
+      </c>
+      <c r="H9">
+        <v>0.4215686274509804</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>NBC</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>0.7571428571428571</v>
+      </c>
+      <c r="E10">
+        <v>0.6309523809523809</v>
+      </c>
+      <c r="F10">
+        <v>0.6883116883116883</v>
+      </c>
+      <c r="G10">
+        <v>0.7280219780219781</v>
+      </c>
+      <c r="H10">
+        <v>0.5294117647058824</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Qiime2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>0.6458333333333334</v>
+      </c>
+      <c r="E11">
+        <v>0.3690476190476191</v>
+      </c>
+      <c r="F11">
+        <v>0.4696969696969697</v>
+      </c>
+      <c r="G11">
+        <v>0.5615942028985508</v>
+      </c>
+      <c r="H11">
+        <v>0.3137254901960784</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>VSEARCH</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D12">
+        <v>0.7647058823529411</v>
+      </c>
+      <c r="E12">
+        <v>0.611764705882353</v>
+      </c>
+      <c r="F12">
+        <v>0.6797385620915033</v>
+      </c>
+      <c r="G12">
+        <v>0.7282913165266106</v>
+      </c>
+      <c r="H12">
+        <v>0.5196078431372549</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Query</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Subject</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Precision</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Recall</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>F1</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>F0.5</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>BLAST100</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D2">
+        <v>0.9464285714285714</v>
+      </c>
+      <c r="E2">
+        <v>0.4953271028037383</v>
+      </c>
+      <c r="F2">
+        <v>0.6503067484662577</v>
+      </c>
+      <c r="G2">
+        <v>0.8006042296072508</v>
+      </c>
+      <c r="H2">
+        <v>0.4910714285714285</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>BLAST97</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>0.9117647058823529</v>
+      </c>
+      <c r="E3">
+        <v>0.6078431372549019</v>
+      </c>
+      <c r="F3">
+        <v>0.7294117647058823</v>
+      </c>
+      <c r="G3">
+        <v>0.8288770053475936</v>
+      </c>
+      <c r="H3">
+        <v>0.5892857142857143</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Kraken2_0.0</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>0.813953488372093</v>
+      </c>
+      <c r="E4">
+        <v>0.7608695652173914</v>
+      </c>
+      <c r="F4">
+        <v>0.7865168539325844</v>
+      </c>
+      <c r="G4">
+        <v>0.8027522935779817</v>
+      </c>
+      <c r="H4">
+        <v>0.6607142857142857</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Kraken2_0.05</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>0.8625</v>
+      </c>
+      <c r="E5">
+        <v>0.711340206185567</v>
+      </c>
+      <c r="F5">
+        <v>0.7796610169491526</v>
+      </c>
+      <c r="G5">
+        <v>0.8273381294964028</v>
+      </c>
+      <c r="H5">
+        <v>0.6517857142857143</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Kraken2_0.1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>0.8918918918918919</v>
+      </c>
+      <c r="E6">
+        <v>0.66</v>
+      </c>
+      <c r="F6">
+        <v>0.7586206896551725</v>
+      </c>
+      <c r="G6">
+        <v>0.8333333333333335</v>
+      </c>
+      <c r="H6">
+        <v>0.625</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MMSeqs2_100</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>0.9473684210526315</v>
+      </c>
+      <c r="E7">
+        <v>0.5142857142857142</v>
+      </c>
+      <c r="F7">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="G7">
+        <v>0.8108108108108107</v>
+      </c>
+      <c r="H7">
+        <v>0.5178571428571429</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>MMSeqs2_97</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>0.8961038961038961</v>
+      </c>
+      <c r="E8">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="F8">
+        <v>0.7796610169491525</v>
+      </c>
+      <c r="G8">
+        <v>0.8455882352941176</v>
+      </c>
+      <c r="H8">
+        <v>0.6517857142857143</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Mothur</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>0.7093023255813954</v>
+      </c>
+      <c r="E9">
+        <v>0.7349397590361446</v>
+      </c>
+      <c r="F9">
+        <v>0.7218934911242604</v>
+      </c>
+      <c r="G9">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="H9">
+        <v>0.5803571428571429</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>NBC</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>0.7671232876712328</v>
+      </c>
+      <c r="E10">
+        <v>0.6153846153846154</v>
+      </c>
+      <c r="F10">
+        <v>0.6829268292682927</v>
+      </c>
+      <c r="G10">
+        <v>0.7310704960835509</v>
+      </c>
+      <c r="H10">
+        <v>0.5357142857142857</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Qiime2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>0.7466666666666667</v>
+      </c>
+      <c r="E11">
+        <v>0.6153846153846154</v>
+      </c>
+      <c r="F11">
+        <v>0.674698795180723</v>
+      </c>
+      <c r="G11">
+        <v>0.7161125319693096</v>
+      </c>
+      <c r="H11">
+        <v>0.5178571428571429</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>VSEARCH</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D12">
         <v>0.8717948717948718</v>
       </c>
+      <c r="E12">
+        <v>0.6938775510204082</v>
+      </c>
+      <c r="F12">
+        <v>0.7727272727272728</v>
+      </c>
+      <c r="G12">
+        <v>0.8292682926829269</v>
+      </c>
+      <c r="H12">
+        <v>0.6428571428571429</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Type</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Query</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Subject</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Precision</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Recall</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>F1</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>F0.5</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>BLAST100</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D2">
+        <v>0.9625</v>
+      </c>
+      <c r="E2">
+        <v>0.6875</v>
+      </c>
+      <c r="F2">
+        <v>0.8020833333333334</v>
+      </c>
+      <c r="G2">
+        <v>0.8912037037037037</v>
+      </c>
+      <c r="H2">
+        <v>0.6752136752136753</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>BLAST97</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D3">
+        <v>0.9404761904761905</v>
+      </c>
+      <c r="E3">
+        <v>0.7181818181818181</v>
+      </c>
+      <c r="F3">
+        <v>0.8144329896907216</v>
+      </c>
+      <c r="G3">
+        <v>0.8856502242152466</v>
+      </c>
+      <c r="H3">
+        <v>0.6923076923076923</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Kraken2_0.0</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D4">
+        <v>0.9880952380952381</v>
+      </c>
+      <c r="E4">
+        <v>0.7280701754385965</v>
+      </c>
+      <c r="F4">
+        <v>0.8383838383838385</v>
+      </c>
+      <c r="G4">
+        <v>0.9222222222222223</v>
+      </c>
+      <c r="H4">
+        <v>0.7264957264957265</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Kraken2_0.05</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0.6173913043478261</v>
+      </c>
+      <c r="F5">
+        <v>0.7634408602150538</v>
+      </c>
+      <c r="G5">
+        <v>0.8897243107769424</v>
+      </c>
+      <c r="H5">
+        <v>0.6239316239316239</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Kraken2_0.1</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>0.5391304347826087</v>
+      </c>
+      <c r="F6">
+        <v>0.7005649717514124</v>
+      </c>
+      <c r="G6">
+        <v>0.8539944903581267</v>
+      </c>
+      <c r="H6">
+        <v>0.5470085470085471</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>MMSeqs2_100</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0.0170940170940171</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>MMSeqs2_97</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0.0170940170940171</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Mothur</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D9">
+        <v>0.8910891089108911</v>
+      </c>
+      <c r="E9">
+        <v>0.8653846153846154</v>
+      </c>
+      <c r="F9">
+        <v>0.878048780487805</v>
+      </c>
+      <c r="G9">
+        <v>0.8858267716535434</v>
+      </c>
+      <c r="H9">
+        <v>0.7863247863247863</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Qiime2</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D10">
+        <v>0.9361702127659575</v>
+      </c>
+      <c r="E10">
+        <v>0.8073394495412844</v>
+      </c>
+      <c r="F10">
+        <v>0.8669950738916257</v>
+      </c>
+      <c r="G10">
+        <v>0.9072164948453608</v>
+      </c>
+      <c r="H10">
+        <v>0.7692307692307693</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>VSEARCH</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
       <c r="F11">
-        <v>0.68</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>0.7640449438202247</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>0.825242718446602</v>
-      </c>
-      <c r="I11">
-        <v>0.625</v>
+        <v>0.0170940170940171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add exclusion plots for Co1
</commit_message>
<xml_diff>
--- a/results/tables/All_F1_tables.xlsx
+++ b/results/tables/All_F1_tables.xlsx
@@ -849,7 +849,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Kraken2_0.0</t>
+          <t>CustomNBC</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -863,25 +863,25 @@
         </is>
       </c>
       <c r="D4">
-        <v>0.7941176470588235</v>
+        <v>0.6885245901639344</v>
       </c>
       <c r="E4">
-        <v>0.6352941176470588</v>
+        <v>0.525</v>
       </c>
       <c r="F4">
-        <v>0.7058823529411765</v>
+        <v>0.5957446808510638</v>
       </c>
       <c r="G4">
-        <v>0.7563025210084033</v>
+        <v>0.6481481481481481</v>
       </c>
       <c r="H4">
-        <v>0.5454545454545454</v>
+        <v>0.4242424242424243</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kraken2_0.05</t>
+          <t>Kraken2_0.0</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -895,25 +895,25 @@
         </is>
       </c>
       <c r="D5">
-        <v>0.8793103448275862</v>
+        <v>0.7941176470588235</v>
       </c>
       <c r="E5">
-        <v>0.5543478260869565</v>
+        <v>0.6352941176470588</v>
       </c>
       <c r="F5">
-        <v>0.6799999999999999</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="G5">
-        <v>0.787037037037037</v>
+        <v>0.7563025210084033</v>
       </c>
       <c r="H5">
-        <v>0.5151515151515151</v>
+        <v>0.5454545454545454</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kraken2_0.1</t>
+          <t>Kraken2_0.05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -927,25 +927,25 @@
         </is>
       </c>
       <c r="D6">
-        <v>0.9038461538461539</v>
+        <v>0.8793103448275862</v>
       </c>
       <c r="E6">
-        <v>0.5</v>
+        <v>0.5543478260869565</v>
       </c>
       <c r="F6">
-        <v>0.6438356164383562</v>
+        <v>0.6799999999999999</v>
       </c>
       <c r="G6">
-        <v>0.7781456953642384</v>
+        <v>0.787037037037037</v>
       </c>
       <c r="H6">
-        <v>0.4747474747474748</v>
+        <v>0.5151515151515151</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MMSeqs2_100</t>
+          <t>Kraken2_0.1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -959,25 +959,25 @@
         </is>
       </c>
       <c r="D7">
-        <v>0.9076923076923077</v>
+        <v>0.9038461538461539</v>
       </c>
       <c r="E7">
-        <v>0.6344086021505376</v>
+        <v>0.5</v>
       </c>
       <c r="F7">
-        <v>0.7468354430379748</v>
+        <v>0.6438356164383562</v>
       </c>
       <c r="G7">
-        <v>0.8356940509915014</v>
+        <v>0.7781456953642384</v>
       </c>
       <c r="H7">
-        <v>0.5959595959595959</v>
+        <v>0.4747474747474748</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MMSeqs2_97</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -991,16 +991,16 @@
         </is>
       </c>
       <c r="D8">
-        <v>0.8194444444444444</v>
+        <v>0.9076923076923077</v>
       </c>
       <c r="E8">
-        <v>0.686046511627907</v>
+        <v>0.6344086021505376</v>
       </c>
       <c r="F8">
-        <v>0.7468354430379746</v>
+        <v>0.7468354430379748</v>
       </c>
       <c r="G8">
-        <v>0.7887700534759359</v>
+        <v>0.8356940509915014</v>
       </c>
       <c r="H8">
         <v>0.5959595959595959</v>
@@ -1009,7 +1009,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1023,25 +1023,25 @@
         </is>
       </c>
       <c r="D9">
-        <v>0.6721311475409836</v>
+        <v>0.8194444444444444</v>
       </c>
       <c r="E9">
-        <v>0.5189873417721519</v>
+        <v>0.686046511627907</v>
       </c>
       <c r="F9">
-        <v>0.5857142857142856</v>
+        <v>0.7468354430379746</v>
       </c>
       <c r="G9">
-        <v>0.6346749226006192</v>
+        <v>0.7887700534759359</v>
       </c>
       <c r="H9">
-        <v>0.4141414141414141</v>
+        <v>0.5959595959595959</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>NBC</t>
+          <t>Mothur</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1055,19 +1055,19 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.6885245901639344</v>
+        <v>0.6721311475409836</v>
       </c>
       <c r="E10">
-        <v>0.525</v>
+        <v>0.5189873417721519</v>
       </c>
       <c r="F10">
-        <v>0.5957446808510638</v>
+        <v>0.5857142857142856</v>
       </c>
       <c r="G10">
-        <v>0.6481481481481481</v>
+        <v>0.6346749226006192</v>
       </c>
       <c r="H10">
-        <v>0.4242424242424243</v>
+        <v>0.4141414141414141</v>
       </c>
     </row>
     <row r="11">
@@ -1256,7 +1256,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Kraken2_0.0</t>
+          <t>CustomNBC</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1270,16 +1270,16 @@
         </is>
       </c>
       <c r="D4">
-        <v>0.7761194029850746</v>
+        <v>0.8387096774193549</v>
       </c>
       <c r="E4">
-        <v>0.6190476190476191</v>
+        <v>0.5842696629213483</v>
       </c>
       <c r="F4">
         <v>0.6887417218543046</v>
       </c>
       <c r="G4">
-        <v>0.7386363636363638</v>
+        <v>0.7715133531157269</v>
       </c>
       <c r="H4">
         <v>0.5252525252525253</v>
@@ -1288,7 +1288,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kraken2_0.05</t>
+          <t>Kraken2_0.0</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1302,25 +1302,25 @@
         </is>
       </c>
       <c r="D5">
-        <v>0.7868852459016393</v>
+        <v>0.7761194029850746</v>
       </c>
       <c r="E5">
-        <v>0.5581395348837209</v>
+        <v>0.6190476190476191</v>
       </c>
       <c r="F5">
-        <v>0.6530612244897959</v>
+        <v>0.6887417218543046</v>
       </c>
       <c r="G5">
-        <v>0.7272727272727272</v>
+        <v>0.7386363636363638</v>
       </c>
       <c r="H5">
-        <v>0.4848484848484849</v>
+        <v>0.5252525252525253</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kraken2_0.1</t>
+          <t>Kraken2_0.05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1334,25 +1334,25 @@
         </is>
       </c>
       <c r="D6">
-        <v>0.8181818181818182</v>
+        <v>0.7868852459016393</v>
       </c>
       <c r="E6">
-        <v>0.5056179775280899</v>
+        <v>0.5581395348837209</v>
       </c>
       <c r="F6">
-        <v>0.6250000000000001</v>
+        <v>0.6530612244897959</v>
       </c>
       <c r="G6">
-        <v>0.7281553398058251</v>
+        <v>0.7272727272727272</v>
       </c>
       <c r="H6">
-        <v>0.4545454545454545</v>
+        <v>0.4848484848484849</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MMSeqs2_100</t>
+          <t>Kraken2_0.1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1366,25 +1366,25 @@
         </is>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0.8181818181818182</v>
       </c>
       <c r="E7">
-        <v>0.5151515151515151</v>
+        <v>0.5056179775280899</v>
       </c>
       <c r="F7">
-        <v>0.6799999999999999</v>
+        <v>0.6250000000000001</v>
       </c>
       <c r="G7">
-        <v>0.8415841584158416</v>
+        <v>0.7281553398058251</v>
       </c>
       <c r="H7">
-        <v>0.5151515151515151</v>
+        <v>0.4545454545454545</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MMSeqs2_97</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1398,25 +1398,25 @@
         </is>
       </c>
       <c r="D8">
-        <v>0.9230769230769231</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>0.6382978723404256</v>
+        <v>0.5151515151515151</v>
       </c>
       <c r="F8">
-        <v>0.7547169811320755</v>
+        <v>0.6799999999999999</v>
       </c>
       <c r="G8">
-        <v>0.8474576271186441</v>
+        <v>0.8415841584158416</v>
       </c>
       <c r="H8">
-        <v>0.6060606060606061</v>
+        <v>0.5151515151515151</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1430,25 +1430,25 @@
         </is>
       </c>
       <c r="D9">
-        <v>0.78125</v>
+        <v>0.9230769230769231</v>
       </c>
       <c r="E9">
-        <v>0.5882352941176471</v>
+        <v>0.6382978723404256</v>
       </c>
       <c r="F9">
-        <v>0.6711409395973155</v>
+        <v>0.7547169811320755</v>
       </c>
       <c r="G9">
-        <v>0.7331378299120235</v>
+        <v>0.8474576271186441</v>
       </c>
       <c r="H9">
-        <v>0.5050505050505051</v>
+        <v>0.6060606060606061</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>NBC</t>
+          <t>Mothur</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1462,19 +1462,19 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.8387096774193549</v>
+        <v>0.78125</v>
       </c>
       <c r="E10">
-        <v>0.5842696629213483</v>
+        <v>0.5882352941176471</v>
       </c>
       <c r="F10">
-        <v>0.6887417218543046</v>
+        <v>0.6711409395973155</v>
       </c>
       <c r="G10">
-        <v>0.7715133531157269</v>
+        <v>0.7331378299120235</v>
       </c>
       <c r="H10">
-        <v>0.5252525252525253</v>
+        <v>0.5050505050505051</v>
       </c>
     </row>
     <row r="11">
@@ -1663,7 +1663,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Kraken2_0.0</t>
+          <t>CustomNBC</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1677,25 +1677,25 @@
         </is>
       </c>
       <c r="D4">
-        <v>0.8888888888888888</v>
+        <v>0.8</v>
       </c>
       <c r="E4">
-        <v>0.8</v>
+        <v>0.631578947368421</v>
       </c>
       <c r="F4">
-        <v>0.8421052631578948</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="G4">
-        <v>0.8695652173913044</v>
+        <v>0.759493670886076</v>
       </c>
       <c r="H4">
-        <v>0.75</v>
+        <v>0.5833333333333334</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kraken2_0.05</t>
+          <t>Kraken2_0.0</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1709,25 +1709,25 @@
         </is>
       </c>
       <c r="D5">
-        <v>0.9285714285714286</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="E5">
-        <v>0.6190476190476191</v>
+        <v>0.8</v>
       </c>
       <c r="F5">
-        <v>0.742857142857143</v>
+        <v>0.8421052631578948</v>
       </c>
       <c r="G5">
-        <v>0.8441558441558441</v>
+        <v>0.8695652173913044</v>
       </c>
       <c r="H5">
-        <v>0.625</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kraken2_0.1</t>
+          <t>Kraken2_0.05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1741,25 +1741,25 @@
         </is>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="E6">
-        <v>0.4090909090909091</v>
+        <v>0.6190476190476191</v>
       </c>
       <c r="F6">
-        <v>0.5806451612903226</v>
+        <v>0.742857142857143</v>
       </c>
       <c r="G6">
-        <v>0.7758620689655171</v>
+        <v>0.8441558441558441</v>
       </c>
       <c r="H6">
-        <v>0.4583333333333333</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MMSeqs2_100</t>
+          <t>Kraken2_0.1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1773,25 +1773,25 @@
         </is>
       </c>
       <c r="D7">
-        <v>0.9333333333333333</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>0.6666666666666666</v>
+        <v>0.4090909090909091</v>
       </c>
       <c r="F7">
-        <v>0.7777777777777778</v>
+        <v>0.5806451612903226</v>
       </c>
       <c r="G7">
-        <v>0.8641975308641976</v>
+        <v>0.7758620689655171</v>
       </c>
       <c r="H7">
-        <v>0.6666666666666666</v>
+        <v>0.4583333333333333</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MMSeqs2_97</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1805,25 +1805,25 @@
         </is>
       </c>
       <c r="D8">
-        <v>0.9411764705882353</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="E8">
-        <v>0.7619047619047619</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F8">
-        <v>0.8421052631578947</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="G8">
-        <v>0.898876404494382</v>
+        <v>0.8641975308641976</v>
       </c>
       <c r="H8">
-        <v>0.75</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1837,25 +1837,25 @@
         </is>
       </c>
       <c r="D9">
-        <v>0.6923076923076923</v>
+        <v>0.9411764705882353</v>
       </c>
       <c r="E9">
-        <v>0.5</v>
+        <v>0.7619047619047619</v>
       </c>
       <c r="F9">
-        <v>0.5806451612903226</v>
+        <v>0.8421052631578947</v>
       </c>
       <c r="G9">
-        <v>0.6428571428571428</v>
+        <v>0.898876404494382</v>
       </c>
       <c r="H9">
-        <v>0.4583333333333333</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>NBC</t>
+          <t>Mothur</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1869,19 +1869,19 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.8</v>
+        <v>0.6923076923076923</v>
       </c>
       <c r="E10">
-        <v>0.631578947368421</v>
+        <v>0.5</v>
       </c>
       <c r="F10">
-        <v>0.7058823529411765</v>
+        <v>0.5806451612903226</v>
       </c>
       <c r="G10">
-        <v>0.759493670886076</v>
+        <v>0.6428571428571428</v>
       </c>
       <c r="H10">
-        <v>0.5833333333333334</v>
+        <v>0.4583333333333333</v>
       </c>
     </row>
     <row r="11">
@@ -2070,7 +2070,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Kraken2_0.0</t>
+          <t>CustomNBC</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -2084,25 +2084,25 @@
         </is>
       </c>
       <c r="D4">
-        <v>0.4545454545454545</v>
+        <v>0.9</v>
       </c>
       <c r="E4">
-        <v>0.7142857142857143</v>
+        <v>0.36</v>
       </c>
       <c r="F4">
-        <v>0.5555555555555556</v>
+        <v>0.5142857142857143</v>
       </c>
       <c r="G4">
-        <v>0.4901960784313725</v>
+        <v>0.6923076923076923</v>
       </c>
       <c r="H4">
-        <v>0.4074074074074074</v>
+        <v>0.3703703703703703</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kraken2_0.05</t>
+          <t>Kraken2_0.0</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -2116,25 +2116,25 @@
         </is>
       </c>
       <c r="D5">
-        <v>0.5625</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="E5">
-        <v>0.4736842105263158</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="F5">
-        <v>0.5142857142857142</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="G5">
-        <v>0.5421686746987953</v>
+        <v>0.4901960784313725</v>
       </c>
       <c r="H5">
-        <v>0.3703703703703703</v>
+        <v>0.4074074074074074</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kraken2_0.1</t>
+          <t>Kraken2_0.05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -2148,25 +2148,25 @@
         </is>
       </c>
       <c r="D6">
-        <v>0.6666666666666666</v>
+        <v>0.5625</v>
       </c>
       <c r="E6">
-        <v>0.3636363636363636</v>
+        <v>0.4736842105263158</v>
       </c>
       <c r="F6">
-        <v>0.4705882352941177</v>
+        <v>0.5142857142857142</v>
       </c>
       <c r="G6">
-        <v>0.5714285714285715</v>
+        <v>0.5421686746987953</v>
       </c>
       <c r="H6">
-        <v>0.3333333333333333</v>
+        <v>0.3703703703703703</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MMSeqs2_100</t>
+          <t>Kraken2_0.1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2180,25 +2180,25 @@
         </is>
       </c>
       <c r="D7">
-        <v>0.9</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E7">
-        <v>0.36</v>
+        <v>0.3636363636363636</v>
       </c>
       <c r="F7">
-        <v>0.5142857142857143</v>
+        <v>0.4705882352941177</v>
       </c>
       <c r="G7">
-        <v>0.6923076923076923</v>
+        <v>0.5714285714285715</v>
       </c>
       <c r="H7">
-        <v>0.3703703703703703</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MMSeqs2_97</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2212,25 +2212,25 @@
         </is>
       </c>
       <c r="D8">
-        <v>0.7142857142857143</v>
+        <v>0.9</v>
       </c>
       <c r="E8">
-        <v>0.4545454545454545</v>
+        <v>0.36</v>
       </c>
       <c r="F8">
-        <v>0.5555555555555556</v>
+        <v>0.5142857142857143</v>
       </c>
       <c r="G8">
-        <v>0.6410256410256411</v>
+        <v>0.6923076923076923</v>
       </c>
       <c r="H8">
-        <v>0.4074074074074074</v>
+        <v>0.3703703703703703</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2244,25 +2244,25 @@
         </is>
       </c>
       <c r="D9">
-        <v>0.5</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="E9">
-        <v>0.3684210526315789</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="F9">
-        <v>0.4242424242424242</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="G9">
-        <v>0.4666666666666667</v>
+        <v>0.6410256410256411</v>
       </c>
       <c r="H9">
-        <v>0.2962962962962963</v>
+        <v>0.4074074074074074</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>NBC</t>
+          <t>Mothur</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2276,19 +2276,19 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="E10">
-        <v>0.36</v>
+        <v>0.3684210526315789</v>
       </c>
       <c r="F10">
-        <v>0.5142857142857143</v>
+        <v>0.4242424242424242</v>
       </c>
       <c r="G10">
-        <v>0.6923076923076923</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="H10">
-        <v>0.3703703703703703</v>
+        <v>0.2962962962962963</v>
       </c>
     </row>
     <row r="11">
@@ -2852,7 +2852,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Kraken2_0.0</t>
+          <t>CustomNBC</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -2866,25 +2866,25 @@
         </is>
       </c>
       <c r="D4">
-        <v>0.8333333333333334</v>
+        <v>0.7571428571428571</v>
       </c>
       <c r="E4">
-        <v>0.6741573033707865</v>
+        <v>0.6309523809523809</v>
       </c>
       <c r="F4">
-        <v>0.7453416149068324</v>
+        <v>0.6883116883116883</v>
       </c>
       <c r="G4">
-        <v>0.7957559681697614</v>
+        <v>0.7280219780219781</v>
       </c>
       <c r="H4">
-        <v>0.5980392156862745</v>
+        <v>0.5294117647058824</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kraken2_0.05</t>
+          <t>Kraken2_0.0</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -2898,25 +2898,25 @@
         </is>
       </c>
       <c r="D5">
-        <v>0.8636363636363636</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="E5">
-        <v>0.6195652173913043</v>
+        <v>0.6741573033707865</v>
       </c>
       <c r="F5">
-        <v>0.7215189873417721</v>
+        <v>0.7453416149068324</v>
       </c>
       <c r="G5">
-        <v>0.800561797752809</v>
+        <v>0.7957559681697614</v>
       </c>
       <c r="H5">
-        <v>0.5686274509803921</v>
+        <v>0.5980392156862745</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kraken2_0.1</t>
+          <t>Kraken2_0.05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -2930,25 +2930,25 @@
         </is>
       </c>
       <c r="D6">
-        <v>0.9137931034482759</v>
+        <v>0.8636363636363636</v>
       </c>
       <c r="E6">
-        <v>0.5520833333333334</v>
+        <v>0.6195652173913043</v>
       </c>
       <c r="F6">
-        <v>0.6883116883116883</v>
+        <v>0.7215189873417721</v>
       </c>
       <c r="G6">
-        <v>0.8079268292682928</v>
+        <v>0.800561797752809</v>
       </c>
       <c r="H6">
-        <v>0.5294117647058824</v>
+        <v>0.5686274509803921</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MMSeqs2_100</t>
+          <t>Kraken2_0.1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2962,25 +2962,25 @@
         </is>
       </c>
       <c r="D7">
-        <v>0.9666666666666667</v>
+        <v>0.9137931034482759</v>
       </c>
       <c r="E7">
-        <v>0.5858585858585859</v>
+        <v>0.5520833333333334</v>
       </c>
       <c r="F7">
-        <v>0.729559748427673</v>
+        <v>0.6883116883116883</v>
       </c>
       <c r="G7">
-        <v>0.8554572271386429</v>
+        <v>0.8079268292682928</v>
       </c>
       <c r="H7">
-        <v>0.5784313725490197</v>
+        <v>0.5294117647058824</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MMSeqs2_97</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2994,25 +2994,25 @@
         </is>
       </c>
       <c r="D8">
-        <v>0.9014084507042254</v>
+        <v>0.9666666666666667</v>
       </c>
       <c r="E8">
-        <v>0.6808510638297872</v>
+        <v>0.5858585858585859</v>
       </c>
       <c r="F8">
-        <v>0.7757575757575758</v>
+        <v>0.729559748427673</v>
       </c>
       <c r="G8">
-        <v>0.8465608465608466</v>
+        <v>0.8554572271386429</v>
       </c>
       <c r="H8">
-        <v>0.6372549019607843</v>
+        <v>0.5784313725490197</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -3026,25 +3026,25 @@
         </is>
       </c>
       <c r="D9">
-        <v>0.6666666666666666</v>
+        <v>0.9014084507042254</v>
       </c>
       <c r="E9">
-        <v>0.525</v>
+        <v>0.6808510638297872</v>
       </c>
       <c r="F9">
-        <v>0.5874125874125874</v>
+        <v>0.7757575757575758</v>
       </c>
       <c r="G9">
-        <v>0.6325301204819277</v>
+        <v>0.8465608465608466</v>
       </c>
       <c r="H9">
-        <v>0.4215686274509804</v>
+        <v>0.6372549019607843</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>NBC</t>
+          <t>Mothur</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -3058,19 +3058,19 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.7571428571428571</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E10">
-        <v>0.6309523809523809</v>
+        <v>0.525</v>
       </c>
       <c r="F10">
-        <v>0.6883116883116883</v>
+        <v>0.5874125874125874</v>
       </c>
       <c r="G10">
-        <v>0.7280219780219781</v>
+        <v>0.6325301204819277</v>
       </c>
       <c r="H10">
-        <v>0.5294117647058824</v>
+        <v>0.4215686274509804</v>
       </c>
     </row>
     <row r="11">
@@ -3259,7 +3259,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Kraken2_0.0</t>
+          <t>CustomNBC</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -3273,25 +3273,25 @@
         </is>
       </c>
       <c r="D4">
-        <v>0.813953488372093</v>
+        <v>0.7671232876712328</v>
       </c>
       <c r="E4">
-        <v>0.7608695652173914</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="F4">
-        <v>0.7865168539325844</v>
+        <v>0.6829268292682927</v>
       </c>
       <c r="G4">
-        <v>0.8027522935779817</v>
+        <v>0.7310704960835509</v>
       </c>
       <c r="H4">
-        <v>0.6607142857142857</v>
+        <v>0.5357142857142857</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kraken2_0.05</t>
+          <t>Kraken2_0.0</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -3305,25 +3305,25 @@
         </is>
       </c>
       <c r="D5">
-        <v>0.8625</v>
+        <v>0.813953488372093</v>
       </c>
       <c r="E5">
-        <v>0.711340206185567</v>
+        <v>0.7608695652173914</v>
       </c>
       <c r="F5">
-        <v>0.7796610169491526</v>
+        <v>0.7865168539325844</v>
       </c>
       <c r="G5">
-        <v>0.8273381294964028</v>
+        <v>0.8027522935779817</v>
       </c>
       <c r="H5">
-        <v>0.6517857142857143</v>
+        <v>0.6607142857142857</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kraken2_0.1</t>
+          <t>Kraken2_0.05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -3337,25 +3337,25 @@
         </is>
       </c>
       <c r="D6">
-        <v>0.8918918918918919</v>
+        <v>0.8625</v>
       </c>
       <c r="E6">
-        <v>0.66</v>
+        <v>0.711340206185567</v>
       </c>
       <c r="F6">
-        <v>0.7586206896551725</v>
+        <v>0.7796610169491526</v>
       </c>
       <c r="G6">
-        <v>0.8333333333333335</v>
+        <v>0.8273381294964028</v>
       </c>
       <c r="H6">
-        <v>0.625</v>
+        <v>0.6517857142857143</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MMSeqs2_100</t>
+          <t>Kraken2_0.1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -3369,25 +3369,25 @@
         </is>
       </c>
       <c r="D7">
-        <v>0.9473684210526315</v>
+        <v>0.8918918918918919</v>
       </c>
       <c r="E7">
-        <v>0.5142857142857142</v>
+        <v>0.66</v>
       </c>
       <c r="F7">
-        <v>0.6666666666666666</v>
+        <v>0.7586206896551725</v>
       </c>
       <c r="G7">
-        <v>0.8108108108108107</v>
+        <v>0.8333333333333335</v>
       </c>
       <c r="H7">
-        <v>0.5178571428571429</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MMSeqs2_97</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -3401,25 +3401,25 @@
         </is>
       </c>
       <c r="D8">
-        <v>0.8961038961038961</v>
+        <v>0.9473684210526315</v>
       </c>
       <c r="E8">
-        <v>0.6899999999999999</v>
+        <v>0.5142857142857142</v>
       </c>
       <c r="F8">
-        <v>0.7796610169491525</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G8">
-        <v>0.8455882352941176</v>
+        <v>0.8108108108108107</v>
       </c>
       <c r="H8">
-        <v>0.6517857142857143</v>
+        <v>0.5178571428571429</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -3433,25 +3433,25 @@
         </is>
       </c>
       <c r="D9">
-        <v>0.7093023255813954</v>
+        <v>0.8961038961038961</v>
       </c>
       <c r="E9">
-        <v>0.7349397590361446</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F9">
-        <v>0.7218934911242604</v>
+        <v>0.7796610169491525</v>
       </c>
       <c r="G9">
-        <v>0.7142857142857143</v>
+        <v>0.8455882352941176</v>
       </c>
       <c r="H9">
-        <v>0.5803571428571429</v>
+        <v>0.6517857142857143</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>NBC</t>
+          <t>Mothur</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -3465,19 +3465,19 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.7671232876712328</v>
+        <v>0.7093023255813954</v>
       </c>
       <c r="E10">
-        <v>0.6153846153846154</v>
+        <v>0.7349397590361446</v>
       </c>
       <c r="F10">
-        <v>0.6829268292682927</v>
+        <v>0.7218934911242604</v>
       </c>
       <c r="G10">
-        <v>0.7310704960835509</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="H10">
-        <v>0.5357142857142857</v>
+        <v>0.5803571428571429</v>
       </c>
     </row>
     <row r="11">

</xml_diff>

<commit_message>
Update README. Add input data.
</commit_message>
<xml_diff>
--- a/results/tables/All_F1_tables.xlsx
+++ b/results/tables/All_F1_tables.xlsx
@@ -359,7 +359,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -415,28 +415,28 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>100 Australian speces</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D2">
-        <v>0.9795918367346939</v>
+        <v>0.9076923076923077</v>
       </c>
       <c r="E2">
-        <v>0.6666666666666666</v>
+        <v>0.6344086021505376</v>
       </c>
       <c r="F2">
-        <v>0.793388429752066</v>
+        <v>0.7468354430379748</v>
       </c>
       <c r="G2">
-        <v>0.8955223880597016</v>
+        <v>0.8356940509915014</v>
       </c>
       <c r="H2">
-        <v>0.7474747474747475</v>
+        <v>0.5959595959595959</v>
       </c>
     </row>
     <row r="3">
@@ -447,284 +447,316 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>100 Australian speces</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D3">
-        <v>0.9583333333333334</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="E3">
-        <v>0.6666666666666666</v>
+        <v>0.5274725274725275</v>
       </c>
       <c r="F3">
-        <v>0.7863247863247863</v>
+        <v>0.6530612244897959</v>
       </c>
       <c r="G3">
-        <v>0.8812260536398469</v>
+        <v>0.761904761904762</v>
       </c>
       <c r="H3">
-        <v>0.7474747474747475</v>
+        <v>0.4848484848484849</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Kraken2_0.0</t>
+          <t>CustomNBC</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>100 Australian speces</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D4">
-        <v>0.96</v>
+        <v>0.6885245901639344</v>
       </c>
       <c r="E4">
-        <v>0.6956521739130435</v>
+        <v>0.525</v>
       </c>
       <c r="F4">
-        <v>0.8067226890756302</v>
+        <v>0.5957446808510638</v>
       </c>
       <c r="G4">
-        <v>0.8921933085501859</v>
+        <v>0.6481481481481481</v>
       </c>
       <c r="H4">
-        <v>0.7676767676767676</v>
+        <v>0.4242424242424243</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kraken2_0.05</t>
+          <t>Kraken2_0.0</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>100 Australian speces</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D5">
-        <v>0.9743589743589743</v>
+        <v>0.7941176470588235</v>
       </c>
       <c r="E5">
-        <v>0.5428571428571428</v>
+        <v>0.6352941176470588</v>
       </c>
       <c r="F5">
-        <v>0.6972477064220183</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="G5">
-        <v>0.8407079646017698</v>
+        <v>0.7563025210084033</v>
       </c>
       <c r="H5">
-        <v>0.6666666666666666</v>
+        <v>0.5454545454545454</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kraken2_0.1</t>
+          <t>Kraken2_0.05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>100 Australian speces</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D6">
-        <v>0.9642857142857143</v>
+        <v>0.8793103448275862</v>
       </c>
       <c r="E6">
-        <v>0.3857142857142857</v>
+        <v>0.5543478260869565</v>
       </c>
       <c r="F6">
-        <v>0.5510204081632653</v>
+        <v>0.6799999999999999</v>
       </c>
       <c r="G6">
-        <v>0.7417582417582418</v>
+        <v>0.787037037037037</v>
       </c>
       <c r="H6">
-        <v>0.5555555555555556</v>
+        <v>0.5151515151515151</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MMSeqs2_100</t>
+          <t>Kraken2_0.1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>100 Australian speces</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>0.9038461538461539</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>0.6438356164383562</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>0.7781456953642384</v>
       </c>
       <c r="H7">
-        <v>0.2828282828282828</v>
+        <v>0.4747474747474748</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MMSeqs2_97</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>100 Australian speces</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>0.9076923076923077</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.6344086021505376</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>0.7468354430379748</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>0.8356940509915014</v>
       </c>
       <c r="H8">
-        <v>0.2828282828282828</v>
+        <v>0.5959595959595959</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>100 Australian speces</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D9">
-        <v>0.8666666666666667</v>
+        <v>0.8194444444444444</v>
       </c>
       <c r="E9">
-        <v>0.8253968253968254</v>
+        <v>0.686046511627907</v>
       </c>
       <c r="F9">
-        <v>0.8455284552845528</v>
+        <v>0.7468354430379746</v>
       </c>
       <c r="G9">
-        <v>0.8580858085808584</v>
+        <v>0.7887700534759359</v>
       </c>
       <c r="H9">
-        <v>0.8080808080808081</v>
+        <v>0.5959595959595959</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Qiime2</t>
+          <t>Mothur</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>100 Australian speces</t>
+          <t>100 Australian species</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D10">
-        <v>0.8909090909090909</v>
+        <v>0.6721311475409836</v>
       </c>
       <c r="E10">
-        <v>0.5833333333333334</v>
+        <v>0.5189873417721519</v>
       </c>
       <c r="F10">
-        <v>0.7050359712230215</v>
+        <v>0.5857142857142856</v>
       </c>
       <c r="G10">
-        <v>0.8059210526315789</v>
+        <v>0.6346749226006192</v>
       </c>
       <c r="H10">
-        <v>0.5858585858585859</v>
+        <v>0.4141414141414141</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>Qiime2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>100 Australian species</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>0.5686274509803921</v>
+      </c>
+      <c r="E11">
+        <v>0.3766233766233766</v>
+      </c>
+      <c r="F11">
+        <v>0.453125</v>
+      </c>
+      <c r="G11">
+        <v>0.5160142348754448</v>
+      </c>
+      <c r="H11">
+        <v>0.2929292929292929</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>VSEARCH</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>100 Australian speces</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>CO1</t>
-        </is>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0.2828282828282828</v>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>100 Australian species</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D12">
+        <v>0.7272727272727273</v>
+      </c>
+      <c r="E12">
+        <v>0.4761904761904762</v>
+      </c>
+      <c r="F12">
+        <v>0.5755395683453238</v>
+      </c>
+      <c r="G12">
+        <v>0.6578947368421053</v>
+      </c>
+      <c r="H12">
+        <v>0.404040404040404</v>
       </c>
     </row>
   </sheetData>
@@ -795,23 +827,23 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D2">
-        <v>0.9076923076923077</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0.6344086021505376</v>
+        <v>0.5151515151515151</v>
       </c>
       <c r="F2">
-        <v>0.7468354430379748</v>
+        <v>0.6799999999999999</v>
       </c>
       <c r="G2">
-        <v>0.8356940509915014</v>
+        <v>0.8415841584158416</v>
       </c>
       <c r="H2">
-        <v>0.5959595959595959</v>
+        <v>0.5151515151515151</v>
       </c>
     </row>
     <row r="3">
@@ -827,20 +859,20 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D3">
-        <v>0.8571428571428571</v>
+        <v>0.9056603773584906</v>
       </c>
       <c r="E3">
-        <v>0.5274725274725275</v>
+        <v>0.5106382978723404</v>
       </c>
       <c r="F3">
         <v>0.6530612244897959</v>
       </c>
       <c r="G3">
-        <v>0.761904761904762</v>
+        <v>0.784313725490196</v>
       </c>
       <c r="H3">
         <v>0.4848484848484849</v>
@@ -859,23 +891,23 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D4">
-        <v>0.6885245901639344</v>
+        <v>0.8387096774193549</v>
       </c>
       <c r="E4">
-        <v>0.525</v>
+        <v>0.5842696629213483</v>
       </c>
       <c r="F4">
-        <v>0.5957446808510638</v>
+        <v>0.6887417218543046</v>
       </c>
       <c r="G4">
-        <v>0.6481481481481481</v>
+        <v>0.7715133531157269</v>
       </c>
       <c r="H4">
-        <v>0.4242424242424243</v>
+        <v>0.5252525252525253</v>
       </c>
     </row>
     <row r="5">
@@ -891,23 +923,23 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D5">
-        <v>0.7941176470588235</v>
+        <v>0.7761194029850746</v>
       </c>
       <c r="E5">
-        <v>0.6352941176470588</v>
+        <v>0.6190476190476191</v>
       </c>
       <c r="F5">
-        <v>0.7058823529411765</v>
+        <v>0.6887417218543046</v>
       </c>
       <c r="G5">
-        <v>0.7563025210084033</v>
+        <v>0.7386363636363638</v>
       </c>
       <c r="H5">
-        <v>0.5454545454545454</v>
+        <v>0.5252525252525253</v>
       </c>
     </row>
     <row r="6">
@@ -923,23 +955,23 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D6">
-        <v>0.8793103448275862</v>
+        <v>0.7868852459016393</v>
       </c>
       <c r="E6">
-        <v>0.5543478260869565</v>
+        <v>0.5581395348837209</v>
       </c>
       <c r="F6">
-        <v>0.6799999999999999</v>
+        <v>0.6530612244897959</v>
       </c>
       <c r="G6">
-        <v>0.787037037037037</v>
+        <v>0.7272727272727272</v>
       </c>
       <c r="H6">
-        <v>0.5151515151515151</v>
+        <v>0.4848484848484849</v>
       </c>
     </row>
     <row r="7">
@@ -955,23 +987,23 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D7">
-        <v>0.9038461538461539</v>
+        <v>0.8181818181818182</v>
       </c>
       <c r="E7">
-        <v>0.5</v>
+        <v>0.5056179775280899</v>
       </c>
       <c r="F7">
-        <v>0.6438356164383562</v>
+        <v>0.6250000000000001</v>
       </c>
       <c r="G7">
-        <v>0.7781456953642384</v>
+        <v>0.7281553398058251</v>
       </c>
       <c r="H7">
-        <v>0.4747474747474748</v>
+        <v>0.4545454545454545</v>
       </c>
     </row>
     <row r="8">
@@ -987,23 +1019,23 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D8">
-        <v>0.9076923076923077</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>0.6344086021505376</v>
+        <v>0.5151515151515151</v>
       </c>
       <c r="F8">
-        <v>0.7468354430379748</v>
+        <v>0.6799999999999999</v>
       </c>
       <c r="G8">
-        <v>0.8356940509915014</v>
+        <v>0.8415841584158416</v>
       </c>
       <c r="H8">
-        <v>0.5959595959595959</v>
+        <v>0.5151515151515151</v>
       </c>
     </row>
     <row r="9">
@@ -1019,23 +1051,23 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D9">
-        <v>0.8194444444444444</v>
+        <v>0.9230769230769231</v>
       </c>
       <c r="E9">
-        <v>0.686046511627907</v>
+        <v>0.6382978723404256</v>
       </c>
       <c r="F9">
-        <v>0.7468354430379746</v>
+        <v>0.7547169811320755</v>
       </c>
       <c r="G9">
-        <v>0.7887700534759359</v>
+        <v>0.8474576271186441</v>
       </c>
       <c r="H9">
-        <v>0.5959595959595959</v>
+        <v>0.6060606060606061</v>
       </c>
     </row>
     <row r="10">
@@ -1051,23 +1083,23 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D10">
-        <v>0.6721311475409836</v>
+        <v>0.78125</v>
       </c>
       <c r="E10">
-        <v>0.5189873417721519</v>
+        <v>0.5882352941176471</v>
       </c>
       <c r="F10">
-        <v>0.5857142857142856</v>
+        <v>0.6711409395973155</v>
       </c>
       <c r="G10">
-        <v>0.6346749226006192</v>
+        <v>0.7331378299120235</v>
       </c>
       <c r="H10">
-        <v>0.4141414141414141</v>
+        <v>0.5050505050505051</v>
       </c>
     </row>
     <row r="11">
@@ -1083,23 +1115,23 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D11">
-        <v>0.5686274509803921</v>
+        <v>0.7368421052631579</v>
       </c>
       <c r="E11">
-        <v>0.3766233766233766</v>
+        <v>0.5</v>
       </c>
       <c r="F11">
-        <v>0.453125</v>
+        <v>0.5957446808510638</v>
       </c>
       <c r="G11">
-        <v>0.5160142348754448</v>
+        <v>0.673076923076923</v>
       </c>
       <c r="H11">
-        <v>0.2929292929292929</v>
+        <v>0.4242424242424243</v>
       </c>
     </row>
     <row r="12">
@@ -1115,23 +1147,23 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D12">
-        <v>0.7272727272727273</v>
+        <v>0.7818181818181819</v>
       </c>
       <c r="E12">
-        <v>0.4761904761904762</v>
+        <v>0.4942528735632184</v>
       </c>
       <c r="F12">
-        <v>0.5755395683453238</v>
+        <v>0.6056338028169014</v>
       </c>
       <c r="G12">
-        <v>0.6578947368421053</v>
+        <v>0.7003257328990228</v>
       </c>
       <c r="H12">
-        <v>0.404040404040404</v>
+        <v>0.4343434343434344</v>
       </c>
     </row>
   </sheetData>
@@ -1141,7 +1173,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1202,23 +1234,23 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>16S</t>
+          <t>CO1</t>
         </is>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0.9795918367346939</v>
       </c>
       <c r="E2">
-        <v>0.5151515151515151</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F2">
-        <v>0.6799999999999999</v>
+        <v>0.793388429752066</v>
       </c>
       <c r="G2">
-        <v>0.8415841584158416</v>
+        <v>0.8955223880597016</v>
       </c>
       <c r="H2">
-        <v>0.5151515151515151</v>
+        <v>0.7474747474747475</v>
       </c>
     </row>
     <row r="3">
@@ -1234,29 +1266,29 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>16S</t>
+          <t>CO1</t>
         </is>
       </c>
       <c r="D3">
-        <v>0.9056603773584906</v>
+        <v>0.9583333333333334</v>
       </c>
       <c r="E3">
-        <v>0.5106382978723404</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F3">
-        <v>0.6530612244897959</v>
+        <v>0.7863247863247863</v>
       </c>
       <c r="G3">
-        <v>0.784313725490196</v>
+        <v>0.8812260536398469</v>
       </c>
       <c r="H3">
-        <v>0.4848484848484849</v>
+        <v>0.7474747474747475</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CustomNBC</t>
+          <t>Kraken2_0.0</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1266,29 +1298,29 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>16S</t>
+          <t>CO1</t>
         </is>
       </c>
       <c r="D4">
-        <v>0.8387096774193549</v>
+        <v>0.96</v>
       </c>
       <c r="E4">
-        <v>0.5842696629213483</v>
+        <v>0.6956521739130435</v>
       </c>
       <c r="F4">
-        <v>0.6887417218543046</v>
+        <v>0.8067226890756302</v>
       </c>
       <c r="G4">
-        <v>0.7715133531157269</v>
+        <v>0.8921933085501859</v>
       </c>
       <c r="H4">
-        <v>0.5252525252525253</v>
+        <v>0.7676767676767676</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kraken2_0.0</t>
+          <t>Kraken2_0.05</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1298,29 +1330,29 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>16S</t>
+          <t>CO1</t>
         </is>
       </c>
       <c r="D5">
-        <v>0.7761194029850746</v>
+        <v>0.9743589743589743</v>
       </c>
       <c r="E5">
-        <v>0.6190476190476191</v>
+        <v>0.5428571428571428</v>
       </c>
       <c r="F5">
-        <v>0.6887417218543046</v>
+        <v>0.6972477064220183</v>
       </c>
       <c r="G5">
-        <v>0.7386363636363638</v>
+        <v>0.8407079646017698</v>
       </c>
       <c r="H5">
-        <v>0.5252525252525253</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kraken2_0.05</t>
+          <t>Kraken2_0.1</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1330,29 +1362,29 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>16S</t>
+          <t>CO1</t>
         </is>
       </c>
       <c r="D6">
-        <v>0.7868852459016393</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="E6">
-        <v>0.5581395348837209</v>
+        <v>0.3857142857142857</v>
       </c>
       <c r="F6">
-        <v>0.6530612244897959</v>
+        <v>0.5510204081632653</v>
       </c>
       <c r="G6">
-        <v>0.7272727272727272</v>
+        <v>0.7417582417582418</v>
       </c>
       <c r="H6">
-        <v>0.4848484848484849</v>
+        <v>0.5555555555555556</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Kraken2_0.1</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1362,29 +1394,29 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>16S</t>
+          <t>CO1</t>
         </is>
       </c>
       <c r="D7">
-        <v>0.8181818181818182</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0.5056179775280899</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>0.6250000000000001</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>0.7281553398058251</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>0.4545454545454545</v>
+        <v>0.2828282828282828</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MMSeqs2_100</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1394,29 +1426,29 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>16S</t>
+          <t>CO1</t>
         </is>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>0.5151515151515151</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>0.6799999999999999</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>0.8415841584158416</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>0.5151515151515151</v>
+        <v>0.2828282828282828</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MMSeqs2_97</t>
+          <t>Mothur</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1426,29 +1458,29 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>16S</t>
+          <t>CO1</t>
         </is>
       </c>
       <c r="D9">
-        <v>0.9230769230769231</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="E9">
-        <v>0.6382978723404256</v>
+        <v>0.8253968253968254</v>
       </c>
       <c r="F9">
-        <v>0.7547169811320755</v>
+        <v>0.8455284552845528</v>
       </c>
       <c r="G9">
-        <v>0.8474576271186441</v>
+        <v>0.8580858085808584</v>
       </c>
       <c r="H9">
-        <v>0.6060606060606061</v>
+        <v>0.8080808080808081</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>Qiime2</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1458,29 +1490,29 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>16S</t>
+          <t>CO1</t>
         </is>
       </c>
       <c r="D10">
-        <v>0.78125</v>
+        <v>0.8909090909090909</v>
       </c>
       <c r="E10">
-        <v>0.5882352941176471</v>
+        <v>0.5833333333333334</v>
       </c>
       <c r="F10">
-        <v>0.6711409395973155</v>
+        <v>0.7050359712230215</v>
       </c>
       <c r="G10">
-        <v>0.7331378299120235</v>
+        <v>0.8059210526315789</v>
       </c>
       <c r="H10">
-        <v>0.5050505050505051</v>
+        <v>0.5858585858585859</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Qiime2</t>
+          <t>VSEARCH</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1490,55 +1522,23 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>16S</t>
+          <t>CO1</t>
         </is>
       </c>
       <c r="D11">
-        <v>0.7368421052631579</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F11">
-        <v>0.5957446808510638</v>
+        <v>0</v>
       </c>
       <c r="G11">
-        <v>0.673076923076923</v>
+        <v>0</v>
       </c>
       <c r="H11">
-        <v>0.4242424242424243</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>VSEARCH</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>100 Australian species</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>16S</t>
-        </is>
-      </c>
-      <c r="D12">
-        <v>0.7818181818181819</v>
-      </c>
-      <c r="E12">
-        <v>0.4942528735632184</v>
-      </c>
-      <c r="F12">
-        <v>0.6056338028169014</v>
-      </c>
-      <c r="G12">
-        <v>0.7003257328990228</v>
-      </c>
-      <c r="H12">
-        <v>0.4343434343434344</v>
+        <v>0.2828282828282828</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add CustomNBC for CO1
</commit_message>
<xml_diff>
--- a/results/tables/All_F1_tables.xlsx
+++ b/results/tables/All_F1_tables.xlsx
@@ -1173,7 +1173,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1288,7 +1288,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Kraken2_0.0</t>
+          <t>CustomNBC</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -1302,25 +1302,25 @@
         </is>
       </c>
       <c r="D4">
-        <v>0.96</v>
+        <v>0.864406779661017</v>
       </c>
       <c r="E4">
-        <v>0.6956521739130435</v>
+        <v>0.8095238095238095</v>
       </c>
       <c r="F4">
-        <v>0.8067226890756302</v>
+        <v>0.8360655737704918</v>
       </c>
       <c r="G4">
-        <v>0.8921933085501859</v>
+        <v>0.8528428093645484</v>
       </c>
       <c r="H4">
-        <v>0.7676767676767676</v>
+        <v>0.797979797979798</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kraken2_0.05</t>
+          <t>Kraken2_0.0</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1334,25 +1334,25 @@
         </is>
       </c>
       <c r="D5">
-        <v>0.9743589743589743</v>
+        <v>0.96</v>
       </c>
       <c r="E5">
-        <v>0.5428571428571428</v>
+        <v>0.6956521739130435</v>
       </c>
       <c r="F5">
-        <v>0.6972477064220183</v>
+        <v>0.8067226890756302</v>
       </c>
       <c r="G5">
-        <v>0.8407079646017698</v>
+        <v>0.8921933085501859</v>
       </c>
       <c r="H5">
-        <v>0.6666666666666666</v>
+        <v>0.7676767676767676</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kraken2_0.1</t>
+          <t>Kraken2_0.05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1366,25 +1366,25 @@
         </is>
       </c>
       <c r="D6">
-        <v>0.9642857142857143</v>
+        <v>0.9743589743589743</v>
       </c>
       <c r="E6">
-        <v>0.3857142857142857</v>
+        <v>0.5428571428571428</v>
       </c>
       <c r="F6">
-        <v>0.5510204081632653</v>
+        <v>0.6972477064220183</v>
       </c>
       <c r="G6">
-        <v>0.7417582417582418</v>
+        <v>0.8407079646017698</v>
       </c>
       <c r="H6">
-        <v>0.5555555555555556</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MMSeqs2_100</t>
+          <t>Kraken2_0.1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1398,25 +1398,25 @@
         </is>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.3857142857142857</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>0.5510204081632653</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>0.7417582417582418</v>
       </c>
       <c r="H7">
-        <v>0.2828282828282828</v>
+        <v>0.5555555555555556</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MMSeqs2_97</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1448,7 +1448,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1462,25 +1462,25 @@
         </is>
       </c>
       <c r="D9">
-        <v>0.8666666666666667</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0.8253968253968254</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>0.8455284552845528</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>0.8580858085808584</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>0.8080808080808081</v>
+        <v>0.2828282828282828</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Qiime2</t>
+          <t>Mothur</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1494,50 +1494,82 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.8909090909090909</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="E10">
-        <v>0.5833333333333334</v>
+        <v>0.8253968253968254</v>
       </c>
       <c r="F10">
-        <v>0.7050359712230215</v>
+        <v>0.8455284552845528</v>
       </c>
       <c r="G10">
-        <v>0.8059210526315789</v>
+        <v>0.8580858085808584</v>
       </c>
       <c r="H10">
-        <v>0.5858585858585859</v>
+        <v>0.8080808080808081</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>Qiime2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>100 Australian species</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>0.8909090909090909</v>
+      </c>
+      <c r="E11">
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="F11">
+        <v>0.7050359712230215</v>
+      </c>
+      <c r="G11">
+        <v>0.8059210526315789</v>
+      </c>
+      <c r="H11">
+        <v>0.5858585858585859</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>VSEARCH</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>100 Australian species</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>CO1</t>
         </is>
       </c>
-      <c r="D11">
+      <c r="D12">
         <v>0</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>0</v>
       </c>
-      <c r="F11">
+      <c r="F12">
         <v>0</v>
       </c>
-      <c r="G11">
+      <c r="G12">
         <v>0</v>
       </c>
-      <c r="H11">
+      <c r="H12">
         <v>0.2828282828282828</v>
       </c>
     </row>
@@ -2362,7 +2394,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2477,7 +2509,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Kraken2_0.0</t>
+          <t>CustomNBC</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -2491,25 +2523,25 @@
         </is>
       </c>
       <c r="D4">
+        <v>0.92</v>
+      </c>
+      <c r="E4">
         <v>1</v>
       </c>
-      <c r="E4">
-        <v>0.76</v>
-      </c>
       <c r="F4">
-        <v>0.8636363636363636</v>
+        <v>0.9583333333333334</v>
       </c>
       <c r="G4">
-        <v>0.9405940594059405</v>
+        <v>0.934959349593496</v>
       </c>
       <c r="H4">
-        <v>0.7777777777777778</v>
+        <v>0.9259259259259259</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kraken2_0.05</t>
+          <t>Kraken2_0.0</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -2526,22 +2558,22 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>0.44</v>
+        <v>0.76</v>
       </c>
       <c r="F5">
-        <v>0.6111111111111112</v>
+        <v>0.8636363636363636</v>
       </c>
       <c r="G5">
-        <v>0.7971014492753624</v>
+        <v>0.9405940594059405</v>
       </c>
       <c r="H5">
-        <v>0.4814814814814815</v>
+        <v>0.7777777777777778</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kraken2_0.1</t>
+          <t>Kraken2_0.05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -2558,22 +2590,22 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>0.24</v>
+        <v>0.44</v>
       </c>
       <c r="F6">
-        <v>0.3870967741935484</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="G6">
-        <v>0.6122448979591837</v>
+        <v>0.7971014492753624</v>
       </c>
       <c r="H6">
-        <v>0.2962962962962963</v>
+        <v>0.4814814814814815</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MMSeqs2_100</t>
+          <t>Kraken2_0.1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2587,25 +2619,25 @@
         </is>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.24</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>0.3870967741935484</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>0.6122448979591837</v>
       </c>
       <c r="H7">
-        <v>0.07407407407407407</v>
+        <v>0.2962962962962963</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MMSeqs2_97</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2637,7 +2669,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2651,25 +2683,25 @@
         </is>
       </c>
       <c r="D9">
-        <v>0.92</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>0.9583333333333334</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>0.934959349593496</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>0.9259259259259259</v>
+        <v>0.07407407407407407</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Qiime2</t>
+          <t>Mothur</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2686,47 +2718,79 @@
         <v>0.92</v>
       </c>
       <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
         <v>0.9583333333333334</v>
       </c>
-      <c r="F10">
-        <v>0.9387755102040817</v>
-      </c>
       <c r="G10">
-        <v>0.9274193548387097</v>
+        <v>0.934959349593496</v>
       </c>
       <c r="H10">
-        <v>0.8888888888888888</v>
+        <v>0.9259259259259259</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>Qiime2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Lutjanidae</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>0.92</v>
+      </c>
+      <c r="E11">
+        <v>0.9583333333333334</v>
+      </c>
+      <c r="F11">
+        <v>0.9387755102040817</v>
+      </c>
+      <c r="G11">
+        <v>0.9274193548387097</v>
+      </c>
+      <c r="H11">
+        <v>0.8888888888888888</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>VSEARCH</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>Lutjanidae</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>CO1</t>
         </is>
       </c>
-      <c r="D11">
+      <c r="D12">
         <v>0</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>0</v>
       </c>
-      <c r="F11">
+      <c r="F12">
         <v>0</v>
       </c>
-      <c r="G11">
+      <c r="G12">
         <v>0</v>
       </c>
-      <c r="H11">
+      <c r="H12">
         <v>0.07407407407407407</v>
       </c>
     </row>
@@ -3551,7 +3615,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3666,7 +3730,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Kraken2_0.0</t>
+          <t>CustomNBC</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -3680,25 +3744,25 @@
         </is>
       </c>
       <c r="D4">
-        <v>0.9880952380952381</v>
+        <v>0.9101123595505618</v>
       </c>
       <c r="E4">
-        <v>0.7280701754385965</v>
+        <v>0.7570093457943925</v>
       </c>
       <c r="F4">
-        <v>0.8383838383838385</v>
+        <v>0.826530612244898</v>
       </c>
       <c r="G4">
-        <v>0.9222222222222223</v>
+        <v>0.8747300215982722</v>
       </c>
       <c r="H4">
-        <v>0.7264957264957265</v>
+        <v>0.7094017094017094</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kraken2_0.05</t>
+          <t>Kraken2_0.0</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -3712,25 +3776,25 @@
         </is>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0.9880952380952381</v>
       </c>
       <c r="E5">
-        <v>0.6173913043478261</v>
+        <v>0.7280701754385965</v>
       </c>
       <c r="F5">
-        <v>0.7634408602150538</v>
+        <v>0.8383838383838385</v>
       </c>
       <c r="G5">
-        <v>0.8897243107769424</v>
+        <v>0.9222222222222223</v>
       </c>
       <c r="H5">
-        <v>0.6239316239316239</v>
+        <v>0.7264957264957265</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kraken2_0.1</t>
+          <t>Kraken2_0.05</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -3747,22 +3811,22 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>0.5391304347826087</v>
+        <v>0.6173913043478261</v>
       </c>
       <c r="F6">
-        <v>0.7005649717514124</v>
+        <v>0.7634408602150538</v>
       </c>
       <c r="G6">
-        <v>0.8539944903581267</v>
+        <v>0.8897243107769424</v>
       </c>
       <c r="H6">
-        <v>0.5470085470085471</v>
+        <v>0.6239316239316239</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MMSeqs2_100</t>
+          <t>Kraken2_0.1</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -3776,25 +3840,25 @@
         </is>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.5391304347826087</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>0.7005649717514124</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>0.8539944903581267</v>
       </c>
       <c r="H7">
-        <v>0.0170940170940171</v>
+        <v>0.5470085470085471</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MMSeqs2_97</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -3826,7 +3890,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -3840,25 +3904,25 @@
         </is>
       </c>
       <c r="D9">
-        <v>0.8910891089108911</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0.8653846153846154</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>0.878048780487805</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>0.8858267716535434</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>0.7863247863247863</v>
+        <v>0.0170940170940171</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Qiime2</t>
+          <t>Mothur</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -3872,50 +3936,82 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.9361702127659575</v>
+        <v>0.8910891089108911</v>
       </c>
       <c r="E10">
-        <v>0.8073394495412844</v>
+        <v>0.8653846153846154</v>
       </c>
       <c r="F10">
-        <v>0.8669950738916257</v>
+        <v>0.878048780487805</v>
       </c>
       <c r="G10">
-        <v>0.9072164948453608</v>
+        <v>0.8858267716535434</v>
       </c>
       <c r="H10">
-        <v>0.7692307692307693</v>
+        <v>0.7863247863247863</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
+          <t>Qiime2</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Rottnest</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D11">
+        <v>0.9361702127659575</v>
+      </c>
+      <c r="E11">
+        <v>0.8073394495412844</v>
+      </c>
+      <c r="F11">
+        <v>0.8669950738916257</v>
+      </c>
+      <c r="G11">
+        <v>0.9072164948453608</v>
+      </c>
+      <c r="H11">
+        <v>0.7692307692307693</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
           <t>VSEARCH</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="B12" t="inlineStr">
         <is>
           <t>Rottnest</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>CO1</t>
         </is>
       </c>
-      <c r="D11">
+      <c r="D12">
         <v>0</v>
       </c>
-      <c r="E11">
+      <c r="E12">
         <v>0</v>
       </c>
-      <c r="F11">
+      <c r="F12">
         <v>0</v>
       </c>
-      <c r="G11">
+      <c r="G12">
         <v>0</v>
       </c>
-      <c r="H11">
+      <c r="H12">
         <v>0.0170940170940171</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add a nicer table
</commit_message>
<xml_diff>
--- a/results/tables/All_F1_tables.xlsx
+++ b/results/tables/All_F1_tables.xlsx
@@ -1654,19 +1654,19 @@
         </is>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>0.01492537313432836</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>0.02777777777777778</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>0.05747126436781608</v>
       </c>
       <c r="H13">
-        <v>0.2828282828282828</v>
+        <v>0.2929292929292929</v>
       </c>
     </row>
   </sheetData>
@@ -2971,19 +2971,19 @@
         </is>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>0.3333333333333334</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="H13">
-        <v>0.07407407407407407</v>
+        <v>0.2592592592592592</v>
       </c>
     </row>
   </sheetData>
@@ -4288,19 +4288,19 @@
         </is>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>0.7352941176470589</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>0.2358490566037736</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>0.3571428571428571</v>
       </c>
       <c r="G13">
-        <v>0</v>
+        <v>0.5165289256198347</v>
       </c>
       <c r="H13">
-        <v>0.0170940170940171</v>
+        <v>0.2307692307692308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
This should be it! all final results included.
</commit_message>
<xml_diff>
--- a/results/tables/All_F1_tables.xlsx
+++ b/results/tables/All_F1_tables.xlsx
@@ -1494,19 +1494,19 @@
         </is>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>0.9722222222222222</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>0.660377358490566</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>0.8177570093457943</v>
       </c>
       <c r="H8">
-        <v>0.2828282828282828</v>
+        <v>0.6363636363636364</v>
       </c>
     </row>
     <row r="9">
@@ -1526,19 +1526,19 @@
         </is>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>0.9830508474576272</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.8285714285714286</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>0.8992248062015504</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>0.9477124183006537</v>
       </c>
       <c r="H9">
-        <v>0.2828282828282828</v>
+        <v>0.8686868686868687</v>
       </c>
     </row>
     <row r="10">
@@ -2811,19 +2811,19 @@
         </is>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.44</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>0.7971014492753624</v>
       </c>
       <c r="H8">
-        <v>0.07407407407407407</v>
+        <v>0.4814814814814815</v>
       </c>
     </row>
     <row r="9">
@@ -2843,19 +2843,19 @@
         </is>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.92</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>0.9583333333333334</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>0.9829059829059831</v>
       </c>
       <c r="H9">
-        <v>0.07407407407407407</v>
+        <v>0.9259259259259259</v>
       </c>
     </row>
     <row r="10">
@@ -3049,7 +3049,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -3081,7 +3081,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -3113,7 +3113,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -3145,7 +3145,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -3177,7 +3177,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -3209,7 +3209,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -3241,7 +3241,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -3273,7 +3273,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -3305,7 +3305,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -3337,7 +3337,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -3369,7 +3369,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -3401,7 +3401,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -3488,7 +3488,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -3520,7 +3520,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -3552,7 +3552,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -3584,7 +3584,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -3616,7 +3616,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -3648,7 +3648,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -3680,7 +3680,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -3712,7 +3712,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -3744,7 +3744,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -3776,7 +3776,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -3808,7 +3808,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -3840,7 +3840,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -3927,7 +3927,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -3959,7 +3959,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -3991,7 +3991,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -4023,7 +4023,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -4055,7 +4055,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -4087,7 +4087,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -4119,7 +4119,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -4128,19 +4128,19 @@
         </is>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>0.9830508474576272</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.5087719298245614</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>0.6705202312138728</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>0.8285714285714286</v>
       </c>
       <c r="H8">
-        <v>0.0170940170940171</v>
+        <v>0.5128205128205128</v>
       </c>
     </row>
     <row r="9">
@@ -4151,7 +4151,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -4160,19 +4160,19 @@
         </is>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>0.979381443298969</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.8407079646017699</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>0.9047619047619049</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>0.9481037924151696</v>
       </c>
       <c r="H9">
-        <v>0.0170940170940171</v>
+        <v>0.8290598290598291</v>
       </c>
     </row>
     <row r="10">
@@ -4183,7 +4183,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -4215,7 +4215,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -4247,7 +4247,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -4279,7 +4279,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Rottnest</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">

</xml_diff>

<commit_message>
Added DADA2. Added a better table. I think DADA2 currently not finished.
</commit_message>
<xml_diff>
--- a/results/tables/All_F1_tables.xlsx
+++ b/results/tables/All_F1_tables.xlsx
@@ -359,7 +359,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -506,7 +506,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kraken2_0.0</t>
+          <t>DADA2_Species</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -520,25 +520,25 @@
         </is>
       </c>
       <c r="D5">
-        <v>0.7941176470588235</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0.6352941176470588</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0.7058823529411765</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>0.7563025210084033</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>0.5454545454545454</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kraken2_0.05</t>
+          <t>DADA2_Taxonomy</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -552,25 +552,25 @@
         </is>
       </c>
       <c r="D6">
-        <v>0.8793103448275862</v>
+        <v>0.3617021276595745</v>
       </c>
       <c r="E6">
-        <v>0.5543478260869565</v>
+        <v>0.2463768115942029</v>
       </c>
       <c r="F6">
-        <v>0.6799999999999999</v>
+        <v>0.2931034482758621</v>
       </c>
       <c r="G6">
-        <v>0.787037037037037</v>
+        <v>0.3307392996108949</v>
       </c>
       <c r="H6">
-        <v>0.5151515151515151</v>
+        <v>0.1717171717171717</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Kraken2_0.1</t>
+          <t>Kraken2_0.0</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -584,25 +584,25 @@
         </is>
       </c>
       <c r="D7">
-        <v>0.9038461538461539</v>
+        <v>0.7941176470588235</v>
       </c>
       <c r="E7">
-        <v>0.5</v>
+        <v>0.6352941176470588</v>
       </c>
       <c r="F7">
-        <v>0.6438356164383562</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="G7">
-        <v>0.7781456953642384</v>
+        <v>0.7563025210084033</v>
       </c>
       <c r="H7">
-        <v>0.4747474747474748</v>
+        <v>0.5454545454545454</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MMSeqs2_100</t>
+          <t>Kraken2_0.05</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -616,25 +616,25 @@
         </is>
       </c>
       <c r="D8">
-        <v>0.9076923076923077</v>
+        <v>0.8793103448275862</v>
       </c>
       <c r="E8">
-        <v>0.6344086021505376</v>
+        <v>0.5543478260869565</v>
       </c>
       <c r="F8">
-        <v>0.7468354430379748</v>
+        <v>0.6799999999999999</v>
       </c>
       <c r="G8">
-        <v>0.8356940509915014</v>
+        <v>0.787037037037037</v>
       </c>
       <c r="H8">
-        <v>0.5959595959595959</v>
+        <v>0.5151515151515151</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MMSeqs2_97</t>
+          <t>Kraken2_0.1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -648,25 +648,25 @@
         </is>
       </c>
       <c r="D9">
-        <v>0.8194444444444444</v>
+        <v>0.9038461538461539</v>
       </c>
       <c r="E9">
-        <v>0.686046511627907</v>
+        <v>0.5</v>
       </c>
       <c r="F9">
-        <v>0.7468354430379746</v>
+        <v>0.6438356164383562</v>
       </c>
       <c r="G9">
-        <v>0.7887700534759359</v>
+        <v>0.7781456953642384</v>
       </c>
       <c r="H9">
-        <v>0.5959595959595959</v>
+        <v>0.4747474747474748</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Metabuli</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -680,25 +680,25 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.7808219178082192</v>
+        <v>0.9076923076923077</v>
       </c>
       <c r="E10">
-        <v>0.6867469879518072</v>
+        <v>0.6344086021505376</v>
       </c>
       <c r="F10">
-        <v>0.7307692307692306</v>
+        <v>0.7468354430379748</v>
       </c>
       <c r="G10">
-        <v>0.76</v>
+        <v>0.8356940509915014</v>
       </c>
       <c r="H10">
-        <v>0.5757575757575758</v>
+        <v>0.5959595959595959</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -712,25 +712,25 @@
         </is>
       </c>
       <c r="D11">
-        <v>0.6721311475409836</v>
+        <v>0.8194444444444444</v>
       </c>
       <c r="E11">
-        <v>0.5189873417721519</v>
+        <v>0.686046511627907</v>
       </c>
       <c r="F11">
-        <v>0.5857142857142856</v>
+        <v>0.7468354430379746</v>
       </c>
       <c r="G11">
-        <v>0.6346749226006192</v>
+        <v>0.7887700534759359</v>
       </c>
       <c r="H11">
-        <v>0.4141414141414141</v>
+        <v>0.5959595959595959</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Qiime2</t>
+          <t>Metabuli</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -744,50 +744,114 @@
         </is>
       </c>
       <c r="D12">
-        <v>0.5686274509803921</v>
+        <v>0.7808219178082192</v>
       </c>
       <c r="E12">
-        <v>0.3766233766233766</v>
+        <v>0.6867469879518072</v>
       </c>
       <c r="F12">
-        <v>0.453125</v>
+        <v>0.7307692307692306</v>
       </c>
       <c r="G12">
-        <v>0.5160142348754448</v>
+        <v>0.76</v>
       </c>
       <c r="H12">
-        <v>0.2929292929292929</v>
+        <v>0.5757575757575758</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>Mothur</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>100 Australian species</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D13">
+        <v>0.6721311475409836</v>
+      </c>
+      <c r="E13">
+        <v>0.5189873417721519</v>
+      </c>
+      <c r="F13">
+        <v>0.5857142857142856</v>
+      </c>
+      <c r="G13">
+        <v>0.6346749226006192</v>
+      </c>
+      <c r="H13">
+        <v>0.4141414141414141</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Qiime2</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>100 Australian species</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D14">
+        <v>0.5686274509803921</v>
+      </c>
+      <c r="E14">
+        <v>0.3766233766233766</v>
+      </c>
+      <c r="F14">
+        <v>0.453125</v>
+      </c>
+      <c r="G14">
+        <v>0.5160142348754448</v>
+      </c>
+      <c r="H14">
+        <v>0.2929292929292929</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>VSEARCH</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>100 Australian species</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>12S</t>
         </is>
       </c>
-      <c r="D13">
+      <c r="D15">
         <v>0.7272727272727273</v>
       </c>
-      <c r="E13">
+      <c r="E15">
         <v>0.4761904761904762</v>
       </c>
-      <c r="F13">
+      <c r="F15">
         <v>0.5755395683453238</v>
       </c>
-      <c r="G13">
+      <c r="G15">
         <v>0.6578947368421053</v>
       </c>
-      <c r="H13">
+      <c r="H15">
         <v>0.404040404040404</v>
       </c>
     </row>
@@ -798,7 +862,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -945,7 +1009,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kraken2_0.0</t>
+          <t>DADA2_Species</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -959,25 +1023,25 @@
         </is>
       </c>
       <c r="D5">
-        <v>0.7761194029850746</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0.6190476190476191</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0.6887417218543046</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>0.7386363636363638</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>0.5252525252525253</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kraken2_0.05</t>
+          <t>DADA2_Taxonomy</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -991,25 +1055,25 @@
         </is>
       </c>
       <c r="D6">
-        <v>0.7868852459016393</v>
+        <v>0.3650793650793651</v>
       </c>
       <c r="E6">
-        <v>0.5581395348837209</v>
+        <v>0.3898305084745763</v>
       </c>
       <c r="F6">
-        <v>0.6530612244897959</v>
+        <v>0.3770491803278688</v>
       </c>
       <c r="G6">
-        <v>0.7272727272727272</v>
+        <v>0.3697749196141479</v>
       </c>
       <c r="H6">
-        <v>0.4848484848484849</v>
+        <v>0.2323232323232323</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Kraken2_0.1</t>
+          <t>Kraken2_0.0</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1023,25 +1087,25 @@
         </is>
       </c>
       <c r="D7">
-        <v>0.8181818181818182</v>
+        <v>0.7761194029850746</v>
       </c>
       <c r="E7">
-        <v>0.5056179775280899</v>
+        <v>0.6190476190476191</v>
       </c>
       <c r="F7">
-        <v>0.6250000000000001</v>
+        <v>0.6887417218543046</v>
       </c>
       <c r="G7">
-        <v>0.7281553398058251</v>
+        <v>0.7386363636363638</v>
       </c>
       <c r="H7">
-        <v>0.4545454545454545</v>
+        <v>0.5252525252525253</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MMSeqs2_100</t>
+          <t>Kraken2_0.05</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1055,25 +1119,25 @@
         </is>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0.7868852459016393</v>
       </c>
       <c r="E8">
-        <v>0.5151515151515151</v>
+        <v>0.5581395348837209</v>
       </c>
       <c r="F8">
-        <v>0.6799999999999999</v>
+        <v>0.6530612244897959</v>
       </c>
       <c r="G8">
-        <v>0.8415841584158416</v>
+        <v>0.7272727272727272</v>
       </c>
       <c r="H8">
-        <v>0.5151515151515151</v>
+        <v>0.4848484848484849</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MMSeqs2_97</t>
+          <t>Kraken2_0.1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1087,25 +1151,25 @@
         </is>
       </c>
       <c r="D9">
-        <v>0.9230769230769231</v>
+        <v>0.8181818181818182</v>
       </c>
       <c r="E9">
-        <v>0.6382978723404256</v>
+        <v>0.5056179775280899</v>
       </c>
       <c r="F9">
-        <v>0.7547169811320755</v>
+        <v>0.6250000000000001</v>
       </c>
       <c r="G9">
-        <v>0.8474576271186441</v>
+        <v>0.7281553398058251</v>
       </c>
       <c r="H9">
-        <v>0.6060606060606061</v>
+        <v>0.4545454545454545</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Metabuli</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1119,25 +1183,25 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.7236842105263158</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>0.7051282051282052</v>
+        <v>0.5151515151515151</v>
       </c>
       <c r="F10">
-        <v>0.7142857142857143</v>
+        <v>0.6799999999999999</v>
       </c>
       <c r="G10">
-        <v>0.7198952879581152</v>
+        <v>0.8415841584158416</v>
       </c>
       <c r="H10">
-        <v>0.5555555555555556</v>
+        <v>0.5151515151515151</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1151,25 +1215,25 @@
         </is>
       </c>
       <c r="D11">
-        <v>0.78125</v>
+        <v>0.9230769230769231</v>
       </c>
       <c r="E11">
-        <v>0.5882352941176471</v>
+        <v>0.6382978723404256</v>
       </c>
       <c r="F11">
-        <v>0.6711409395973155</v>
+        <v>0.7547169811320755</v>
       </c>
       <c r="G11">
-        <v>0.7331378299120235</v>
+        <v>0.8474576271186441</v>
       </c>
       <c r="H11">
-        <v>0.5050505050505051</v>
+        <v>0.6060606060606061</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Qiime2</t>
+          <t>Metabuli</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1183,50 +1247,114 @@
         </is>
       </c>
       <c r="D12">
-        <v>0.7368421052631579</v>
+        <v>0.7236842105263158</v>
       </c>
       <c r="E12">
-        <v>0.5</v>
+        <v>0.7051282051282052</v>
       </c>
       <c r="F12">
-        <v>0.5957446808510638</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="G12">
-        <v>0.673076923076923</v>
+        <v>0.7198952879581152</v>
       </c>
       <c r="H12">
-        <v>0.4242424242424243</v>
+        <v>0.5555555555555556</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>Mothur</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>100 Australian species</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D13">
+        <v>0.78125</v>
+      </c>
+      <c r="E13">
+        <v>0.5882352941176471</v>
+      </c>
+      <c r="F13">
+        <v>0.6711409395973155</v>
+      </c>
+      <c r="G13">
+        <v>0.7331378299120235</v>
+      </c>
+      <c r="H13">
+        <v>0.5050505050505051</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Qiime2</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>100 Australian species</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D14">
+        <v>0.7368421052631579</v>
+      </c>
+      <c r="E14">
+        <v>0.5</v>
+      </c>
+      <c r="F14">
+        <v>0.5957446808510638</v>
+      </c>
+      <c r="G14">
+        <v>0.673076923076923</v>
+      </c>
+      <c r="H14">
+        <v>0.4242424242424243</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>VSEARCH</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>100 Australian species</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>16S</t>
         </is>
       </c>
-      <c r="D13">
+      <c r="D15">
         <v>0.7818181818181819</v>
       </c>
-      <c r="E13">
+      <c r="E15">
         <v>0.4942528735632184</v>
       </c>
-      <c r="F13">
+      <c r="F15">
         <v>0.6056338028169014</v>
       </c>
-      <c r="G13">
+      <c r="G15">
         <v>0.7003257328990228</v>
       </c>
-      <c r="H13">
+      <c r="H15">
         <v>0.4343434343434344</v>
       </c>
     </row>
@@ -1237,7 +1365,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1384,7 +1512,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kraken2_0.0</t>
+          <t>DADA2_Species</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1398,25 +1526,25 @@
         </is>
       </c>
       <c r="D5">
-        <v>0.96</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0.6956521739130435</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0.8067226890756302</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>0.8921933085501859</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>0.7676767676767676</v>
+        <v>0.2828282828282828</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kraken2_0.05</t>
+          <t>DADA2_Taxonomy</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1430,25 +1558,25 @@
         </is>
       </c>
       <c r="D6">
-        <v>0.9743589743589743</v>
+        <v>0.2682926829268293</v>
       </c>
       <c r="E6">
-        <v>0.5428571428571428</v>
+        <v>0.2682926829268293</v>
       </c>
       <c r="F6">
-        <v>0.6972477064220183</v>
+        <v>0.2682926829268293</v>
       </c>
       <c r="G6">
-        <v>0.8407079646017698</v>
+        <v>0.2682926829268293</v>
       </c>
       <c r="H6">
-        <v>0.6666666666666666</v>
+        <v>0.3939393939393939</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Kraken2_0.1</t>
+          <t>Kraken2_0.0</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1462,25 +1590,25 @@
         </is>
       </c>
       <c r="D7">
-        <v>0.9642857142857143</v>
+        <v>0.96</v>
       </c>
       <c r="E7">
-        <v>0.3857142857142857</v>
+        <v>0.6956521739130435</v>
       </c>
       <c r="F7">
-        <v>0.5510204081632653</v>
+        <v>0.8067226890756302</v>
       </c>
       <c r="G7">
-        <v>0.7417582417582418</v>
+        <v>0.8921933085501859</v>
       </c>
       <c r="H7">
-        <v>0.5555555555555556</v>
+        <v>0.7676767676767676</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MMSeqs2_100</t>
+          <t>Kraken2_0.05</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1494,25 +1622,25 @@
         </is>
       </c>
       <c r="D8">
-        <v>0.9722222222222222</v>
+        <v>0.9743589743589743</v>
       </c>
       <c r="E8">
-        <v>0.5</v>
+        <v>0.5428571428571428</v>
       </c>
       <c r="F8">
-        <v>0.660377358490566</v>
+        <v>0.6972477064220183</v>
       </c>
       <c r="G8">
-        <v>0.8177570093457943</v>
+        <v>0.8407079646017698</v>
       </c>
       <c r="H8">
-        <v>0.6363636363636364</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MMSeqs2_97</t>
+          <t>Kraken2_0.1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1526,25 +1654,25 @@
         </is>
       </c>
       <c r="D9">
-        <v>0.9830508474576272</v>
+        <v>0.9642857142857143</v>
       </c>
       <c r="E9">
-        <v>0.8285714285714286</v>
+        <v>0.3857142857142857</v>
       </c>
       <c r="F9">
-        <v>0.8992248062015504</v>
+        <v>0.5510204081632653</v>
       </c>
       <c r="G9">
-        <v>0.9477124183006537</v>
+        <v>0.7417582417582418</v>
       </c>
       <c r="H9">
-        <v>0.8686868686868687</v>
+        <v>0.5555555555555556</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Metabuli</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1558,25 +1686,25 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.868421052631579</v>
+        <v>0.9722222222222222</v>
       </c>
       <c r="E10">
-        <v>0.4459459459459459</v>
+        <v>0.5</v>
       </c>
       <c r="F10">
-        <v>0.5892857142857143</v>
+        <v>0.660377358490566</v>
       </c>
       <c r="G10">
-        <v>0.7300884955752212</v>
+        <v>0.8177570093457943</v>
       </c>
       <c r="H10">
-        <v>0.5353535353535354</v>
+        <v>0.6363636363636364</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1590,25 +1718,25 @@
         </is>
       </c>
       <c r="D11">
-        <v>0.8666666666666667</v>
+        <v>0.9830508474576272</v>
       </c>
       <c r="E11">
-        <v>0.8253968253968254</v>
+        <v>0.8285714285714286</v>
       </c>
       <c r="F11">
-        <v>0.8455284552845528</v>
+        <v>0.8992248062015504</v>
       </c>
       <c r="G11">
-        <v>0.8580858085808584</v>
+        <v>0.9477124183006537</v>
       </c>
       <c r="H11">
-        <v>0.8080808080808081</v>
+        <v>0.8686868686868687</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Qiime2</t>
+          <t>Metabuli</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1622,50 +1750,114 @@
         </is>
       </c>
       <c r="D12">
-        <v>0.8909090909090909</v>
+        <v>0.868421052631579</v>
       </c>
       <c r="E12">
-        <v>0.5833333333333334</v>
+        <v>0.4459459459459459</v>
       </c>
       <c r="F12">
-        <v>0.7050359712230215</v>
+        <v>0.5892857142857143</v>
       </c>
       <c r="G12">
-        <v>0.8059210526315789</v>
+        <v>0.7300884955752212</v>
       </c>
       <c r="H12">
-        <v>0.5858585858585859</v>
+        <v>0.5353535353535354</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>Mothur</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>100 Australian species</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D13">
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="E13">
+        <v>0.8253968253968254</v>
+      </c>
+      <c r="F13">
+        <v>0.8455284552845528</v>
+      </c>
+      <c r="G13">
+        <v>0.8580858085808584</v>
+      </c>
+      <c r="H13">
+        <v>0.8080808080808081</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Qiime2</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>100 Australian species</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D14">
+        <v>0.8909090909090909</v>
+      </c>
+      <c r="E14">
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="F14">
+        <v>0.7050359712230215</v>
+      </c>
+      <c r="G14">
+        <v>0.8059210526315789</v>
+      </c>
+      <c r="H14">
+        <v>0.5858585858585859</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>VSEARCH</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>100 Australian species</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>CO1</t>
         </is>
       </c>
-      <c r="D13">
+      <c r="D15">
         <v>0.2</v>
       </c>
-      <c r="E13">
+      <c r="E15">
         <v>0.01492537313432836</v>
       </c>
-      <c r="F13">
+      <c r="F15">
         <v>0.02777777777777778</v>
       </c>
-      <c r="G13">
+      <c r="G15">
         <v>0.05747126436781608</v>
       </c>
-      <c r="H13">
+      <c r="H15">
         <v>0.2929292929292929</v>
       </c>
     </row>
@@ -1676,7 +1868,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1823,7 +2015,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kraken2_0.0</t>
+          <t>DADA2_Species</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -1837,25 +2029,25 @@
         </is>
       </c>
       <c r="D5">
-        <v>0.8888888888888888</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0.8421052631578948</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>0.8695652173913044</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>0.75</v>
+        <v>0.08333333333333333</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kraken2_0.05</t>
+          <t>DADA2_Taxonomy</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1869,25 +2061,25 @@
         </is>
       </c>
       <c r="D6">
-        <v>0.9285714285714286</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="E6">
-        <v>0.6190476190476191</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="F6">
-        <v>0.742857142857143</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="G6">
-        <v>0.8441558441558441</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="H6">
-        <v>0.625</v>
+        <v>0.1666666666666667</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Kraken2_0.1</t>
+          <t>Kraken2_0.0</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1901,25 +2093,25 @@
         </is>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="E7">
-        <v>0.4090909090909091</v>
+        <v>0.8</v>
       </c>
       <c r="F7">
-        <v>0.5806451612903226</v>
+        <v>0.8421052631578948</v>
       </c>
       <c r="G7">
-        <v>0.7758620689655171</v>
+        <v>0.8695652173913044</v>
       </c>
       <c r="H7">
-        <v>0.4583333333333333</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MMSeqs2_100</t>
+          <t>Kraken2_0.05</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1933,25 +2125,25 @@
         </is>
       </c>
       <c r="D8">
-        <v>0.9333333333333333</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="E8">
-        <v>0.6666666666666666</v>
+        <v>0.6190476190476191</v>
       </c>
       <c r="F8">
-        <v>0.7777777777777778</v>
+        <v>0.742857142857143</v>
       </c>
       <c r="G8">
-        <v>0.8641975308641976</v>
+        <v>0.8441558441558441</v>
       </c>
       <c r="H8">
-        <v>0.6666666666666666</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MMSeqs2_97</t>
+          <t>Kraken2_0.1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1965,25 +2157,25 @@
         </is>
       </c>
       <c r="D9">
-        <v>0.9411764705882353</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>0.7619047619047619</v>
+        <v>0.4090909090909091</v>
       </c>
       <c r="F9">
-        <v>0.8421052631578947</v>
+        <v>0.5806451612903226</v>
       </c>
       <c r="G9">
-        <v>0.898876404494382</v>
+        <v>0.7758620689655171</v>
       </c>
       <c r="H9">
-        <v>0.75</v>
+        <v>0.4583333333333333</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Metabuli</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1997,25 +2189,25 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.8947368421052632</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="E10">
-        <v>0.85</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F10">
-        <v>0.8717948717948718</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="G10">
-        <v>0.8854166666666667</v>
+        <v>0.8641975308641976</v>
       </c>
       <c r="H10">
-        <v>0.7916666666666666</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -2029,25 +2221,25 @@
         </is>
       </c>
       <c r="D11">
-        <v>0.6923076923076923</v>
+        <v>0.9411764705882353</v>
       </c>
       <c r="E11">
-        <v>0.5</v>
+        <v>0.7619047619047619</v>
       </c>
       <c r="F11">
-        <v>0.5806451612903226</v>
+        <v>0.8421052631578947</v>
       </c>
       <c r="G11">
-        <v>0.6428571428571428</v>
+        <v>0.898876404494382</v>
       </c>
       <c r="H11">
-        <v>0.4583333333333333</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Qiime2</t>
+          <t>Metabuli</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -2061,50 +2253,114 @@
         </is>
       </c>
       <c r="D12">
-        <v>0.8888888888888888</v>
+        <v>0.8947368421052632</v>
       </c>
       <c r="E12">
-        <v>0.3478260869565217</v>
+        <v>0.85</v>
       </c>
       <c r="F12">
-        <v>0.5</v>
+        <v>0.8717948717948718</v>
       </c>
       <c r="G12">
-        <v>0.6779661016949152</v>
+        <v>0.8854166666666667</v>
       </c>
       <c r="H12">
-        <v>0.3333333333333333</v>
+        <v>0.7916666666666666</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>Mothur</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Lutjanidae</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D13">
+        <v>0.6923076923076923</v>
+      </c>
+      <c r="E13">
+        <v>0.5</v>
+      </c>
+      <c r="F13">
+        <v>0.5806451612903226</v>
+      </c>
+      <c r="G13">
+        <v>0.6428571428571428</v>
+      </c>
+      <c r="H13">
+        <v>0.4583333333333333</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Qiime2</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Lutjanidae</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D14">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="E14">
+        <v>0.3478260869565217</v>
+      </c>
+      <c r="F14">
+        <v>0.5</v>
+      </c>
+      <c r="G14">
+        <v>0.6779661016949152</v>
+      </c>
+      <c r="H14">
+        <v>0.3333333333333333</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>VSEARCH</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>Lutjanidae</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>12S</t>
         </is>
       </c>
-      <c r="D13">
+      <c r="D15">
         <v>0.6666666666666666</v>
       </c>
-      <c r="E13">
+      <c r="E15">
         <v>0.4444444444444444</v>
       </c>
-      <c r="F13">
+      <c r="F15">
         <v>0.5333333333333333</v>
       </c>
-      <c r="G13">
+      <c r="G15">
         <v>0.606060606060606</v>
       </c>
-      <c r="H13">
+      <c r="H15">
         <v>0.4166666666666667</v>
       </c>
     </row>
@@ -2115,7 +2371,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2262,7 +2518,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kraken2_0.0</t>
+          <t>DADA2_Species</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -2276,25 +2532,25 @@
         </is>
       </c>
       <c r="D5">
-        <v>0.4545454545454545</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0.7142857142857143</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0.5555555555555556</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>0.4901960784313725</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>0.4074074074074074</v>
+        <v>0.03703703703703703</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kraken2_0.05</t>
+          <t>DADA2_Taxonomy</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -2308,25 +2564,25 @@
         </is>
       </c>
       <c r="D6">
-        <v>0.5625</v>
+        <v>0.4615384615384616</v>
       </c>
       <c r="E6">
-        <v>0.4736842105263158</v>
+        <v>0.3157894736842105</v>
       </c>
       <c r="F6">
-        <v>0.5142857142857142</v>
+        <v>0.3749999999999999</v>
       </c>
       <c r="G6">
-        <v>0.5421686746987953</v>
+        <v>0.4225352112676056</v>
       </c>
       <c r="H6">
-        <v>0.3703703703703703</v>
+        <v>0.2592592592592592</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Kraken2_0.1</t>
+          <t>Kraken2_0.0</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2340,25 +2596,25 @@
         </is>
       </c>
       <c r="D7">
-        <v>0.6666666666666666</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="E7">
-        <v>0.3636363636363636</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="F7">
-        <v>0.4705882352941177</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="G7">
-        <v>0.5714285714285715</v>
+        <v>0.4901960784313725</v>
       </c>
       <c r="H7">
-        <v>0.3333333333333333</v>
+        <v>0.4074074074074074</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MMSeqs2_100</t>
+          <t>Kraken2_0.05</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2372,16 +2628,16 @@
         </is>
       </c>
       <c r="D8">
-        <v>0.9</v>
+        <v>0.5625</v>
       </c>
       <c r="E8">
-        <v>0.36</v>
+        <v>0.4736842105263158</v>
       </c>
       <c r="F8">
-        <v>0.5142857142857143</v>
+        <v>0.5142857142857142</v>
       </c>
       <c r="G8">
-        <v>0.6923076923076923</v>
+        <v>0.5421686746987953</v>
       </c>
       <c r="H8">
         <v>0.3703703703703703</v>
@@ -2390,7 +2646,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MMSeqs2_97</t>
+          <t>Kraken2_0.1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2404,25 +2660,25 @@
         </is>
       </c>
       <c r="D9">
-        <v>0.7142857142857143</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E9">
-        <v>0.4545454545454545</v>
+        <v>0.3636363636363636</v>
       </c>
       <c r="F9">
-        <v>0.5555555555555556</v>
+        <v>0.4705882352941177</v>
       </c>
       <c r="G9">
-        <v>0.6410256410256411</v>
+        <v>0.5714285714285715</v>
       </c>
       <c r="H9">
-        <v>0.4074074074074074</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Metabuli</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2436,25 +2692,25 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.4583333333333333</v>
+        <v>0.9</v>
       </c>
       <c r="E10">
-        <v>0.8461538461538461</v>
+        <v>0.36</v>
       </c>
       <c r="F10">
-        <v>0.5945945945945945</v>
+        <v>0.5142857142857143</v>
       </c>
       <c r="G10">
-        <v>0.5045871559633027</v>
+        <v>0.6923076923076923</v>
       </c>
       <c r="H10">
-        <v>0.4444444444444444</v>
+        <v>0.3703703703703703</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -2468,25 +2724,25 @@
         </is>
       </c>
       <c r="D11">
-        <v>0.5</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="E11">
-        <v>0.3684210526315789</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="F11">
-        <v>0.4242424242424242</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="G11">
-        <v>0.4666666666666667</v>
+        <v>0.6410256410256411</v>
       </c>
       <c r="H11">
-        <v>0.2962962962962963</v>
+        <v>0.4074074074074074</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Qiime2</t>
+          <t>Metabuli</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -2500,50 +2756,114 @@
         </is>
       </c>
       <c r="D12">
-        <v>0.5</v>
+        <v>0.4583333333333333</v>
       </c>
       <c r="E12">
-        <v>0.3</v>
+        <v>0.8461538461538461</v>
       </c>
       <c r="F12">
-        <v>0.3749999999999999</v>
+        <v>0.5945945945945945</v>
       </c>
       <c r="G12">
-        <v>0.4411764705882353</v>
+        <v>0.5045871559633027</v>
       </c>
       <c r="H12">
-        <v>0.2592592592592592</v>
+        <v>0.4444444444444444</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>Mothur</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Lutjanidae</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D13">
+        <v>0.5</v>
+      </c>
+      <c r="E13">
+        <v>0.3684210526315789</v>
+      </c>
+      <c r="F13">
+        <v>0.4242424242424242</v>
+      </c>
+      <c r="G13">
+        <v>0.4666666666666667</v>
+      </c>
+      <c r="H13">
+        <v>0.2962962962962963</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Qiime2</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Lutjanidae</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D14">
+        <v>0.5</v>
+      </c>
+      <c r="E14">
+        <v>0.3</v>
+      </c>
+      <c r="F14">
+        <v>0.3749999999999999</v>
+      </c>
+      <c r="G14">
+        <v>0.4411764705882353</v>
+      </c>
+      <c r="H14">
+        <v>0.2592592592592592</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>VSEARCH</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>Lutjanidae</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>16S</t>
         </is>
       </c>
-      <c r="D13">
+      <c r="D15">
         <v>0.4615384615384616</v>
       </c>
-      <c r="E13">
+      <c r="E15">
         <v>0.3157894736842105</v>
       </c>
-      <c r="F13">
+      <c r="F15">
         <v>0.3749999999999999</v>
       </c>
-      <c r="G13">
+      <c r="G15">
         <v>0.4225352112676056</v>
       </c>
-      <c r="H13">
+      <c r="H15">
         <v>0.2592592592592592</v>
       </c>
     </row>
@@ -2554,7 +2874,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2701,7 +3021,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kraken2_0.0</t>
+          <t>DADA2_Species</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -2715,25 +3035,25 @@
         </is>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0.76</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0.8636363636363636</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>0.9405940594059405</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>0.7777777777777778</v>
+        <v>0.07407407407407407</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kraken2_0.05</t>
+          <t>DADA2_Taxonomy</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -2747,16 +3067,16 @@
         </is>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="E6">
-        <v>0.44</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="F6">
         <v>0.6111111111111112</v>
       </c>
       <c r="G6">
-        <v>0.7971014492753624</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="H6">
         <v>0.4814814814814815</v>
@@ -2765,7 +3085,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Kraken2_0.1</t>
+          <t>Kraken2_0.0</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -2782,22 +3102,22 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>0.24</v>
+        <v>0.76</v>
       </c>
       <c r="F7">
-        <v>0.3870967741935484</v>
+        <v>0.8636363636363636</v>
       </c>
       <c r="G7">
-        <v>0.6122448979591837</v>
+        <v>0.9405940594059405</v>
       </c>
       <c r="H7">
-        <v>0.2962962962962963</v>
+        <v>0.7777777777777778</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MMSeqs2_100</t>
+          <t>Kraken2_0.05</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -2829,7 +3149,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MMSeqs2_97</t>
+          <t>Kraken2_0.1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -2846,22 +3166,22 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <v>0.92</v>
+        <v>0.24</v>
       </c>
       <c r="F9">
-        <v>0.9583333333333334</v>
+        <v>0.3870967741935484</v>
       </c>
       <c r="G9">
-        <v>0.9829059829059831</v>
+        <v>0.6122448979591837</v>
       </c>
       <c r="H9">
-        <v>0.9259259259259259</v>
+        <v>0.2962962962962963</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Metabuli</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -2875,25 +3195,25 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.9411764705882353</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>0.64</v>
+        <v>0.44</v>
       </c>
       <c r="F10">
-        <v>0.7619047619047621</v>
+        <v>0.6111111111111112</v>
       </c>
       <c r="G10">
-        <v>0.8602150537634409</v>
+        <v>0.7971014492753624</v>
       </c>
       <c r="H10">
-        <v>0.6296296296296297</v>
+        <v>0.4814814814814815</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -2907,16 +3227,16 @@
         </is>
       </c>
       <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
         <v>0.92</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
       </c>
       <c r="F11">
         <v>0.9583333333333334</v>
       </c>
       <c r="G11">
-        <v>0.934959349593496</v>
+        <v>0.9829059829059831</v>
       </c>
       <c r="H11">
         <v>0.9259259259259259</v>
@@ -2925,7 +3245,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Qiime2</t>
+          <t>Metabuli</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -2939,50 +3259,114 @@
         </is>
       </c>
       <c r="D12">
-        <v>0.92</v>
+        <v>0.9411764705882353</v>
       </c>
       <c r="E12">
-        <v>0.9583333333333334</v>
+        <v>0.64</v>
       </c>
       <c r="F12">
-        <v>0.9387755102040817</v>
+        <v>0.7619047619047621</v>
       </c>
       <c r="G12">
-        <v>0.9274193548387097</v>
+        <v>0.8602150537634409</v>
       </c>
       <c r="H12">
-        <v>0.8888888888888888</v>
+        <v>0.6296296296296297</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>Mothur</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Lutjanidae</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D13">
+        <v>0.92</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0.9583333333333334</v>
+      </c>
+      <c r="G13">
+        <v>0.934959349593496</v>
+      </c>
+      <c r="H13">
+        <v>0.9259259259259259</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Qiime2</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Lutjanidae</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D14">
+        <v>0.92</v>
+      </c>
+      <c r="E14">
+        <v>0.9583333333333334</v>
+      </c>
+      <c r="F14">
+        <v>0.9387755102040817</v>
+      </c>
+      <c r="G14">
+        <v>0.9274193548387097</v>
+      </c>
+      <c r="H14">
+        <v>0.8888888888888888</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>VSEARCH</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>Lutjanidae</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>CO1</t>
         </is>
       </c>
-      <c r="D13">
+      <c r="D15">
         <v>1</v>
       </c>
-      <c r="E13">
+      <c r="E15">
         <v>0.2</v>
       </c>
-      <c r="F13">
+      <c r="F15">
         <v>0.3333333333333334</v>
       </c>
-      <c r="G13">
+      <c r="G15">
         <v>0.5555555555555556</v>
       </c>
-      <c r="H13">
+      <c r="H15">
         <v>0.2592592592592592</v>
       </c>
     </row>
@@ -2993,7 +3377,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3140,7 +3524,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kraken2_0.0</t>
+          <t>DADA2_Species</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -3154,25 +3538,25 @@
         </is>
       </c>
       <c r="D5">
-        <v>0.8333333333333334</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0.6741573033707865</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0.7453416149068324</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>0.7957559681697614</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>0.5980392156862745</v>
+        <v>0.009803921568627451</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kraken2_0.05</t>
+          <t>DADA2_Taxonomy</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -3186,25 +3570,25 @@
         </is>
       </c>
       <c r="D6">
-        <v>0.8636363636363636</v>
+        <v>0.25</v>
       </c>
       <c r="E6">
-        <v>0.6195652173913043</v>
+        <v>0.1846153846153846</v>
       </c>
       <c r="F6">
-        <v>0.7215189873417721</v>
+        <v>0.2123893805309734</v>
       </c>
       <c r="G6">
-        <v>0.800561797752809</v>
+        <v>0.2334630350194553</v>
       </c>
       <c r="H6">
-        <v>0.5686274509803921</v>
+        <v>0.1274509803921569</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Kraken2_0.1</t>
+          <t>Kraken2_0.0</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -3218,25 +3602,25 @@
         </is>
       </c>
       <c r="D7">
-        <v>0.9137931034482759</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="E7">
-        <v>0.5520833333333334</v>
+        <v>0.6741573033707865</v>
       </c>
       <c r="F7">
-        <v>0.6883116883116883</v>
+        <v>0.7453416149068324</v>
       </c>
       <c r="G7">
-        <v>0.8079268292682928</v>
+        <v>0.7957559681697614</v>
       </c>
       <c r="H7">
-        <v>0.5294117647058824</v>
+        <v>0.5980392156862745</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MMSeqs2_100</t>
+          <t>Kraken2_0.05</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -3250,25 +3634,25 @@
         </is>
       </c>
       <c r="D8">
-        <v>0.9666666666666667</v>
+        <v>0.8636363636363636</v>
       </c>
       <c r="E8">
-        <v>0.5858585858585859</v>
+        <v>0.6195652173913043</v>
       </c>
       <c r="F8">
-        <v>0.729559748427673</v>
+        <v>0.7215189873417721</v>
       </c>
       <c r="G8">
-        <v>0.8554572271386429</v>
+        <v>0.800561797752809</v>
       </c>
       <c r="H8">
-        <v>0.5784313725490197</v>
+        <v>0.5686274509803921</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MMSeqs2_97</t>
+          <t>Kraken2_0.1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -3282,25 +3666,25 @@
         </is>
       </c>
       <c r="D9">
-        <v>0.9014084507042254</v>
+        <v>0.9137931034482759</v>
       </c>
       <c r="E9">
-        <v>0.6808510638297872</v>
+        <v>0.5520833333333334</v>
       </c>
       <c r="F9">
-        <v>0.7757575757575758</v>
+        <v>0.6883116883116883</v>
       </c>
       <c r="G9">
-        <v>0.8465608465608466</v>
+        <v>0.8079268292682928</v>
       </c>
       <c r="H9">
-        <v>0.6372549019607843</v>
+        <v>0.5294117647058824</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Metabuli</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -3314,25 +3698,25 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.8441558441558441</v>
+        <v>0.9666666666666667</v>
       </c>
       <c r="E10">
-        <v>0.7303370786516854</v>
+        <v>0.5858585858585859</v>
       </c>
       <c r="F10">
-        <v>0.7831325301204819</v>
+        <v>0.729559748427673</v>
       </c>
       <c r="G10">
-        <v>0.8186397984886651</v>
+        <v>0.8554572271386429</v>
       </c>
       <c r="H10">
-        <v>0.6470588235294118</v>
+        <v>0.5784313725490197</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -3346,25 +3730,25 @@
         </is>
       </c>
       <c r="D11">
-        <v>0.6666666666666666</v>
+        <v>0.9014084507042254</v>
       </c>
       <c r="E11">
-        <v>0.525</v>
+        <v>0.6808510638297872</v>
       </c>
       <c r="F11">
-        <v>0.5874125874125874</v>
+        <v>0.7757575757575758</v>
       </c>
       <c r="G11">
-        <v>0.6325301204819277</v>
+        <v>0.8465608465608466</v>
       </c>
       <c r="H11">
-        <v>0.4215686274509804</v>
+        <v>0.6372549019607843</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Qiime2</t>
+          <t>Metabuli</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -3378,50 +3762,114 @@
         </is>
       </c>
       <c r="D12">
-        <v>0.6458333333333334</v>
+        <v>0.8441558441558441</v>
       </c>
       <c r="E12">
-        <v>0.3690476190476191</v>
+        <v>0.7303370786516854</v>
       </c>
       <c r="F12">
-        <v>0.4696969696969697</v>
+        <v>0.7831325301204819</v>
       </c>
       <c r="G12">
-        <v>0.5615942028985508</v>
+        <v>0.8186397984886651</v>
       </c>
       <c r="H12">
-        <v>0.3137254901960784</v>
+        <v>0.6470588235294118</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>Mothur</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Wadjemup</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D13">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="E13">
+        <v>0.525</v>
+      </c>
+      <c r="F13">
+        <v>0.5874125874125874</v>
+      </c>
+      <c r="G13">
+        <v>0.6325301204819277</v>
+      </c>
+      <c r="H13">
+        <v>0.4215686274509804</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Qiime2</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Wadjemup</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>12S</t>
+        </is>
+      </c>
+      <c r="D14">
+        <v>0.6458333333333334</v>
+      </c>
+      <c r="E14">
+        <v>0.3690476190476191</v>
+      </c>
+      <c r="F14">
+        <v>0.4696969696969697</v>
+      </c>
+      <c r="G14">
+        <v>0.5615942028985508</v>
+      </c>
+      <c r="H14">
+        <v>0.3137254901960784</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>VSEARCH</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>Wadjemup</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>12S</t>
         </is>
       </c>
-      <c r="D13">
+      <c r="D15">
         <v>0.7647058823529411</v>
       </c>
-      <c r="E13">
+      <c r="E15">
         <v>0.611764705882353</v>
       </c>
-      <c r="F13">
+      <c r="F15">
         <v>0.6797385620915033</v>
       </c>
-      <c r="G13">
+      <c r="G15">
         <v>0.7282913165266106</v>
       </c>
-      <c r="H13">
+      <c r="H15">
         <v>0.5196078431372549</v>
       </c>
     </row>
@@ -3432,7 +3880,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3579,7 +4027,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kraken2_0.0</t>
+          <t>DADA2_Species</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -3593,25 +4041,25 @@
         </is>
       </c>
       <c r="D5">
-        <v>0.813953488372093</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0.7608695652173914</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0.7865168539325844</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>0.8027522935779817</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>0.6607142857142857</v>
+        <v>0.03571428571428571</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kraken2_0.05</t>
+          <t>DADA2_Taxonomy</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -3625,25 +4073,25 @@
         </is>
       </c>
       <c r="D6">
-        <v>0.8625</v>
+        <v>0.1492537313432836</v>
       </c>
       <c r="E6">
-        <v>0.711340206185567</v>
+        <v>0.196078431372549</v>
       </c>
       <c r="F6">
-        <v>0.7796610169491526</v>
+        <v>0.1694915254237288</v>
       </c>
       <c r="G6">
-        <v>0.8273381294964028</v>
+        <v>0.1567398119122257</v>
       </c>
       <c r="H6">
-        <v>0.6517857142857143</v>
+        <v>0.125</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Kraken2_0.1</t>
+          <t>Kraken2_0.0</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -3657,25 +4105,25 @@
         </is>
       </c>
       <c r="D7">
-        <v>0.8918918918918919</v>
+        <v>0.813953488372093</v>
       </c>
       <c r="E7">
-        <v>0.66</v>
+        <v>0.7608695652173914</v>
       </c>
       <c r="F7">
-        <v>0.7586206896551725</v>
+        <v>0.7865168539325844</v>
       </c>
       <c r="G7">
-        <v>0.8333333333333335</v>
+        <v>0.8027522935779817</v>
       </c>
       <c r="H7">
-        <v>0.625</v>
+        <v>0.6607142857142857</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MMSeqs2_100</t>
+          <t>Kraken2_0.05</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -3689,25 +4137,25 @@
         </is>
       </c>
       <c r="D8">
-        <v>0.9473684210526315</v>
+        <v>0.8625</v>
       </c>
       <c r="E8">
-        <v>0.5142857142857142</v>
+        <v>0.711340206185567</v>
       </c>
       <c r="F8">
-        <v>0.6666666666666666</v>
+        <v>0.7796610169491526</v>
       </c>
       <c r="G8">
-        <v>0.8108108108108107</v>
+        <v>0.8273381294964028</v>
       </c>
       <c r="H8">
-        <v>0.5178571428571429</v>
+        <v>0.6517857142857143</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MMSeqs2_97</t>
+          <t>Kraken2_0.1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -3721,25 +4169,25 @@
         </is>
       </c>
       <c r="D9">
-        <v>0.8961038961038961</v>
+        <v>0.8918918918918919</v>
       </c>
       <c r="E9">
-        <v>0.6899999999999999</v>
+        <v>0.66</v>
       </c>
       <c r="F9">
-        <v>0.7796610169491525</v>
+        <v>0.7586206896551725</v>
       </c>
       <c r="G9">
-        <v>0.8455882352941176</v>
+        <v>0.8333333333333335</v>
       </c>
       <c r="H9">
-        <v>0.6517857142857143</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Metabuli</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -3753,25 +4201,25 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.7727272727272727</v>
+        <v>0.9473684210526315</v>
       </c>
       <c r="E10">
-        <v>0.7727272727272727</v>
+        <v>0.5142857142857142</v>
       </c>
       <c r="F10">
-        <v>0.7727272727272727</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G10">
-        <v>0.7727272727272727</v>
+        <v>0.8108108108108107</v>
       </c>
       <c r="H10">
-        <v>0.6428571428571429</v>
+        <v>0.5178571428571429</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -3785,25 +4233,25 @@
         </is>
       </c>
       <c r="D11">
-        <v>0.7093023255813954</v>
+        <v>0.8961038961038961</v>
       </c>
       <c r="E11">
-        <v>0.7349397590361446</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F11">
-        <v>0.7218934911242604</v>
+        <v>0.7796610169491525</v>
       </c>
       <c r="G11">
-        <v>0.7142857142857143</v>
+        <v>0.8455882352941176</v>
       </c>
       <c r="H11">
-        <v>0.5803571428571429</v>
+        <v>0.6517857142857143</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Qiime2</t>
+          <t>Metabuli</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -3817,50 +4265,114 @@
         </is>
       </c>
       <c r="D12">
-        <v>0.7466666666666667</v>
+        <v>0.7727272727272727</v>
       </c>
       <c r="E12">
-        <v>0.6153846153846154</v>
+        <v>0.7727272727272727</v>
       </c>
       <c r="F12">
-        <v>0.674698795180723</v>
+        <v>0.7727272727272727</v>
       </c>
       <c r="G12">
-        <v>0.7161125319693096</v>
+        <v>0.7727272727272727</v>
       </c>
       <c r="H12">
-        <v>0.5178571428571429</v>
+        <v>0.6428571428571429</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>Mothur</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Wadjemup</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D13">
+        <v>0.7093023255813954</v>
+      </c>
+      <c r="E13">
+        <v>0.7349397590361446</v>
+      </c>
+      <c r="F13">
+        <v>0.7218934911242604</v>
+      </c>
+      <c r="G13">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="H13">
+        <v>0.5803571428571429</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Qiime2</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Wadjemup</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>16S</t>
+        </is>
+      </c>
+      <c r="D14">
+        <v>0.7466666666666667</v>
+      </c>
+      <c r="E14">
+        <v>0.6153846153846154</v>
+      </c>
+      <c r="F14">
+        <v>0.674698795180723</v>
+      </c>
+      <c r="G14">
+        <v>0.7161125319693096</v>
+      </c>
+      <c r="H14">
+        <v>0.5178571428571429</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>VSEARCH</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>Wadjemup</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>16S</t>
         </is>
       </c>
-      <c r="D13">
+      <c r="D15">
         <v>0.8717948717948718</v>
       </c>
-      <c r="E13">
+      <c r="E15">
         <v>0.6938775510204082</v>
       </c>
-      <c r="F13">
+      <c r="F15">
         <v>0.7727272727272728</v>
       </c>
-      <c r="G13">
+      <c r="G15">
         <v>0.8292682926829269</v>
       </c>
-      <c r="H13">
+      <c r="H15">
         <v>0.6428571428571429</v>
       </c>
     </row>
@@ -3871,7 +4383,7 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4018,7 +4530,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Kraken2_0.0</t>
+          <t>DADA2_Species</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -4032,25 +4544,25 @@
         </is>
       </c>
       <c r="D5">
-        <v>0.9880952380952381</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0.7280701754385965</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <v>0.8383838383838385</v>
+        <v>0</v>
       </c>
       <c r="G5">
-        <v>0.9222222222222223</v>
+        <v>0</v>
       </c>
       <c r="H5">
-        <v>0.7264957264957265</v>
+        <v>0.0170940170940171</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kraken2_0.05</t>
+          <t>DADA2_Taxonomy</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -4064,25 +4576,25 @@
         </is>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="E6">
-        <v>0.6173913043478261</v>
+        <v>0.4126984126984127</v>
       </c>
       <c r="F6">
-        <v>0.7634408602150538</v>
+        <v>0.3687943262411347</v>
       </c>
       <c r="G6">
-        <v>0.8897243107769424</v>
+        <v>0.3466666666666666</v>
       </c>
       <c r="H6">
-        <v>0.6239316239316239</v>
+        <v>0.2393162393162393</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Kraken2_0.1</t>
+          <t>Kraken2_0.0</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -4096,25 +4608,25 @@
         </is>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0.9880952380952381</v>
       </c>
       <c r="E7">
-        <v>0.5391304347826087</v>
+        <v>0.7280701754385965</v>
       </c>
       <c r="F7">
-        <v>0.7005649717514124</v>
+        <v>0.8383838383838385</v>
       </c>
       <c r="G7">
-        <v>0.8539944903581267</v>
+        <v>0.9222222222222223</v>
       </c>
       <c r="H7">
-        <v>0.5470085470085471</v>
+        <v>0.7264957264957265</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MMSeqs2_100</t>
+          <t>Kraken2_0.05</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -4128,25 +4640,25 @@
         </is>
       </c>
       <c r="D8">
-        <v>0.9830508474576272</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>0.5087719298245614</v>
+        <v>0.6173913043478261</v>
       </c>
       <c r="F8">
-        <v>0.6705202312138728</v>
+        <v>0.7634408602150538</v>
       </c>
       <c r="G8">
-        <v>0.8285714285714286</v>
+        <v>0.8897243107769424</v>
       </c>
       <c r="H8">
-        <v>0.5128205128205128</v>
+        <v>0.6239316239316239</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MMSeqs2_97</t>
+          <t>Kraken2_0.1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -4160,25 +4672,25 @@
         </is>
       </c>
       <c r="D9">
-        <v>0.979381443298969</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>0.8407079646017699</v>
+        <v>0.5391304347826087</v>
       </c>
       <c r="F9">
-        <v>0.9047619047619049</v>
+        <v>0.7005649717514124</v>
       </c>
       <c r="G9">
-        <v>0.9481037924151696</v>
+        <v>0.8539944903581267</v>
       </c>
       <c r="H9">
-        <v>0.8290598290598291</v>
+        <v>0.5470085470085471</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Metabuli</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -4192,25 +4704,25 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.927536231884058</v>
+        <v>0.9830508474576272</v>
       </c>
       <c r="E10">
-        <v>0.5765765765765766</v>
+        <v>0.5087719298245614</v>
       </c>
       <c r="F10">
-        <v>0.7111111111111111</v>
+        <v>0.6705202312138728</v>
       </c>
       <c r="G10">
-        <v>0.82687338501292</v>
+        <v>0.8285714285714286</v>
       </c>
       <c r="H10">
-        <v>0.5555555555555556</v>
+        <v>0.5128205128205128</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -4224,25 +4736,25 @@
         </is>
       </c>
       <c r="D11">
-        <v>0.8910891089108911</v>
+        <v>0.979381443298969</v>
       </c>
       <c r="E11">
-        <v>0.8653846153846154</v>
+        <v>0.8407079646017699</v>
       </c>
       <c r="F11">
-        <v>0.878048780487805</v>
+        <v>0.9047619047619049</v>
       </c>
       <c r="G11">
-        <v>0.8858267716535434</v>
+        <v>0.9481037924151696</v>
       </c>
       <c r="H11">
-        <v>0.7863247863247863</v>
+        <v>0.8290598290598291</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Qiime2</t>
+          <t>Metabuli</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -4256,50 +4768,114 @@
         </is>
       </c>
       <c r="D12">
-        <v>0.9361702127659575</v>
+        <v>0.927536231884058</v>
       </c>
       <c r="E12">
-        <v>0.8073394495412844</v>
+        <v>0.5765765765765766</v>
       </c>
       <c r="F12">
-        <v>0.8669950738916257</v>
+        <v>0.7111111111111111</v>
       </c>
       <c r="G12">
-        <v>0.9072164948453608</v>
+        <v>0.82687338501292</v>
       </c>
       <c r="H12">
-        <v>0.7692307692307693</v>
+        <v>0.5555555555555556</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>Mothur</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Wadjemup</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D13">
+        <v>0.8910891089108911</v>
+      </c>
+      <c r="E13">
+        <v>0.8653846153846154</v>
+      </c>
+      <c r="F13">
+        <v>0.878048780487805</v>
+      </c>
+      <c r="G13">
+        <v>0.8858267716535434</v>
+      </c>
+      <c r="H13">
+        <v>0.7863247863247863</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Qiime2</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Wadjemup</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>CO1</t>
+        </is>
+      </c>
+      <c r="D14">
+        <v>0.9361702127659575</v>
+      </c>
+      <c r="E14">
+        <v>0.8073394495412844</v>
+      </c>
+      <c r="F14">
+        <v>0.8669950738916257</v>
+      </c>
+      <c r="G14">
+        <v>0.9072164948453608</v>
+      </c>
+      <c r="H14">
+        <v>0.7692307692307693</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>VSEARCH</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>Wadjemup</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>CO1</t>
         </is>
       </c>
-      <c r="D13">
+      <c r="D15">
         <v>0.7352941176470589</v>
       </c>
-      <c r="E13">
+      <c r="E15">
         <v>0.2358490566037736</v>
       </c>
-      <c r="F13">
+      <c r="F15">
         <v>0.3571428571428571</v>
       </c>
-      <c r="G13">
+      <c r="G15">
         <v>0.5165289256198347</v>
       </c>
-      <c r="H13">
+      <c r="H15">
         <v>0.2307692307692308</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DADA2 stuff finished. all figures done. are we good?
</commit_message>
<xml_diff>
--- a/results/tables/All_F1_tables.xlsx
+++ b/results/tables/All_F1_tables.xlsx
@@ -520,19 +520,19 @@
         </is>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.9076923076923077</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.6344086021505376</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.7468354430379748</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>0.8356940509915014</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>0.5959595959595959</v>
       </c>
     </row>
     <row r="6">
@@ -1023,19 +1023,19 @@
         </is>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.9803921568627451</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.5102040816326531</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.6711409395973154</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>0.8278145695364236</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>0.5050505050505051</v>
       </c>
     </row>
     <row r="6">
@@ -1426,7 +1426,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D2">
@@ -1458,7 +1458,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D3">
@@ -1490,7 +1490,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D4">
@@ -1522,7 +1522,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D5">
@@ -1554,7 +1554,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D6">
@@ -1586,7 +1586,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D7">
@@ -1618,7 +1618,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D8">
@@ -1650,7 +1650,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D9">
@@ -1682,7 +1682,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D10">
@@ -1714,7 +1714,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D11">
@@ -1746,7 +1746,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D12">
@@ -1778,7 +1778,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D13">
@@ -1810,7 +1810,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D14">
@@ -1842,7 +1842,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D15">
@@ -2029,19 +2029,19 @@
         </is>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.7777777777777778</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>0.8641975308641976</v>
       </c>
       <c r="H5">
-        <v>0.08333333333333333</v>
+        <v>0.6666666666666666</v>
       </c>
     </row>
     <row r="6">
@@ -2532,19 +2532,19 @@
         </is>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.9</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.5142857142857143</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>0.6923076923076923</v>
       </c>
       <c r="H5">
-        <v>0.03703703703703703</v>
+        <v>0.3703703703703703</v>
       </c>
     </row>
     <row r="6">
@@ -2935,7 +2935,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D2">
@@ -2967,7 +2967,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D3">
@@ -2999,7 +2999,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D4">
@@ -3031,7 +3031,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D5">
@@ -3063,7 +3063,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D6">
@@ -3095,7 +3095,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D7">
@@ -3127,7 +3127,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D8">
@@ -3159,7 +3159,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D9">
@@ -3191,7 +3191,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D10">
@@ -3223,7 +3223,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D11">
@@ -3255,7 +3255,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D12">
@@ -3287,7 +3287,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D13">
@@ -3319,7 +3319,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D14">
@@ -3351,7 +3351,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D15">
@@ -3538,19 +3538,19 @@
         </is>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.5816326530612245</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.7215189873417721</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>0.8431952662721893</v>
       </c>
       <c r="H5">
-        <v>0.009803921568627451</v>
+        <v>0.5686274509803921</v>
       </c>
     </row>
     <row r="6">
@@ -4041,19 +4041,19 @@
         </is>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>0.7926829268292683</v>
       </c>
       <c r="H5">
-        <v>0.03571428571428571</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6">
@@ -4444,7 +4444,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D2">
@@ -4476,7 +4476,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D3">
@@ -4508,7 +4508,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D4">
@@ -4540,7 +4540,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D5">
@@ -4572,7 +4572,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D6">
@@ -4604,7 +4604,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D7">
@@ -4636,7 +4636,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D8">
@@ -4668,7 +4668,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D9">
@@ -4700,7 +4700,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D10">
@@ -4732,7 +4732,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D11">
@@ -4764,7 +4764,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D12">
@@ -4796,7 +4796,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D13">
@@ -4828,7 +4828,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D14">
@@ -4860,7 +4860,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>CO1</t>
+          <t>COI</t>
         </is>
       </c>
       <c r="D15">

</xml_diff>

<commit_message>
New Metabuli version results
</commit_message>
<xml_diff>
--- a/results/tables/All_F1_tables.xlsx
+++ b/results/tables/All_F1_tables.xlsx
@@ -744,19 +744,19 @@
         </is>
       </c>
       <c r="D12">
-        <v>0.7808219178082192</v>
+        <v>0.8115942028985508</v>
       </c>
       <c r="E12">
-        <v>0.6867469879518072</v>
+        <v>0.6511627906976745</v>
       </c>
       <c r="F12">
-        <v>0.7307692307692306</v>
+        <v>0.7225806451612903</v>
       </c>
       <c r="G12">
-        <v>0.76</v>
+        <v>0.7734806629834254</v>
       </c>
       <c r="H12">
-        <v>0.5757575757575758</v>
+        <v>0.5656565656565656</v>
       </c>
     </row>
     <row r="13">
@@ -1247,19 +1247,19 @@
         </is>
       </c>
       <c r="D12">
-        <v>0.7236842105263158</v>
+        <v>0.7464788732394366</v>
       </c>
       <c r="E12">
-        <v>0.7051282051282052</v>
+        <v>0.654320987654321</v>
       </c>
       <c r="F12">
-        <v>0.7142857142857143</v>
+        <v>0.6973684210526315</v>
       </c>
       <c r="G12">
-        <v>0.7198952879581152</v>
+        <v>0.726027397260274</v>
       </c>
       <c r="H12">
-        <v>0.5555555555555556</v>
+        <v>0.5353535353535354</v>
       </c>
     </row>
     <row r="13">
@@ -1750,19 +1750,19 @@
         </is>
       </c>
       <c r="D12">
-        <v>0.868421052631579</v>
+        <v>0.9491525423728814</v>
       </c>
       <c r="E12">
-        <v>0.4459459459459459</v>
+        <v>0.8235294117647058</v>
       </c>
       <c r="F12">
-        <v>0.5892857142857143</v>
+        <v>0.8818897637795277</v>
       </c>
       <c r="G12">
-        <v>0.7300884955752212</v>
+        <v>0.9210526315789472</v>
       </c>
       <c r="H12">
-        <v>0.5353535353535354</v>
+        <v>0.8484848484848485</v>
       </c>
     </row>
     <row r="13">
@@ -2253,19 +2253,19 @@
         </is>
       </c>
       <c r="D12">
-        <v>0.8947368421052632</v>
+        <v>0.9411764705882353</v>
       </c>
       <c r="E12">
-        <v>0.85</v>
+        <v>0.7619047619047619</v>
       </c>
       <c r="F12">
-        <v>0.8717948717948718</v>
+        <v>0.8421052631578947</v>
       </c>
       <c r="G12">
-        <v>0.8854166666666667</v>
+        <v>0.898876404494382</v>
       </c>
       <c r="H12">
-        <v>0.7916666666666666</v>
+        <v>0.75</v>
       </c>
     </row>
     <row r="13">
@@ -3259,19 +3259,19 @@
         </is>
       </c>
       <c r="D12">
-        <v>0.9411764705882353</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>0.64</v>
+        <v>0.92</v>
       </c>
       <c r="F12">
-        <v>0.7619047619047621</v>
+        <v>0.9583333333333334</v>
       </c>
       <c r="G12">
-        <v>0.8602150537634409</v>
+        <v>0.9829059829059831</v>
       </c>
       <c r="H12">
-        <v>0.6296296296296297</v>
+        <v>0.9259259259259259</v>
       </c>
     </row>
     <row r="13">
@@ -3762,16 +3762,16 @@
         </is>
       </c>
       <c r="D12">
-        <v>0.8441558441558441</v>
+        <v>0.8552631578947368</v>
       </c>
       <c r="E12">
-        <v>0.7303370786516854</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="F12">
-        <v>0.7831325301204819</v>
+        <v>0.783132530120482</v>
       </c>
       <c r="G12">
-        <v>0.8186397984886651</v>
+        <v>0.8248730964467005</v>
       </c>
       <c r="H12">
         <v>0.6470588235294118</v>
@@ -4265,19 +4265,19 @@
         </is>
       </c>
       <c r="D12">
-        <v>0.7727272727272727</v>
+        <v>0.7931034482758621</v>
       </c>
       <c r="E12">
-        <v>0.7727272727272727</v>
+        <v>0.7666666666666667</v>
       </c>
       <c r="F12">
-        <v>0.7727272727272727</v>
+        <v>0.7796610169491527</v>
       </c>
       <c r="G12">
-        <v>0.7727272727272727</v>
+        <v>0.7876712328767123</v>
       </c>
       <c r="H12">
-        <v>0.6428571428571429</v>
+        <v>0.6517857142857143</v>
       </c>
     </row>
     <row r="13">
@@ -4768,19 +4768,19 @@
         </is>
       </c>
       <c r="D12">
-        <v>0.927536231884058</v>
+        <v>0.9782608695652174</v>
       </c>
       <c r="E12">
-        <v>0.5765765765765766</v>
+        <v>0.7964601769911505</v>
       </c>
       <c r="F12">
-        <v>0.7111111111111111</v>
+        <v>0.8780487804878049</v>
       </c>
       <c r="G12">
-        <v>0.82687338501292</v>
+        <v>0.9355509355509356</v>
       </c>
       <c r="H12">
-        <v>0.5555555555555556</v>
+        <v>0.7863247863247863</v>
       </c>
     </row>
     <row r="13">

</xml_diff>

<commit_message>
full rewrite of COI part. input amplicons changed. entire pipeline output changed.
</commit_message>
<xml_diff>
--- a/results/tables/All_F1_tables.xlsx
+++ b/results/tables/All_F1_tables.xlsx
@@ -14,8 +14,6 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
     <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
-    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -1365,7 +1363,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1430,19 +1428,19 @@
         </is>
       </c>
       <c r="D2">
-        <v>0.9795918367346939</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>0.6666666666666666</v>
+        <v>0.6904761904761905</v>
       </c>
       <c r="F2">
-        <v>0.793388429752066</v>
+        <v>0.8169014084507042</v>
       </c>
       <c r="G2">
-        <v>0.8955223880597016</v>
+        <v>0.9177215189873418</v>
       </c>
       <c r="H2">
-        <v>0.7474747474747475</v>
+        <v>0.7373737373737373</v>
       </c>
     </row>
     <row r="3">
@@ -1462,19 +1460,19 @@
         </is>
       </c>
       <c r="D3">
-        <v>0.9583333333333334</v>
+        <v>0.9803921568627451</v>
       </c>
       <c r="E3">
-        <v>0.6666666666666666</v>
+        <v>0.6024096385542169</v>
       </c>
       <c r="F3">
-        <v>0.7863247863247863</v>
+        <v>0.746268656716418</v>
       </c>
       <c r="G3">
-        <v>0.8812260536398469</v>
+        <v>0.8710801393728221</v>
       </c>
       <c r="H3">
-        <v>0.7474747474747475</v>
+        <v>0.6565656565656566</v>
       </c>
     </row>
     <row r="4">
@@ -1494,19 +1492,19 @@
         </is>
       </c>
       <c r="D4">
-        <v>0.864406779661017</v>
+        <v>0.863013698630137</v>
       </c>
       <c r="E4">
-        <v>0.8095238095238095</v>
+        <v>0.8513513513513513</v>
       </c>
       <c r="F4">
-        <v>0.8360655737704918</v>
+        <v>0.8571428571428572</v>
       </c>
       <c r="G4">
-        <v>0.8528428093645484</v>
+        <v>0.8606557377049179</v>
       </c>
       <c r="H4">
-        <v>0.797979797979798</v>
+        <v>0.7878787878787878</v>
       </c>
     </row>
     <row r="5">
@@ -1526,25 +1524,25 @@
         </is>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.6785714285714286</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.8085106382978724</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>0.9134615384615385</v>
       </c>
       <c r="H5">
-        <v>0.2828282828282828</v>
+        <v>0.7272727272727273</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DADA2Tax</t>
+          <t>Kraken2_0.0</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1558,25 +1556,25 @@
         </is>
       </c>
       <c r="D6">
-        <v>0.3333333333333333</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>0.2244897959183673</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>0.2682926829268293</v>
+        <v>0</v>
       </c>
       <c r="G6">
-        <v>0.3038674033149171</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>0.3939393939393939</v>
+        <v>0.1515151515151515</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Kraken2_0.0</t>
+          <t>Kraken2_0.05</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1590,25 +1588,25 @@
         </is>
       </c>
       <c r="D7">
-        <v>0.96</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>0.6956521739130435</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <v>0.8067226890756302</v>
+        <v>0</v>
       </c>
       <c r="G7">
-        <v>0.8921933085501859</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>0.7676767676767676</v>
+        <v>0.1515151515151515</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Kraken2_0.05</t>
+          <t>Kraken2_0.1</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1622,25 +1620,25 @@
         </is>
       </c>
       <c r="D8">
-        <v>0.9743589743589743</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>0.5428571428571428</v>
+        <v>0</v>
       </c>
       <c r="F8">
-        <v>0.6972477064220183</v>
+        <v>0</v>
       </c>
       <c r="G8">
-        <v>0.8407079646017698</v>
+        <v>0</v>
       </c>
       <c r="H8">
-        <v>0.6666666666666666</v>
+        <v>0.1515151515151515</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Kraken2_0.1</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1654,25 +1652,25 @@
         </is>
       </c>
       <c r="D9">
-        <v>0.9642857142857143</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>0.3857142857142857</v>
+        <v>0.6785714285714286</v>
       </c>
       <c r="F9">
-        <v>0.5510204081632653</v>
+        <v>0.8085106382978724</v>
       </c>
       <c r="G9">
-        <v>0.7417582417582418</v>
+        <v>0.9134615384615385</v>
       </c>
       <c r="H9">
-        <v>0.5555555555555556</v>
+        <v>0.7272727272727273</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MMSeqs2_100</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1686,25 +1684,25 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.9722222222222222</v>
+        <v>0.9682539682539683</v>
       </c>
       <c r="E10">
-        <v>0.5</v>
+        <v>0.7439024390243902</v>
       </c>
       <c r="F10">
-        <v>0.660377358490566</v>
+        <v>0.8413793103448277</v>
       </c>
       <c r="G10">
-        <v>0.8177570093457943</v>
+        <v>0.9131736526946107</v>
       </c>
       <c r="H10">
-        <v>0.6363636363636364</v>
+        <v>0.7676767676767676</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MMSeqs2_97</t>
+          <t>Metabuli</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1718,25 +1716,25 @@
         </is>
       </c>
       <c r="D11">
-        <v>0.9830508474576272</v>
+        <v>0.9230769230769231</v>
       </c>
       <c r="E11">
-        <v>0.8285714285714286</v>
+        <v>0.2926829268292683</v>
       </c>
       <c r="F11">
-        <v>0.8992248062015504</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="G11">
-        <v>0.9477124183006537</v>
+        <v>0.6451612903225807</v>
       </c>
       <c r="H11">
-        <v>0.8686868686868687</v>
+        <v>0.3939393939393939</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Metabuli</t>
+          <t>Mothur</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1750,25 +1748,25 @@
         </is>
       </c>
       <c r="D12">
-        <v>0.9491525423728814</v>
+        <v>0.8648648648648649</v>
       </c>
       <c r="E12">
-        <v>0.8235294117647058</v>
+        <v>0.8648648648648649</v>
       </c>
       <c r="F12">
-        <v>0.8818897637795277</v>
+        <v>0.8648648648648649</v>
       </c>
       <c r="G12">
-        <v>0.9210526315789472</v>
+        <v>0.8648648648648649</v>
       </c>
       <c r="H12">
-        <v>0.8484848484848485</v>
+        <v>0.797979797979798</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>Qiime2</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1782,25 +1780,25 @@
         </is>
       </c>
       <c r="D13">
-        <v>0.8666666666666667</v>
+        <v>0.864406779661017</v>
       </c>
       <c r="E13">
-        <v>0.8253968253968254</v>
+        <v>0.6219512195121951</v>
       </c>
       <c r="F13">
-        <v>0.8455284552845528</v>
+        <v>0.723404255319149</v>
       </c>
       <c r="G13">
-        <v>0.8580858085808584</v>
+        <v>0.8018867924528302</v>
       </c>
       <c r="H13">
-        <v>0.8080808080808081</v>
+        <v>0.6060606060606061</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Qiime2</t>
+          <t>VSEARCH</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -1814,51 +1812,19 @@
         </is>
       </c>
       <c r="D14">
-        <v>0.8909090909090909</v>
+        <v>0.8695652173913043</v>
       </c>
       <c r="E14">
-        <v>0.5833333333333334</v>
+        <v>0.8</v>
       </c>
       <c r="F14">
-        <v>0.7050359712230215</v>
+        <v>0.8333333333333333</v>
       </c>
       <c r="G14">
-        <v>0.8059210526315789</v>
+        <v>0.8547008547008546</v>
       </c>
       <c r="H14">
-        <v>0.5858585858585859</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>VSEARCH</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>100 Australian species</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>COI</t>
-        </is>
-      </c>
-      <c r="D15">
-        <v>0.2</v>
-      </c>
-      <c r="E15">
-        <v>0.01492537313432836</v>
-      </c>
-      <c r="F15">
-        <v>0.02777777777777778</v>
-      </c>
-      <c r="G15">
-        <v>0.05747126436781608</v>
-      </c>
-      <c r="H15">
-        <v>0.2929292929292929</v>
+        <v>0.7575757575757576</v>
       </c>
     </row>
   </sheetData>
@@ -2930,28 +2896,28 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Lutjanidae</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>COI</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0.9661016949152542</v>
       </c>
       <c r="E2">
-        <v>0.52</v>
+        <v>0.5757575757575758</v>
       </c>
       <c r="F2">
-        <v>0.6842105263157895</v>
+        <v>0.7215189873417721</v>
       </c>
       <c r="G2">
-        <v>0.8441558441558442</v>
+        <v>0.8507462686567164</v>
       </c>
       <c r="H2">
-        <v>0.5555555555555556</v>
+        <v>0.5686274509803921</v>
       </c>
     </row>
     <row r="3">
@@ -2962,28 +2928,28 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Lutjanidae</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>COI</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0.8805970149253731</v>
       </c>
       <c r="E3">
-        <v>0.68</v>
+        <v>0.6344086021505376</v>
       </c>
       <c r="F3">
-        <v>0.8095238095238095</v>
+        <v>0.7375</v>
       </c>
       <c r="G3">
-        <v>0.913978494623656</v>
+        <v>0.817174515235457</v>
       </c>
       <c r="H3">
-        <v>0.7037037037037037</v>
+        <v>0.5882352941176471</v>
       </c>
     </row>
     <row r="4">
@@ -2994,28 +2960,28 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Lutjanidae</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>COI</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D4">
-        <v>0.92</v>
+        <v>0.7571428571428571</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>0.6309523809523809</v>
       </c>
       <c r="F4">
-        <v>0.9583333333333334</v>
+        <v>0.6883116883116883</v>
       </c>
       <c r="G4">
-        <v>0.934959349593496</v>
+        <v>0.7280219780219781</v>
       </c>
       <c r="H4">
-        <v>0.9259259259259259</v>
+        <v>0.5294117647058824</v>
       </c>
     </row>
     <row r="5">
@@ -3026,28 +2992,28 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Lutjanidae</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>COI</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.5816326530612245</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.7215189873417721</v>
       </c>
       <c r="G5">
-        <v>0</v>
+        <v>0.8431952662721893</v>
       </c>
       <c r="H5">
-        <v>0.07407407407407407</v>
+        <v>0.5686274509803921</v>
       </c>
     </row>
     <row r="6">
@@ -3058,28 +3024,28 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Lutjanidae</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>COI</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D6">
-        <v>0.7142857142857143</v>
+        <v>0.21875</v>
       </c>
       <c r="E6">
-        <v>0.4761904761904762</v>
+        <v>0.09210526315789473</v>
       </c>
       <c r="F6">
-        <v>0.5714285714285714</v>
+        <v>0.1296296296296296</v>
       </c>
       <c r="G6">
-        <v>0.6493506493506493</v>
+        <v>0.1715686274509804</v>
       </c>
       <c r="H6">
-        <v>0.4444444444444444</v>
+        <v>0.07843137254901961</v>
       </c>
     </row>
     <row r="7">
@@ -3090,28 +3056,28 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Lutjanidae</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>COI</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="E7">
-        <v>0.76</v>
+        <v>0.6741573033707865</v>
       </c>
       <c r="F7">
-        <v>0.8636363636363636</v>
+        <v>0.7453416149068324</v>
       </c>
       <c r="G7">
-        <v>0.9405940594059405</v>
+        <v>0.7957559681697614</v>
       </c>
       <c r="H7">
-        <v>0.7777777777777778</v>
+        <v>0.5980392156862745</v>
       </c>
     </row>
     <row r="8">
@@ -3122,28 +3088,28 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Lutjanidae</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>COI</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>0.8636363636363636</v>
       </c>
       <c r="E8">
-        <v>0.44</v>
+        <v>0.6195652173913043</v>
       </c>
       <c r="F8">
-        <v>0.6111111111111112</v>
+        <v>0.7215189873417721</v>
       </c>
       <c r="G8">
-        <v>0.7971014492753624</v>
+        <v>0.800561797752809</v>
       </c>
       <c r="H8">
-        <v>0.4814814814814815</v>
+        <v>0.5686274509803921</v>
       </c>
     </row>
     <row r="9">
@@ -3154,28 +3120,28 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Lutjanidae</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>COI</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0.9137931034482759</v>
       </c>
       <c r="E9">
-        <v>0.24</v>
+        <v>0.5520833333333334</v>
       </c>
       <c r="F9">
-        <v>0.3870967741935484</v>
+        <v>0.6883116883116883</v>
       </c>
       <c r="G9">
-        <v>0.6122448979591837</v>
+        <v>0.8079268292682928</v>
       </c>
       <c r="H9">
-        <v>0.2962962962962963</v>
+        <v>0.5294117647058824</v>
       </c>
     </row>
     <row r="10">
@@ -3186,28 +3152,28 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Lutjanidae</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>COI</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>0.9666666666666667</v>
       </c>
       <c r="E10">
-        <v>0.44</v>
+        <v>0.5858585858585859</v>
       </c>
       <c r="F10">
-        <v>0.6111111111111112</v>
+        <v>0.729559748427673</v>
       </c>
       <c r="G10">
-        <v>0.7971014492753624</v>
+        <v>0.8554572271386429</v>
       </c>
       <c r="H10">
-        <v>0.4814814814814815</v>
+        <v>0.5784313725490197</v>
       </c>
     </row>
     <row r="11">
@@ -3218,28 +3184,28 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Lutjanidae</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>COI</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>0.9014084507042254</v>
       </c>
       <c r="E11">
-        <v>0.92</v>
+        <v>0.6808510638297872</v>
       </c>
       <c r="F11">
-        <v>0.9583333333333334</v>
+        <v>0.7757575757575758</v>
       </c>
       <c r="G11">
-        <v>0.9829059829059831</v>
+        <v>0.8465608465608466</v>
       </c>
       <c r="H11">
-        <v>0.9259259259259259</v>
+        <v>0.6372549019607843</v>
       </c>
     </row>
     <row r="12">
@@ -3250,28 +3216,28 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Lutjanidae</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>COI</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>0.8552631578947368</v>
       </c>
       <c r="E12">
-        <v>0.92</v>
+        <v>0.7222222222222222</v>
       </c>
       <c r="F12">
-        <v>0.9583333333333334</v>
+        <v>0.783132530120482</v>
       </c>
       <c r="G12">
-        <v>0.9829059829059831</v>
+        <v>0.8248730964467005</v>
       </c>
       <c r="H12">
-        <v>0.9259259259259259</v>
+        <v>0.6470588235294118</v>
       </c>
     </row>
     <row r="13">
@@ -3282,28 +3248,28 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Lutjanidae</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>COI</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D13">
-        <v>0.92</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="E13">
-        <v>1</v>
+        <v>0.525</v>
       </c>
       <c r="F13">
-        <v>0.9583333333333334</v>
+        <v>0.5874125874125874</v>
       </c>
       <c r="G13">
-        <v>0.934959349593496</v>
+        <v>0.6325301204819277</v>
       </c>
       <c r="H13">
-        <v>0.9259259259259259</v>
+        <v>0.4215686274509804</v>
       </c>
     </row>
     <row r="14">
@@ -3314,28 +3280,28 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Lutjanidae</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>COI</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D14">
-        <v>0.92</v>
+        <v>0.6458333333333334</v>
       </c>
       <c r="E14">
-        <v>0.9583333333333334</v>
+        <v>0.3690476190476191</v>
       </c>
       <c r="F14">
-        <v>0.9387755102040817</v>
+        <v>0.4696969696969697</v>
       </c>
       <c r="G14">
-        <v>0.9274193548387097</v>
+        <v>0.5615942028985508</v>
       </c>
       <c r="H14">
-        <v>0.8888888888888888</v>
+        <v>0.3137254901960784</v>
       </c>
     </row>
     <row r="15">
@@ -3346,28 +3312,28 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Lutjanidae</t>
+          <t>Wadjemup</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>COI</t>
+          <t>12S</t>
         </is>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0.7647058823529411</v>
       </c>
       <c r="E15">
-        <v>0.2</v>
+        <v>0.611764705882353</v>
       </c>
       <c r="F15">
-        <v>0.3333333333333334</v>
+        <v>0.6797385620915033</v>
       </c>
       <c r="G15">
-        <v>0.5555555555555556</v>
+        <v>0.7282913165266106</v>
       </c>
       <c r="H15">
-        <v>0.2592592592592592</v>
+        <v>0.5196078431372549</v>
       </c>
     </row>
   </sheetData>
@@ -3438,23 +3404,23 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D2">
-        <v>0.9661016949152542</v>
+        <v>0.9464285714285714</v>
       </c>
       <c r="E2">
-        <v>0.5757575757575758</v>
+        <v>0.4953271028037383</v>
       </c>
       <c r="F2">
-        <v>0.7215189873417721</v>
+        <v>0.6503067484662577</v>
       </c>
       <c r="G2">
-        <v>0.8507462686567164</v>
+        <v>0.8006042296072508</v>
       </c>
       <c r="H2">
-        <v>0.5686274509803921</v>
+        <v>0.4910714285714285</v>
       </c>
     </row>
     <row r="3">
@@ -3470,23 +3436,23 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D3">
-        <v>0.8805970149253731</v>
+        <v>0.9117647058823529</v>
       </c>
       <c r="E3">
-        <v>0.6344086021505376</v>
+        <v>0.6078431372549019</v>
       </c>
       <c r="F3">
-        <v>0.7375</v>
+        <v>0.7294117647058823</v>
       </c>
       <c r="G3">
-        <v>0.817174515235457</v>
+        <v>0.8288770053475936</v>
       </c>
       <c r="H3">
-        <v>0.5882352941176471</v>
+        <v>0.5892857142857143</v>
       </c>
     </row>
     <row r="4">
@@ -3502,23 +3468,23 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D4">
-        <v>0.7571428571428571</v>
+        <v>0.7671232876712328</v>
       </c>
       <c r="E4">
-        <v>0.6309523809523809</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="F4">
-        <v>0.6883116883116883</v>
+        <v>0.6829268292682927</v>
       </c>
       <c r="G4">
-        <v>0.7280219780219781</v>
+        <v>0.7310704960835509</v>
       </c>
       <c r="H4">
-        <v>0.5294117647058824</v>
+        <v>0.5357142857142857</v>
       </c>
     </row>
     <row r="5">
@@ -3534,23 +3500,23 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D5">
-        <v>0.95</v>
+        <v>0.9285714285714286</v>
       </c>
       <c r="E5">
-        <v>0.5816326530612245</v>
+        <v>0.5</v>
       </c>
       <c r="F5">
-        <v>0.7215189873417721</v>
+        <v>0.65</v>
       </c>
       <c r="G5">
-        <v>0.8431952662721893</v>
+        <v>0.7926829268292683</v>
       </c>
       <c r="H5">
-        <v>0.5686274509803921</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="6">
@@ -3566,23 +3532,23 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D6">
-        <v>0.21875</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="E6">
-        <v>0.09210526315789473</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="F6">
-        <v>0.1296296296296296</v>
+        <v>0.1379310344827586</v>
       </c>
       <c r="G6">
-        <v>0.1715686274509804</v>
+        <v>0.1538461538461538</v>
       </c>
       <c r="H6">
-        <v>0.07843137254901961</v>
+        <v>0.1071428571428571</v>
       </c>
     </row>
     <row r="7">
@@ -3598,23 +3564,23 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D7">
-        <v>0.8333333333333334</v>
+        <v>0.813953488372093</v>
       </c>
       <c r="E7">
-        <v>0.6741573033707865</v>
+        <v>0.7608695652173914</v>
       </c>
       <c r="F7">
-        <v>0.7453416149068324</v>
+        <v>0.7865168539325844</v>
       </c>
       <c r="G7">
-        <v>0.7957559681697614</v>
+        <v>0.8027522935779817</v>
       </c>
       <c r="H7">
-        <v>0.5980392156862745</v>
+        <v>0.6607142857142857</v>
       </c>
     </row>
     <row r="8">
@@ -3630,23 +3596,23 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D8">
-        <v>0.8636363636363636</v>
+        <v>0.8625</v>
       </c>
       <c r="E8">
-        <v>0.6195652173913043</v>
+        <v>0.711340206185567</v>
       </c>
       <c r="F8">
-        <v>0.7215189873417721</v>
+        <v>0.7796610169491526</v>
       </c>
       <c r="G8">
-        <v>0.800561797752809</v>
+        <v>0.8273381294964028</v>
       </c>
       <c r="H8">
-        <v>0.5686274509803921</v>
+        <v>0.6517857142857143</v>
       </c>
     </row>
     <row r="9">
@@ -3662,23 +3628,23 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D9">
-        <v>0.9137931034482759</v>
+        <v>0.8918918918918919</v>
       </c>
       <c r="E9">
-        <v>0.5520833333333334</v>
+        <v>0.66</v>
       </c>
       <c r="F9">
-        <v>0.6883116883116883</v>
+        <v>0.7586206896551725</v>
       </c>
       <c r="G9">
-        <v>0.8079268292682928</v>
+        <v>0.8333333333333335</v>
       </c>
       <c r="H9">
-        <v>0.5294117647058824</v>
+        <v>0.625</v>
       </c>
     </row>
     <row r="10">
@@ -3694,23 +3660,23 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D10">
-        <v>0.9666666666666667</v>
+        <v>0.9473684210526315</v>
       </c>
       <c r="E10">
-        <v>0.5858585858585859</v>
+        <v>0.5142857142857142</v>
       </c>
       <c r="F10">
-        <v>0.729559748427673</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G10">
-        <v>0.8554572271386429</v>
+        <v>0.8108108108108107</v>
       </c>
       <c r="H10">
-        <v>0.5784313725490197</v>
+        <v>0.5178571428571429</v>
       </c>
     </row>
     <row r="11">
@@ -3726,23 +3692,23 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D11">
-        <v>0.9014084507042254</v>
+        <v>0.8961038961038961</v>
       </c>
       <c r="E11">
-        <v>0.6808510638297872</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="F11">
-        <v>0.7757575757575758</v>
+        <v>0.7796610169491525</v>
       </c>
       <c r="G11">
-        <v>0.8465608465608466</v>
+        <v>0.8455882352941176</v>
       </c>
       <c r="H11">
-        <v>0.6372549019607843</v>
+        <v>0.6517857142857143</v>
       </c>
     </row>
     <row r="12">
@@ -3758,23 +3724,23 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D12">
-        <v>0.8552631578947368</v>
+        <v>0.7931034482758621</v>
       </c>
       <c r="E12">
-        <v>0.7222222222222222</v>
+        <v>0.7666666666666667</v>
       </c>
       <c r="F12">
-        <v>0.783132530120482</v>
+        <v>0.7796610169491527</v>
       </c>
       <c r="G12">
-        <v>0.8248730964467005</v>
+        <v>0.7876712328767123</v>
       </c>
       <c r="H12">
-        <v>0.6470588235294118</v>
+        <v>0.6517857142857143</v>
       </c>
     </row>
     <row r="13">
@@ -3790,23 +3756,23 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D13">
-        <v>0.6666666666666666</v>
+        <v>0.7093023255813954</v>
       </c>
       <c r="E13">
-        <v>0.525</v>
+        <v>0.7349397590361446</v>
       </c>
       <c r="F13">
-        <v>0.5874125874125874</v>
+        <v>0.7218934911242604</v>
       </c>
       <c r="G13">
-        <v>0.6325301204819277</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="H13">
-        <v>0.4215686274509804</v>
+        <v>0.5803571428571429</v>
       </c>
     </row>
     <row r="14">
@@ -3822,23 +3788,23 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>12S</t>
+          <t>16S</t>
         </is>
       </c>
       <c r="D14">
-        <v>0.6458333333333334</v>
+        <v>0.7466666666666667</v>
       </c>
       <c r="E14">
-        <v>0.3690476190476191</v>
+        <v>0.6153846153846154</v>
       </c>
       <c r="F14">
-        <v>0.4696969696969697</v>
+        <v>0.674698795180723</v>
       </c>
       <c r="G14">
-        <v>0.5615942028985508</v>
+        <v>0.7161125319693096</v>
       </c>
       <c r="H14">
-        <v>0.3137254901960784</v>
+        <v>0.5178571428571429</v>
       </c>
     </row>
     <row r="15">
@@ -3854,509 +3820,6 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>12S</t>
-        </is>
-      </c>
-      <c r="D15">
-        <v>0.7647058823529411</v>
-      </c>
-      <c r="E15">
-        <v>0.611764705882353</v>
-      </c>
-      <c r="F15">
-        <v>0.6797385620915033</v>
-      </c>
-      <c r="G15">
-        <v>0.7282913165266106</v>
-      </c>
-      <c r="H15">
-        <v>0.5196078431372549</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Query</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Subject</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Precision</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Recall</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>F1</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>F0.5</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Accuracy</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>BLAST100</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>16S</t>
-        </is>
-      </c>
-      <c r="D2">
-        <v>0.9464285714285714</v>
-      </c>
-      <c r="E2">
-        <v>0.4953271028037383</v>
-      </c>
-      <c r="F2">
-        <v>0.6503067484662577</v>
-      </c>
-      <c r="G2">
-        <v>0.8006042296072508</v>
-      </c>
-      <c r="H2">
-        <v>0.4910714285714285</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>BLAST97</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>16S</t>
-        </is>
-      </c>
-      <c r="D3">
-        <v>0.9117647058823529</v>
-      </c>
-      <c r="E3">
-        <v>0.6078431372549019</v>
-      </c>
-      <c r="F3">
-        <v>0.7294117647058823</v>
-      </c>
-      <c r="G3">
-        <v>0.8288770053475936</v>
-      </c>
-      <c r="H3">
-        <v>0.5892857142857143</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>CustomNBC</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>16S</t>
-        </is>
-      </c>
-      <c r="D4">
-        <v>0.7671232876712328</v>
-      </c>
-      <c r="E4">
-        <v>0.6153846153846154</v>
-      </c>
-      <c r="F4">
-        <v>0.6829268292682927</v>
-      </c>
-      <c r="G4">
-        <v>0.7310704960835509</v>
-      </c>
-      <c r="H4">
-        <v>0.5357142857142857</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>DADA2Spec</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>16S</t>
-        </is>
-      </c>
-      <c r="D5">
-        <v>0.9285714285714286</v>
-      </c>
-      <c r="E5">
-        <v>0.5</v>
-      </c>
-      <c r="F5">
-        <v>0.65</v>
-      </c>
-      <c r="G5">
-        <v>0.7926829268292683</v>
-      </c>
-      <c r="H5">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>DADA2Tax</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>16S</t>
-        </is>
-      </c>
-      <c r="D6">
-        <v>0.1666666666666667</v>
-      </c>
-      <c r="E6">
-        <v>0.1176470588235294</v>
-      </c>
-      <c r="F6">
-        <v>0.1379310344827586</v>
-      </c>
-      <c r="G6">
-        <v>0.1538461538461538</v>
-      </c>
-      <c r="H6">
-        <v>0.1071428571428571</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Kraken2_0.0</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>16S</t>
-        </is>
-      </c>
-      <c r="D7">
-        <v>0.813953488372093</v>
-      </c>
-      <c r="E7">
-        <v>0.7608695652173914</v>
-      </c>
-      <c r="F7">
-        <v>0.7865168539325844</v>
-      </c>
-      <c r="G7">
-        <v>0.8027522935779817</v>
-      </c>
-      <c r="H7">
-        <v>0.6607142857142857</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Kraken2_0.05</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>16S</t>
-        </is>
-      </c>
-      <c r="D8">
-        <v>0.8625</v>
-      </c>
-      <c r="E8">
-        <v>0.711340206185567</v>
-      </c>
-      <c r="F8">
-        <v>0.7796610169491526</v>
-      </c>
-      <c r="G8">
-        <v>0.8273381294964028</v>
-      </c>
-      <c r="H8">
-        <v>0.6517857142857143</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Kraken2_0.1</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>16S</t>
-        </is>
-      </c>
-      <c r="D9">
-        <v>0.8918918918918919</v>
-      </c>
-      <c r="E9">
-        <v>0.66</v>
-      </c>
-      <c r="F9">
-        <v>0.7586206896551725</v>
-      </c>
-      <c r="G9">
-        <v>0.8333333333333335</v>
-      </c>
-      <c r="H9">
-        <v>0.625</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>MMSeqs2_100</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>16S</t>
-        </is>
-      </c>
-      <c r="D10">
-        <v>0.9473684210526315</v>
-      </c>
-      <c r="E10">
-        <v>0.5142857142857142</v>
-      </c>
-      <c r="F10">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="G10">
-        <v>0.8108108108108107</v>
-      </c>
-      <c r="H10">
-        <v>0.5178571428571429</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>MMSeqs2_97</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>16S</t>
-        </is>
-      </c>
-      <c r="D11">
-        <v>0.8961038961038961</v>
-      </c>
-      <c r="E11">
-        <v>0.6899999999999999</v>
-      </c>
-      <c r="F11">
-        <v>0.7796610169491525</v>
-      </c>
-      <c r="G11">
-        <v>0.8455882352941176</v>
-      </c>
-      <c r="H11">
-        <v>0.6517857142857143</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Metabuli</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>16S</t>
-        </is>
-      </c>
-      <c r="D12">
-        <v>0.7931034482758621</v>
-      </c>
-      <c r="E12">
-        <v>0.7666666666666667</v>
-      </c>
-      <c r="F12">
-        <v>0.7796610169491527</v>
-      </c>
-      <c r="G12">
-        <v>0.7876712328767123</v>
-      </c>
-      <c r="H12">
-        <v>0.6517857142857143</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Mothur</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>16S</t>
-        </is>
-      </c>
-      <c r="D13">
-        <v>0.7093023255813954</v>
-      </c>
-      <c r="E13">
-        <v>0.7349397590361446</v>
-      </c>
-      <c r="F13">
-        <v>0.7218934911242604</v>
-      </c>
-      <c r="G13">
-        <v>0.7142857142857143</v>
-      </c>
-      <c r="H13">
-        <v>0.5803571428571429</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Qiime2</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>16S</t>
-        </is>
-      </c>
-      <c r="D14">
-        <v>0.7466666666666667</v>
-      </c>
-      <c r="E14">
-        <v>0.6153846153846154</v>
-      </c>
-      <c r="F14">
-        <v>0.674698795180723</v>
-      </c>
-      <c r="G14">
-        <v>0.7161125319693096</v>
-      </c>
-      <c r="H14">
-        <v>0.5178571428571429</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>VSEARCH</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
           <t>16S</t>
         </is>
       </c>
@@ -4374,509 +3837,6 @@
       </c>
       <c r="H15">
         <v>0.6428571428571429</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Type</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Query</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Subject</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Precision</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Recall</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>F1</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>F0.5</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Accuracy</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>BLAST100</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>COI</t>
-        </is>
-      </c>
-      <c r="D2">
-        <v>0.9625</v>
-      </c>
-      <c r="E2">
-        <v>0.6875</v>
-      </c>
-      <c r="F2">
-        <v>0.8020833333333334</v>
-      </c>
-      <c r="G2">
-        <v>0.8912037037037037</v>
-      </c>
-      <c r="H2">
-        <v>0.6752136752136753</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>BLAST97</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>COI</t>
-        </is>
-      </c>
-      <c r="D3">
-        <v>0.9404761904761905</v>
-      </c>
-      <c r="E3">
-        <v>0.7181818181818181</v>
-      </c>
-      <c r="F3">
-        <v>0.8144329896907216</v>
-      </c>
-      <c r="G3">
-        <v>0.8856502242152466</v>
-      </c>
-      <c r="H3">
-        <v>0.6923076923076923</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>CustomNBC</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>COI</t>
-        </is>
-      </c>
-      <c r="D4">
-        <v>0.9101123595505618</v>
-      </c>
-      <c r="E4">
-        <v>0.7570093457943925</v>
-      </c>
-      <c r="F4">
-        <v>0.826530612244898</v>
-      </c>
-      <c r="G4">
-        <v>0.8747300215982722</v>
-      </c>
-      <c r="H4">
-        <v>0.7094017094017094</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>DADA2Spec</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>COI</t>
-        </is>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0.0170940170940171</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>DADA2Tax</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>COI</t>
-        </is>
-      </c>
-      <c r="D6">
-        <v>0.3529411764705883</v>
-      </c>
-      <c r="E6">
-        <v>0.2195121951219512</v>
-      </c>
-      <c r="F6">
-        <v>0.2706766917293233</v>
-      </c>
-      <c r="G6">
-        <v>0.3146853146853147</v>
-      </c>
-      <c r="H6">
-        <v>0.1709401709401709</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Kraken2_0.0</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>COI</t>
-        </is>
-      </c>
-      <c r="D7">
-        <v>0.9880952380952381</v>
-      </c>
-      <c r="E7">
-        <v>0.7280701754385965</v>
-      </c>
-      <c r="F7">
-        <v>0.8383838383838385</v>
-      </c>
-      <c r="G7">
-        <v>0.9222222222222223</v>
-      </c>
-      <c r="H7">
-        <v>0.7264957264957265</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Kraken2_0.05</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>COI</t>
-        </is>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>0.6173913043478261</v>
-      </c>
-      <c r="F8">
-        <v>0.7634408602150538</v>
-      </c>
-      <c r="G8">
-        <v>0.8897243107769424</v>
-      </c>
-      <c r="H8">
-        <v>0.6239316239316239</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>Kraken2_0.1</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>COI</t>
-        </is>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>0.5391304347826087</v>
-      </c>
-      <c r="F9">
-        <v>0.7005649717514124</v>
-      </c>
-      <c r="G9">
-        <v>0.8539944903581267</v>
-      </c>
-      <c r="H9">
-        <v>0.5470085470085471</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>MMSeqs2_100</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>COI</t>
-        </is>
-      </c>
-      <c r="D10">
-        <v>0.9830508474576272</v>
-      </c>
-      <c r="E10">
-        <v>0.5087719298245614</v>
-      </c>
-      <c r="F10">
-        <v>0.6705202312138728</v>
-      </c>
-      <c r="G10">
-        <v>0.8285714285714286</v>
-      </c>
-      <c r="H10">
-        <v>0.5128205128205128</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>MMSeqs2_97</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>COI</t>
-        </is>
-      </c>
-      <c r="D11">
-        <v>0.979381443298969</v>
-      </c>
-      <c r="E11">
-        <v>0.8407079646017699</v>
-      </c>
-      <c r="F11">
-        <v>0.9047619047619049</v>
-      </c>
-      <c r="G11">
-        <v>0.9481037924151696</v>
-      </c>
-      <c r="H11">
-        <v>0.8290598290598291</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>Metabuli</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>COI</t>
-        </is>
-      </c>
-      <c r="D12">
-        <v>0.9782608695652174</v>
-      </c>
-      <c r="E12">
-        <v>0.7964601769911505</v>
-      </c>
-      <c r="F12">
-        <v>0.8780487804878049</v>
-      </c>
-      <c r="G12">
-        <v>0.9355509355509356</v>
-      </c>
-      <c r="H12">
-        <v>0.7863247863247863</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Mothur</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>COI</t>
-        </is>
-      </c>
-      <c r="D13">
-        <v>0.8910891089108911</v>
-      </c>
-      <c r="E13">
-        <v>0.8653846153846154</v>
-      </c>
-      <c r="F13">
-        <v>0.878048780487805</v>
-      </c>
-      <c r="G13">
-        <v>0.8858267716535434</v>
-      </c>
-      <c r="H13">
-        <v>0.7863247863247863</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Qiime2</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>COI</t>
-        </is>
-      </c>
-      <c r="D14">
-        <v>0.9361702127659575</v>
-      </c>
-      <c r="E14">
-        <v>0.8073394495412844</v>
-      </c>
-      <c r="F14">
-        <v>0.8669950738916257</v>
-      </c>
-      <c r="G14">
-        <v>0.9072164948453608</v>
-      </c>
-      <c r="H14">
-        <v>0.7692307692307693</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>VSEARCH</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Wadjemup</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>COI</t>
-        </is>
-      </c>
-      <c r="D15">
-        <v>0.7352941176470589</v>
-      </c>
-      <c r="E15">
-        <v>0.2358490566037736</v>
-      </c>
-      <c r="F15">
-        <v>0.3571428571428571</v>
-      </c>
-      <c r="G15">
-        <v>0.5165289256198347</v>
-      </c>
-      <c r="H15">
-        <v>0.2307692307692308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug in kraken2
</commit_message>
<xml_diff>
--- a/results/tables/All_F1_tables.xlsx
+++ b/results/tables/All_F1_tables.xlsx
@@ -1363,7 +1363,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1542,7 +1542,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Kraken2_0.0</t>
+          <t>DADA2Tax</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -1556,25 +1556,25 @@
         </is>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>0.2564102564102564</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>0.1818181818181818</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>0.2127659574468085</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>0.2369668246445497</v>
       </c>
       <c r="H6">
-        <v>0.1515151515151515</v>
+        <v>0.2525252525252525</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Kraken2_0.05</t>
+          <t>Kraken2_0.0</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -1606,7 +1606,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Kraken2_0.1</t>
+          <t>Kraken2_0.05</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -1638,7 +1638,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>MMSeqs2_100</t>
+          <t>Kraken2_0.1</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -1652,25 +1652,25 @@
         </is>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9">
-        <v>0.6785714285714286</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>0.8085106382978724</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>0.9134615384615385</v>
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>0.7272727272727273</v>
+        <v>0.1515151515151515</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MMSeqs2_97</t>
+          <t>MMSeqs2_100</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -1684,25 +1684,25 @@
         </is>
       </c>
       <c r="D10">
-        <v>0.9682539682539683</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>0.7439024390243902</v>
+        <v>0.6785714285714286</v>
       </c>
       <c r="F10">
-        <v>0.8413793103448277</v>
+        <v>0.8085106382978724</v>
       </c>
       <c r="G10">
-        <v>0.9131736526946107</v>
+        <v>0.9134615384615385</v>
       </c>
       <c r="H10">
-        <v>0.7676767676767676</v>
+        <v>0.7272727272727273</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Metabuli</t>
+          <t>MMSeqs2_97</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -1716,25 +1716,25 @@
         </is>
       </c>
       <c r="D11">
-        <v>0.9230769230769231</v>
+        <v>0.9682539682539683</v>
       </c>
       <c r="E11">
-        <v>0.2926829268292683</v>
+        <v>0.7439024390243902</v>
       </c>
       <c r="F11">
-        <v>0.4444444444444444</v>
+        <v>0.8413793103448277</v>
       </c>
       <c r="G11">
-        <v>0.6451612903225807</v>
+        <v>0.9131736526946107</v>
       </c>
       <c r="H11">
-        <v>0.3939393939393939</v>
+        <v>0.7676767676767676</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Mothur</t>
+          <t>Metabuli</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -1748,25 +1748,25 @@
         </is>
       </c>
       <c r="D12">
-        <v>0.8648648648648649</v>
+        <v>0.9230769230769231</v>
       </c>
       <c r="E12">
-        <v>0.8648648648648649</v>
+        <v>0.2926829268292683</v>
       </c>
       <c r="F12">
-        <v>0.8648648648648649</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="G12">
-        <v>0.8648648648648649</v>
+        <v>0.6451612903225807</v>
       </c>
       <c r="H12">
-        <v>0.797979797979798</v>
+        <v>0.3939393939393939</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Qiime2</t>
+          <t>Mothur</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -1780,50 +1780,82 @@
         </is>
       </c>
       <c r="D13">
-        <v>0.864406779661017</v>
+        <v>0.8648648648648649</v>
       </c>
       <c r="E13">
-        <v>0.6219512195121951</v>
+        <v>0.8648648648648649</v>
       </c>
       <c r="F13">
-        <v>0.723404255319149</v>
+        <v>0.8648648648648649</v>
       </c>
       <c r="G13">
-        <v>0.8018867924528302</v>
+        <v>0.8648648648648649</v>
       </c>
       <c r="H13">
-        <v>0.6060606060606061</v>
+        <v>0.797979797979798</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>Qiime2</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>100 Australian species</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>COI</t>
+        </is>
+      </c>
+      <c r="D14">
+        <v>0.864406779661017</v>
+      </c>
+      <c r="E14">
+        <v>0.6219512195121951</v>
+      </c>
+      <c r="F14">
+        <v>0.723404255319149</v>
+      </c>
+      <c r="G14">
+        <v>0.8018867924528302</v>
+      </c>
+      <c r="H14">
+        <v>0.6060606060606061</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>VSEARCH</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>100 Australian species</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>100 Australian species</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
         <is>
           <t>COI</t>
         </is>
       </c>
-      <c r="D14">
+      <c r="D15">
         <v>0.8695652173913043</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <v>0.8</v>
       </c>
-      <c r="F14">
+      <c r="F15">
         <v>0.8333333333333333</v>
       </c>
-      <c r="G14">
+      <c r="G15">
         <v>0.8547008547008546</v>
       </c>
-      <c r="H14">
+      <c r="H15">
         <v>0.7575757575757576</v>
       </c>
     </row>

</xml_diff>